<commit_message>
Update to FCRs 150518
</commit_message>
<xml_diff>
--- a/alternativefeeddata.xlsx
+++ b/alternativefeeddata.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="179">
   <si>
     <t xml:space="preserve">Taxon </t>
   </si>
@@ -127,9 +127,6 @@
     <t>African Catfish</t>
   </si>
   <si>
-    <t>Target_taxon</t>
-  </si>
-  <si>
     <t>Shepphard et al 1994</t>
   </si>
   <si>
@@ -244,21 +241,6 @@
     <t>Zonocerus variegatus</t>
   </si>
   <si>
-    <t xml:space="preserve"> FCR of the cultured species (opposed to the feed organism)</t>
-  </si>
-  <si>
-    <t>Target_FCR -</t>
-  </si>
-  <si>
-    <t>Taxon of the cultured species</t>
-  </si>
-  <si>
-    <t>Sub_potential</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Potential for feed to substitute fishmeal or fishoil with apositive or no change influence on feed conversion </t>
-  </si>
-  <si>
     <t>Mud Catfish</t>
   </si>
   <si>
@@ -394,9 +376,6 @@
     <t>R_0</t>
   </si>
   <si>
-    <t xml:space="preserve">MDemersal </t>
-  </si>
-  <si>
     <t>Gilthead seabream</t>
   </si>
   <si>
@@ -443,6 +422,147 @@
   </si>
   <si>
     <t xml:space="preserve">Begum et al 1994 </t>
+  </si>
+  <si>
+    <t>Silkworm pupae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nandeesha et al 1990 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silkworm pupae </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Common Carp </t>
+  </si>
+  <si>
+    <t>Cyprinus carpio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jian carp </t>
+  </si>
+  <si>
+    <t>Ji et al 2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rangcharyulu et al 2003 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mutliple: Silver, mrigal, rohu, catla </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hypophthalmychthys molitrix, Cirrhinus mrigala, Labeo rohita, and catla catla </t>
+  </si>
+  <si>
+    <t>Silkworm pupae (Treated)</t>
+  </si>
+  <si>
+    <t>Rangcharyulu et al 2004</t>
+  </si>
+  <si>
+    <t>Silkworm pupae (Unreated)</t>
+  </si>
+  <si>
+    <t>Lee et al 2012</t>
+  </si>
+  <si>
+    <t>Paralichthys olivaceus</t>
+  </si>
+  <si>
+    <t>Olive flounder</t>
+  </si>
+  <si>
+    <t>M.Org</t>
+  </si>
+  <si>
+    <t>Lee et al 2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Promate </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MDemersals </t>
+  </si>
+  <si>
+    <t>Combination</t>
+  </si>
+  <si>
+    <t>Ostazewska</t>
+  </si>
+  <si>
+    <t>Chrionmomid larvae</t>
+  </si>
+  <si>
+    <t>Oncorhynchus mykiss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Promate + silkworm </t>
+  </si>
+  <si>
+    <t>Ictalurus punctatus</t>
+  </si>
+  <si>
+    <t>Channel catfish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Newton 2005 </t>
+  </si>
+  <si>
+    <t>Black solider fly</t>
+  </si>
+  <si>
+    <t>Hermetia illuscens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sealey et al 2011 </t>
+  </si>
+  <si>
+    <t>Sealey et al 2012</t>
+  </si>
+  <si>
+    <t>Black solider fly (enriched)</t>
+  </si>
+  <si>
+    <t>St-Hilaire et al 2007</t>
+  </si>
+  <si>
+    <t>St-Hilaire et al 2008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lock et al 2016 </t>
+  </si>
+  <si>
+    <t>Atlantic salmon</t>
+  </si>
+  <si>
+    <t>Salmo salar</t>
+  </si>
+  <si>
+    <t>Lock et al 2017</t>
+  </si>
+  <si>
+    <t>Lock et al 2018</t>
+  </si>
+  <si>
+    <t>Psetta maxima</t>
+  </si>
+  <si>
+    <t>Turbot</t>
+  </si>
+  <si>
+    <t>OMarine</t>
+  </si>
+  <si>
+    <t>Common housefly</t>
+  </si>
+  <si>
+    <t>Musca domestica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ogunji et al 2008 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ogunji et al 2007 </t>
   </si>
 </sst>
 </file>
@@ -769,28 +889,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D24" sqref="D24"/>
+      <selection pane="bottomRight" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
-    <col min="5" max="6" width="16.42578125" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" customWidth="1"/>
-    <col min="9" max="9" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.453125" customWidth="1"/>
+    <col min="2" max="2" width="28.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7265625" customWidth="1"/>
+    <col min="5" max="6" width="16.453125" customWidth="1"/>
+    <col min="7" max="7" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.54296875" customWidth="1"/>
+    <col min="9" max="9" width="28.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -801,10 +921,10 @@
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>28</v>
@@ -822,7 +942,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -833,10 +953,10 @@
         <v>13</v>
       </c>
       <c r="J2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -847,7 +967,7 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E3">
         <v>61</v>
@@ -862,7 +982,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -873,7 +993,7 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E4">
         <v>68</v>
@@ -888,7 +1008,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -899,7 +1019,7 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E5">
         <v>110</v>
@@ -914,7 +1034,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -925,7 +1045,7 @@
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E6">
         <v>50</v>
@@ -940,7 +1060,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -951,7 +1071,7 @@
         <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E7">
         <v>19</v>
@@ -966,7 +1086,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -977,7 +1097,7 @@
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E8">
         <v>61</v>
@@ -992,7 +1112,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1003,7 +1123,7 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E9">
         <v>68</v>
@@ -1018,7 +1138,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1029,7 +1149,7 @@
         <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E10">
         <v>110</v>
@@ -1044,7 +1164,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1055,7 +1175,7 @@
         <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E11">
         <v>50</v>
@@ -1070,7 +1190,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1081,7 +1201,7 @@
         <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E12">
         <v>19</v>
@@ -1096,7 +1216,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1107,7 +1227,7 @@
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -1122,7 +1242,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1133,7 +1253,7 @@
         <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -1148,7 +1268,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -1159,7 +1279,7 @@
         <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -1174,7 +1294,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1185,7 +1305,7 @@
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E16">
         <v>0.16</v>
@@ -1200,7 +1320,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -1211,7 +1331,7 @@
         <v>19</v>
       </c>
       <c r="D17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E17">
         <v>0.08</v>
@@ -1226,7 +1346,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -1237,7 +1357,7 @@
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E18">
         <v>1.5</v>
@@ -1252,7 +1372,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -1263,7 +1383,7 @@
         <v>8</v>
       </c>
       <c r="D19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E19">
         <v>0.1</v>
@@ -1278,7 +1398,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -1289,7 +1409,7 @@
         <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E20">
         <v>8</v>
@@ -1304,7 +1424,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -1315,7 +1435,7 @@
         <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -1330,7 +1450,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -1341,7 +1461,7 @@
         <v>19</v>
       </c>
       <c r="D22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E22">
         <v>0.3</v>
@@ -1356,7 +1476,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -1367,7 +1487,7 @@
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E23">
         <v>0.45</v>
@@ -1382,7 +1502,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -1393,7 +1513,7 @@
         <v>8</v>
       </c>
       <c r="D24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E24">
         <v>0.05</v>
@@ -1408,7 +1528,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>11</v>
       </c>
@@ -1419,7 +1539,7 @@
         <v>12</v>
       </c>
       <c r="D25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E25">
         <v>2.37</v>
@@ -1434,7 +1554,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>11</v>
       </c>
@@ -1445,7 +1565,7 @@
         <v>15</v>
       </c>
       <c r="D26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E26">
         <v>4</v>
@@ -1460,7 +1580,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>11</v>
       </c>
@@ -1471,7 +1591,7 @@
         <v>19</v>
       </c>
       <c r="D27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E27">
         <v>2.12</v>
@@ -1486,7 +1606,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -1497,16 +1617,16 @@
         <v>30</v>
       </c>
       <c r="D28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H28">
         <v>0.42</v>
       </c>
       <c r="I28" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -1517,54 +1637,54 @@
         <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E29">
         <v>2.65</v>
       </c>
       <c r="G29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H29">
         <v>0.53</v>
       </c>
       <c r="I29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J29" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E30">
         <v>2.65</v>
       </c>
       <c r="G30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H30">
         <v>0.45</v>
       </c>
       <c r="I30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J30" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -1575,22 +1695,22 @@
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E31">
         <v>3.6</v>
       </c>
       <c r="G31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J31" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -1601,22 +1721,22 @@
         <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E32">
         <v>34</v>
       </c>
       <c r="G32" t="s">
+        <v>49</v>
+      </c>
+      <c r="I32" t="s">
+        <v>57</v>
+      </c>
+      <c r="J32" t="s">
         <v>50</v>
       </c>
-      <c r="I32" t="s">
-        <v>58</v>
-      </c>
-      <c r="J32" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -1627,22 +1747,22 @@
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E33">
         <v>14</v>
       </c>
       <c r="G33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J33" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -1653,22 +1773,22 @@
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E34">
         <v>173</v>
       </c>
       <c r="G34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J34" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -1679,22 +1799,22 @@
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E35">
         <v>18</v>
       </c>
       <c r="G35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J35" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -1705,25 +1825,25 @@
         <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E36">
         <v>4341</v>
       </c>
       <c r="G36" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H36">
         <v>0.186</v>
       </c>
       <c r="I36" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J36" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -1734,22 +1854,22 @@
         <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E37">
         <v>4.3410000000000002</v>
       </c>
       <c r="G37" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I37" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J37" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>10</v>
       </c>
@@ -1760,22 +1880,22 @@
         <v>4</v>
       </c>
       <c r="D38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E38">
         <v>23</v>
       </c>
       <c r="G38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I38" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J38" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -1786,19 +1906,33 @@
         <v>4</v>
       </c>
       <c r="D39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E39">
         <v>23</v>
       </c>
       <c r="G39" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I39" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J39" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" t="s">
+        <v>132</v>
+      </c>
+      <c r="H40">
+        <v>0.41</v>
+      </c>
+      <c r="I40" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -1808,122 +1942,122 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC13"/>
+  <dimension ref="A1:AC30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="8" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="1" topLeftCell="I9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomRight" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="27.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.453125" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1796875" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="11" max="11" width="8.140625" customWidth="1"/>
-    <col min="12" max="12" width="8.5703125" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" customWidth="1"/>
-    <col min="14" max="14" width="10.140625" customWidth="1"/>
-    <col min="15" max="15" width="8.5703125" customWidth="1"/>
+    <col min="11" max="11" width="8.1796875" customWidth="1"/>
+    <col min="12" max="12" width="8.54296875" customWidth="1"/>
+    <col min="13" max="13" width="8.7265625" customWidth="1"/>
+    <col min="14" max="14" width="10.1796875" customWidth="1"/>
+    <col min="15" max="15" width="8.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="X1" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1931,7 +2065,7 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
         <v>17</v>
@@ -1946,7 +2080,7 @@
         <v>32</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="I2">
         <v>0.76</v>
@@ -1972,7 +2106,7 @@
         <v>1.1235955056179776</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1980,13 +2114,13 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" t="s">
         <v>70</v>
-      </c>
-      <c r="D3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E3" t="s">
-        <v>71</v>
       </c>
       <c r="F3" t="s">
         <v>31</v>
@@ -1995,7 +2129,7 @@
         <v>32</v>
       </c>
       <c r="H3" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="I3">
         <v>1.51</v>
@@ -2013,7 +2147,7 @@
         <v>1.91</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -2021,19 +2155,19 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F4" t="s">
         <v>31</v>
       </c>
       <c r="G4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="I4">
         <v>2.96</v>
@@ -2051,7 +2185,7 @@
         <v>3.44</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -2059,7 +2193,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D5" t="s">
         <v>17</v>
@@ -2071,7 +2205,7 @@
         <v>31</v>
       </c>
       <c r="G5" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="I5">
         <v>3.8</v>
@@ -2080,7 +2214,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -2088,7 +2222,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D6" t="s">
         <v>17</v>
@@ -2097,13 +2231,13 @@
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>122</v>
+        <v>151</v>
       </c>
       <c r="G6" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="H6" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="I6">
         <v>1.34</v>
@@ -2115,7 +2249,7 @@
         <v>1.28</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -2123,7 +2257,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D7" t="s">
         <v>17</v>
@@ -2132,13 +2266,13 @@
         <v>4</v>
       </c>
       <c r="F7" t="s">
-        <v>122</v>
+        <v>151</v>
       </c>
       <c r="G7" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="H7" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="I7">
         <v>0.9</v>
@@ -2150,7 +2284,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -2158,7 +2292,7 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D8" t="s">
         <v>17</v>
@@ -2167,10 +2301,13 @@
         <v>4</v>
       </c>
       <c r="F8" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="G8" t="s">
-        <v>87</v>
+        <v>81</v>
+      </c>
+      <c r="H8" t="s">
+        <v>155</v>
       </c>
       <c r="I8">
         <v>1.2</v>
@@ -2182,7 +2319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -2190,19 +2327,19 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D9" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E9" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F9" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="G9" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="I9">
         <v>0.89</v>
@@ -2217,7 +2354,7 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -2225,22 +2362,22 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="D10" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="E10" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="F10" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="G10" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="H10" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="I10">
         <v>1.47</v>
@@ -2258,30 +2395,30 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>152</v>
       </c>
       <c r="C11" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="D11" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="E11" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="F11" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="G11" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="H11" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="I11">
         <v>2.0499999999999998</v>
@@ -2299,65 +2436,696 @@
         <v>2.0699999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>1</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>133</v>
+      </c>
+      <c r="D12" t="s">
+        <v>134</v>
+      </c>
+      <c r="E12" t="s">
+        <v>129</v>
+      </c>
+      <c r="F12" t="s">
+        <v>127</v>
+      </c>
+      <c r="G12" t="s">
+        <v>135</v>
+      </c>
+      <c r="H12" t="s">
+        <v>136</v>
+      </c>
+      <c r="I12">
+        <v>3.31</v>
+      </c>
+      <c r="S12">
+        <v>3.19</v>
+      </c>
+      <c r="AC12">
+        <v>3.38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>1</v>
       </c>
       <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>138</v>
+      </c>
+      <c r="D13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E13" t="s">
+        <v>129</v>
+      </c>
+      <c r="F13" t="s">
+        <v>127</v>
+      </c>
+      <c r="G13" t="s">
+        <v>137</v>
+      </c>
+      <c r="H13" t="s">
+        <v>136</v>
+      </c>
+      <c r="I13">
+        <v>1.41</v>
+      </c>
+      <c r="S13">
+        <v>1.36</v>
+      </c>
+      <c r="U13">
+        <v>1.35</v>
+      </c>
+      <c r="W13">
+        <v>1.44</v>
+      </c>
+      <c r="Y13">
+        <v>1.46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>139</v>
+      </c>
+      <c r="D14" t="s">
+        <v>142</v>
+      </c>
+      <c r="E14" t="s">
+        <v>129</v>
+      </c>
+      <c r="F14" t="s">
+        <v>127</v>
+      </c>
+      <c r="G14" t="s">
+        <v>140</v>
+      </c>
+      <c r="H14" t="s">
+        <v>141</v>
+      </c>
+      <c r="I14">
+        <v>3.16</v>
+      </c>
+      <c r="AC14">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
+        <v>143</v>
+      </c>
+      <c r="D15" t="s">
+        <v>144</v>
+      </c>
+      <c r="E15" t="s">
+        <v>129</v>
+      </c>
+      <c r="F15" t="s">
+        <v>127</v>
+      </c>
+      <c r="G15" t="s">
+        <v>140</v>
+      </c>
+      <c r="H15" t="s">
+        <v>141</v>
+      </c>
+      <c r="I15">
+        <v>3.16</v>
+      </c>
+      <c r="AC15">
+        <v>2.98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>145</v>
+      </c>
+      <c r="D16" t="s">
+        <v>134</v>
+      </c>
+      <c r="E16" t="s">
+        <v>129</v>
+      </c>
+      <c r="F16" t="s">
+        <v>151</v>
+      </c>
+      <c r="G16" t="s">
+        <v>147</v>
+      </c>
+      <c r="H16" t="s">
+        <v>146</v>
+      </c>
+      <c r="I16">
+        <f>1/1.08</f>
+        <v>0.92592592592592582</v>
+      </c>
+      <c r="K16">
+        <f>1/1.12</f>
+        <v>0.89285714285714279</v>
+      </c>
+      <c r="M16">
+        <f>1/1.08</f>
+        <v>0.92592592592592582</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>148</v>
+      </c>
+      <c r="C17" t="s">
+        <v>149</v>
+      </c>
+      <c r="D17" t="s">
+        <v>150</v>
+      </c>
+      <c r="F17" t="s">
+        <v>151</v>
+      </c>
+      <c r="G17" t="s">
+        <v>147</v>
+      </c>
+      <c r="H17" t="s">
+        <v>146</v>
+      </c>
+      <c r="I17">
+        <f>1/1.08</f>
+        <v>0.92592592592592582</v>
+      </c>
+      <c r="K17">
+        <f>1/1.14</f>
+        <v>0.87719298245614041</v>
+      </c>
+      <c r="M17">
+        <f>1/1.06</f>
+        <v>0.94339622641509424</v>
+      </c>
+      <c r="Q17">
+        <f>1/0.89</f>
+        <v>1.1235955056179776</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>152</v>
+      </c>
+      <c r="C18" t="s">
+        <v>149</v>
+      </c>
+      <c r="D18" t="s">
+        <v>156</v>
+      </c>
+      <c r="E18" t="s">
+        <v>129</v>
+      </c>
+      <c r="F18" t="s">
+        <v>151</v>
+      </c>
+      <c r="G18" t="s">
+        <v>147</v>
+      </c>
+      <c r="H18" t="s">
+        <v>146</v>
+      </c>
+      <c r="I18">
+        <f>1/1.08</f>
+        <v>0.92592592592592582</v>
+      </c>
+      <c r="K18">
+        <f>1/1.15</f>
+        <v>0.86956521739130443</v>
+      </c>
+      <c r="M18">
+        <f>1/0.94</f>
+        <v>1.0638297872340425</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>153</v>
+      </c>
+      <c r="D19" t="s">
+        <v>154</v>
+      </c>
+      <c r="F19" t="s">
+        <v>118</v>
+      </c>
+      <c r="G19" t="s">
+        <v>81</v>
+      </c>
+      <c r="H19" t="s">
+        <v>155</v>
+      </c>
+      <c r="I19">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s">
+        <v>159</v>
+      </c>
+      <c r="D20" t="s">
+        <v>160</v>
+      </c>
+      <c r="E20" t="s">
+        <v>161</v>
+      </c>
+      <c r="F20" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" t="s">
+        <v>158</v>
+      </c>
+      <c r="H20" t="s">
+        <v>157</v>
+      </c>
+      <c r="I20">
+        <f>1/1.48</f>
+        <v>0.67567567567567566</v>
+      </c>
+      <c r="AC20">
+        <f>1/1.68</f>
+        <v>0.59523809523809523</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
+        <v>162</v>
+      </c>
+      <c r="D21" t="s">
+        <v>160</v>
+      </c>
+      <c r="E21" t="s">
+        <v>161</v>
+      </c>
+      <c r="F21" t="s">
+        <v>118</v>
+      </c>
+      <c r="G21" t="s">
+        <v>81</v>
+      </c>
+      <c r="H21" t="s">
+        <v>155</v>
+      </c>
+      <c r="I21">
+        <v>1.2</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="S21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" t="s">
+        <v>163</v>
+      </c>
+      <c r="D22" t="s">
+        <v>164</v>
+      </c>
+      <c r="E22" t="s">
+        <v>161</v>
+      </c>
+      <c r="F22" t="s">
+        <v>118</v>
+      </c>
+      <c r="G22" t="s">
+        <v>81</v>
+      </c>
+      <c r="H22" t="s">
+        <v>155</v>
+      </c>
+      <c r="I22">
+        <v>1.2</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
+      <c r="S22">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" t="s">
+        <v>165</v>
+      </c>
+      <c r="D23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" t="s">
+        <v>161</v>
+      </c>
+      <c r="F23" t="s">
+        <v>118</v>
+      </c>
+      <c r="G23" t="s">
+        <v>81</v>
+      </c>
+      <c r="H23" t="s">
+        <v>155</v>
+      </c>
+      <c r="I23">
+        <v>1.18</v>
+      </c>
+      <c r="P23">
+        <v>1.22</v>
+      </c>
+      <c r="U23">
+        <v>1.47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" t="s">
+        <v>166</v>
+      </c>
+      <c r="D24" t="s">
+        <v>175</v>
+      </c>
+      <c r="E24" t="s">
+        <v>176</v>
+      </c>
+      <c r="F24" t="s">
+        <v>118</v>
+      </c>
+      <c r="G24" t="s">
+        <v>81</v>
+      </c>
+      <c r="H24" t="s">
+        <v>155</v>
+      </c>
+      <c r="I24">
+        <v>1.18</v>
+      </c>
+      <c r="N24">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" t="s">
+        <v>167</v>
+      </c>
+      <c r="D25" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" t="s">
+        <v>161</v>
+      </c>
+      <c r="F25" t="s">
+        <v>118</v>
+      </c>
+      <c r="G25" t="s">
+        <v>168</v>
+      </c>
+      <c r="H25" t="s">
+        <v>169</v>
+      </c>
+      <c r="I25">
+        <v>1.25</v>
+      </c>
+      <c r="N25">
+        <v>1.24</v>
+      </c>
+      <c r="S25">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="AC25">
+        <v>1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" t="s">
+        <v>170</v>
+      </c>
+      <c r="D26" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" t="s">
+        <v>161</v>
+      </c>
+      <c r="F26" t="s">
+        <v>118</v>
+      </c>
+      <c r="G26" t="s">
+        <v>168</v>
+      </c>
+      <c r="H26" t="s">
+        <v>169</v>
+      </c>
+      <c r="I26">
+        <v>1.25</v>
+      </c>
+      <c r="N26">
+        <v>0.98</v>
+      </c>
+      <c r="AC26">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" t="s">
+        <v>171</v>
+      </c>
+      <c r="D27" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27" t="s">
+        <v>161</v>
+      </c>
+      <c r="F27" t="s">
+        <v>174</v>
+      </c>
+      <c r="G27" t="s">
+        <v>173</v>
+      </c>
+      <c r="H27" t="s">
+        <v>172</v>
+      </c>
+      <c r="I27">
+        <v>0.76</v>
+      </c>
+      <c r="M27">
+        <v>0.76</v>
+      </c>
+      <c r="P27">
+        <v>0.82</v>
+      </c>
+      <c r="S27">
+        <v>0.86</v>
+      </c>
+      <c r="W27">
+        <v>0.98</v>
+      </c>
+      <c r="Y27">
+        <v>1.21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" t="s">
+        <v>177</v>
+      </c>
+      <c r="D28" t="s">
+        <v>175</v>
+      </c>
+      <c r="E28" t="s">
+        <v>176</v>
+      </c>
+      <c r="F28" t="s">
+        <v>122</v>
+      </c>
+      <c r="G28" t="s">
+        <v>124</v>
+      </c>
+      <c r="H28" t="s">
+        <v>123</v>
+      </c>
+      <c r="I28">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="O28">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="R28">
+        <v>1.05</v>
+      </c>
+      <c r="U28">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="X28">
+        <v>1.06</v>
+      </c>
+      <c r="Z28">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="AC28">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" t="s">
+        <v>178</v>
+      </c>
+      <c r="D29" t="s">
+        <v>175</v>
+      </c>
+      <c r="E29" t="s">
+        <v>176</v>
+      </c>
+      <c r="F29" t="s">
+        <v>122</v>
+      </c>
+      <c r="G29" t="s">
+        <v>124</v>
+      </c>
+      <c r="H29" t="s">
+        <v>123</v>
+      </c>
+      <c r="I29">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O29">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="R29">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="U29">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="X29">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Z29">
+        <v>1.2</v>
+      </c>
+      <c r="AC29">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>

</xml_diff>

<commit_message>
Added a couple of algal groups - bulk download done - need to add next
</commit_message>
<xml_diff>
--- a/alternativefeeddata.xlsx
+++ b/alternativefeeddata.xlsx
@@ -13,7 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Footprints " sheetId="1" r:id="rId1"/>
-    <sheet name="Growth" sheetId="3" r:id="rId2"/>
+    <sheet name="FCR " sheetId="3" r:id="rId2"/>
     <sheet name="Codes " sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="227">
   <si>
     <t xml:space="preserve">Taxon </t>
   </si>
@@ -472,9 +472,6 @@
     <t>Olive flounder</t>
   </si>
   <si>
-    <t>M.Org</t>
-  </si>
-  <si>
     <t>Lee et al 2013</t>
   </si>
   <si>
@@ -563,6 +560,153 @@
   </si>
   <si>
     <t xml:space="preserve">Ogunji et al 2007 </t>
+  </si>
+  <si>
+    <t>Kroeckel et al 2013</t>
+  </si>
+  <si>
+    <t>Aniebo et al 2009</t>
+  </si>
+  <si>
+    <t>Fasakin et al 2003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poultry feather meal, viscera and maggot meal </t>
+  </si>
+  <si>
+    <t>Adewolu et al 2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wang et al 2017 </t>
+  </si>
+  <si>
+    <t>Ogunji et al 2009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Replacing </t>
+  </si>
+  <si>
+    <t>Fishmeal</t>
+  </si>
+  <si>
+    <t>Algae</t>
+  </si>
+  <si>
+    <t>Fish oil</t>
+  </si>
+  <si>
+    <t>Schizochytrium limacinum</t>
+  </si>
+  <si>
+    <t>Algal meal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Garcia-Ortega et al 2016 </t>
+  </si>
+  <si>
+    <t>Giant Grouper</t>
+  </si>
+  <si>
+    <t>Epinephelus lanceolatus</t>
+  </si>
+  <si>
+    <t>Bacteria</t>
+  </si>
+  <si>
+    <t>Garcia-Ortega et al 2017</t>
+  </si>
+  <si>
+    <t>Litopenaeus vannamei</t>
+  </si>
+  <si>
+    <t>Shrimp</t>
+  </si>
+  <si>
+    <t>Pacific white shrimp</t>
+  </si>
+  <si>
+    <t>Ju et al 2012</t>
+  </si>
+  <si>
+    <t>Haematococcus pluvialis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kissinger et al 2016 </t>
+  </si>
+  <si>
+    <t>Soy protein, squid trimmings, Algal meal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longfin yellowtail </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seriola rivoliana </t>
+  </si>
+  <si>
+    <t xml:space="preserve">%of algae as proetin source </t>
+  </si>
+  <si>
+    <t>Atlantic cod </t>
+  </si>
+  <si>
+    <t>Gadus morhua</t>
+  </si>
+  <si>
+    <t>Isocrysis sp. Nannochloropsis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Walker and Berlinksy 2011 </t>
+  </si>
+  <si>
+    <t>Porphyra spp.</t>
+  </si>
+  <si>
+    <t>Walker et al 2011</t>
+  </si>
+  <si>
+    <t>OPelagic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nanofrustulum sp. </t>
+  </si>
+  <si>
+    <t>Tetraselmis sp.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kiron et al 2012 </t>
+  </si>
+  <si>
+    <t>Kiron et al 2013</t>
+  </si>
+  <si>
+    <t>Whiteleg shrimp</t>
+  </si>
+  <si>
+    <t>Start on salze 2010</t>
+  </si>
+  <si>
+    <t>Vizcaino et al 2014</t>
+  </si>
+  <si>
+    <t>Scenedesmus almeriensis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fishmeal </t>
+  </si>
+  <si>
+    <t>Vizcaino et al 2015</t>
+  </si>
+  <si>
+    <t>Parrot fish</t>
+  </si>
+  <si>
+    <t>Oplegnathus fasciatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirulina pacifica </t>
+  </si>
+  <si>
+    <t>Kim et al 2013</t>
   </si>
 </sst>
 </file>
@@ -892,10 +1036,10 @@
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B35" sqref="B35"/>
+      <selection pane="bottomRight" activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1942,13 +2086,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC30"/>
+  <dimension ref="A1:AE60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="8" ySplit="1" topLeftCell="I9" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="9" ySplit="1" topLeftCell="J12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D30" sqref="D30"/>
+      <selection pane="bottomRight" activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1956,19 +2100,20 @@
     <col min="3" max="3" width="27.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.7265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.453125" customWidth="1"/>
-    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.1796875" customWidth="1"/>
-    <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="11" max="11" width="8.1796875" customWidth="1"/>
-    <col min="12" max="12" width="8.54296875" customWidth="1"/>
-    <col min="13" max="13" width="8.7265625" customWidth="1"/>
-    <col min="14" max="14" width="10.1796875" customWidth="1"/>
-    <col min="15" max="15" width="8.54296875" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.453125" customWidth="1"/>
+    <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1796875" customWidth="1"/>
+    <col min="11" max="11" width="12" customWidth="1"/>
+    <col min="12" max="12" width="8.1796875" customWidth="1"/>
+    <col min="13" max="13" width="8.54296875" customWidth="1"/>
+    <col min="14" max="14" width="8.7265625" customWidth="1"/>
+    <col min="15" max="15" width="10.1796875" customWidth="1"/>
+    <col min="16" max="16" width="8.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>90</v>
       </c>
@@ -1985,910 +2130,997 @@
         <v>86</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>151</v>
       </c>
       <c r="C2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2" t="s">
+        <v>186</v>
+      </c>
+      <c r="G2" t="s">
+        <v>127</v>
+      </c>
+      <c r="H2" t="s">
+        <v>128</v>
+      </c>
+      <c r="I2" t="s">
+        <v>130</v>
+      </c>
+      <c r="J2">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="Q2">
+        <v>1.96</v>
+      </c>
+      <c r="V2">
+        <v>1.92</v>
+      </c>
+      <c r="Z2">
+        <v>2</v>
+      </c>
+      <c r="AD2">
+        <v>2.0699999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F3" t="s">
+        <v>186</v>
+      </c>
+      <c r="G3" t="s">
+        <v>127</v>
+      </c>
+      <c r="H3" t="s">
+        <v>135</v>
+      </c>
+      <c r="I3" t="s">
+        <v>136</v>
+      </c>
+      <c r="J3">
+        <v>3.31</v>
+      </c>
+      <c r="T3">
+        <v>3.19</v>
+      </c>
+      <c r="AD3">
+        <v>3.38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F4" t="s">
+        <v>186</v>
+      </c>
+      <c r="G4" t="s">
+        <v>127</v>
+      </c>
+      <c r="H4" t="s">
+        <v>137</v>
+      </c>
+      <c r="I4" t="s">
+        <v>136</v>
+      </c>
+      <c r="J4">
+        <v>1.41</v>
+      </c>
+      <c r="T4">
+        <v>1.36</v>
+      </c>
+      <c r="V4">
+        <v>1.35</v>
+      </c>
+      <c r="X4">
+        <v>1.44</v>
+      </c>
+      <c r="Z4">
+        <v>1.46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D5" t="s">
+        <v>142</v>
+      </c>
+      <c r="E5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F5" t="s">
+        <v>186</v>
+      </c>
+      <c r="G5" t="s">
+        <v>127</v>
+      </c>
+      <c r="H5" t="s">
+        <v>140</v>
+      </c>
+      <c r="I5" t="s">
+        <v>141</v>
+      </c>
+      <c r="J5">
+        <v>3.16</v>
+      </c>
+      <c r="AD5">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>143</v>
+      </c>
+      <c r="D6" t="s">
+        <v>144</v>
+      </c>
+      <c r="E6" t="s">
+        <v>129</v>
+      </c>
+      <c r="F6" t="s">
+        <v>186</v>
+      </c>
+      <c r="G6" t="s">
+        <v>127</v>
+      </c>
+      <c r="H6" t="s">
+        <v>140</v>
+      </c>
+      <c r="I6" t="s">
+        <v>141</v>
+      </c>
+      <c r="J6">
+        <v>3.16</v>
+      </c>
+      <c r="AD6">
+        <v>2.98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
         <v>34</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D7" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E7" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F7" t="s">
+        <v>186</v>
+      </c>
+      <c r="G7" t="s">
         <v>31</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H7" t="s">
         <v>32</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I7" t="s">
         <v>91</v>
       </c>
-      <c r="I2">
+      <c r="J7">
         <v>0.76</v>
       </c>
-      <c r="M2">
+      <c r="N7">
         <f>1/1.33</f>
         <v>0.75187969924812026</v>
       </c>
-      <c r="Q2">
+      <c r="R7">
         <f>1/1.19</f>
         <v>0.84033613445378152</v>
       </c>
-      <c r="U2">
+      <c r="V7">
         <f>1/1.02</f>
         <v>0.98039215686274506</v>
       </c>
-      <c r="Y2">
+      <c r="Z7">
         <f>1/1.12</f>
         <v>0.89285714285714279</v>
       </c>
-      <c r="AC2">
+      <c r="AD7">
         <f>1/0.89</f>
         <v>1.1235955056179776</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
         <v>69</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D8" t="s">
         <v>68</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E8" t="s">
         <v>70</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F8" t="s">
+        <v>186</v>
+      </c>
+      <c r="G8" t="s">
         <v>31</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H8" t="s">
         <v>32</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I8" t="s">
         <v>91</v>
       </c>
-      <c r="I3">
+      <c r="J8">
         <v>1.51</v>
       </c>
-      <c r="N3">
+      <c r="O8">
         <v>1.46</v>
       </c>
-      <c r="S3">
+      <c r="T8">
         <v>1.81</v>
       </c>
-      <c r="X3">
+      <c r="Y8">
         <v>1.72</v>
       </c>
-      <c r="AC3">
+      <c r="AD8">
         <v>1.91</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
         <v>74</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D9" t="s">
         <v>72</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E9" t="s">
         <v>73</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F9" t="s">
+        <v>186</v>
+      </c>
+      <c r="G9" t="s">
         <v>31</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H9" t="s">
         <v>71</v>
       </c>
-      <c r="I4">
+      <c r="I9" t="s">
+        <v>91</v>
+      </c>
+      <c r="J9">
         <v>2.96</v>
       </c>
-      <c r="N4">
+      <c r="O9">
         <v>3.09</v>
       </c>
-      <c r="S4">
+      <c r="T9">
         <v>2.88</v>
       </c>
-      <c r="X4">
+      <c r="Y9">
         <v>3.67</v>
       </c>
-      <c r="AC4">
+      <c r="AD9">
         <v>3.44</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
         <v>75</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D10" t="s">
         <v>17</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E10" t="s">
         <v>4</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F10" t="s">
+        <v>186</v>
+      </c>
+      <c r="G10" t="s">
         <v>31</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H10" t="s">
         <v>76</v>
       </c>
-      <c r="I5">
+      <c r="J10">
         <v>3.8</v>
       </c>
-      <c r="S5">
+      <c r="T10">
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>158</v>
+      </c>
+      <c r="D11" t="s">
+        <v>159</v>
+      </c>
+      <c r="E11" t="s">
+        <v>160</v>
+      </c>
+      <c r="F11" t="s">
+        <v>186</v>
+      </c>
+      <c r="G11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" t="s">
+        <v>157</v>
+      </c>
+      <c r="I11" t="s">
+        <v>156</v>
+      </c>
+      <c r="J11">
+        <f>1/1.48</f>
+        <v>0.67567567567567566</v>
+      </c>
+      <c r="AD11">
+        <f>1/1.68</f>
+        <v>0.59523809523809523</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>179</v>
+      </c>
+      <c r="D12" t="s">
+        <v>174</v>
+      </c>
+      <c r="E12" t="s">
+        <v>175</v>
+      </c>
+      <c r="F12" t="s">
+        <v>186</v>
+      </c>
+      <c r="G12" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" t="s">
+        <v>32</v>
+      </c>
+      <c r="I12" t="s">
+        <v>91</v>
+      </c>
+      <c r="J12">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="T12">
+        <v>1.17</v>
+      </c>
+      <c r="AD12">
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>180</v>
+      </c>
+      <c r="D13" t="s">
+        <v>174</v>
+      </c>
+      <c r="E13" t="s">
+        <v>175</v>
+      </c>
+      <c r="F13" t="s">
+        <v>186</v>
+      </c>
+      <c r="G13" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" t="s">
+        <v>32</v>
+      </c>
+      <c r="I13" t="s">
+        <v>91</v>
+      </c>
+      <c r="J13">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="AD13">
+        <v>2.58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>180</v>
+      </c>
+      <c r="D14" t="s">
+        <v>174</v>
+      </c>
+      <c r="E14" t="s">
+        <v>175</v>
+      </c>
+      <c r="F14" t="s">
+        <v>186</v>
+      </c>
+      <c r="G14" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14" t="s">
+        <v>32</v>
+      </c>
+      <c r="I14" t="s">
+        <v>91</v>
+      </c>
+      <c r="J14">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="AD14">
+        <v>3.52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
+        <v>180</v>
+      </c>
+      <c r="D15" t="s">
+        <v>174</v>
+      </c>
+      <c r="E15" t="s">
+        <v>175</v>
+      </c>
+      <c r="F15" t="s">
+        <v>186</v>
+      </c>
+      <c r="G15" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" t="s">
+        <v>91</v>
+      </c>
+      <c r="J15">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="AD15">
+        <v>2.2400000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>180</v>
+      </c>
+      <c r="D16" t="s">
+        <v>174</v>
+      </c>
+      <c r="E16" t="s">
+        <v>175</v>
+      </c>
+      <c r="F16" t="s">
+        <v>186</v>
+      </c>
+      <c r="G16" t="s">
+        <v>31</v>
+      </c>
+      <c r="H16" t="s">
+        <v>32</v>
+      </c>
+      <c r="I16" t="s">
+        <v>91</v>
+      </c>
+      <c r="J16">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="AD16">
+        <v>2.65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>151</v>
+      </c>
+      <c r="C17" t="s">
+        <v>182</v>
+      </c>
+      <c r="D17" t="s">
+        <v>181</v>
+      </c>
+      <c r="E17" t="s">
+        <v>175</v>
+      </c>
+      <c r="F17" t="s">
+        <v>186</v>
+      </c>
+      <c r="G17" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" t="s">
+        <v>32</v>
+      </c>
+      <c r="I17" t="s">
+        <v>91</v>
+      </c>
+      <c r="J17">
+        <v>1.34</v>
+      </c>
+      <c r="O17">
+        <v>1.36</v>
+      </c>
+      <c r="T17">
+        <v>1.44</v>
+      </c>
+      <c r="Y17">
+        <v>1.61</v>
+      </c>
+      <c r="AD17">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" t="s">
+        <v>83</v>
+      </c>
+      <c r="F18" t="s">
+        <v>186</v>
+      </c>
+      <c r="G18" t="s">
+        <v>119</v>
+      </c>
+      <c r="H18" t="s">
+        <v>71</v>
+      </c>
+      <c r="I18" t="s">
+        <v>91</v>
+      </c>
+      <c r="J18">
+        <v>0.89</v>
+      </c>
+      <c r="O18">
+        <v>0.7</v>
+      </c>
+      <c r="T18">
+        <v>0.99</v>
+      </c>
+      <c r="Y18">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
         <v>79</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D19" t="s">
         <v>17</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E19" t="s">
         <v>4</v>
       </c>
-      <c r="F6" t="s">
-        <v>151</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="F19" t="s">
+        <v>186</v>
+      </c>
+      <c r="G19" t="s">
+        <v>150</v>
+      </c>
+      <c r="H19" t="s">
         <v>116</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I19" t="s">
         <v>77</v>
       </c>
-      <c r="I6">
+      <c r="J19">
         <v>1.34</v>
       </c>
-      <c r="P6">
+      <c r="Q19">
         <v>1.02</v>
       </c>
-      <c r="W6">
+      <c r="X19">
         <v>1.28</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s">
         <v>80</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D20" t="s">
         <v>17</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E20" t="s">
         <v>4</v>
       </c>
-      <c r="F7" t="s">
-        <v>151</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="F20" t="s">
+        <v>186</v>
+      </c>
+      <c r="G20" t="s">
+        <v>150</v>
+      </c>
+      <c r="H20" t="s">
         <v>78</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I20" t="s">
         <v>117</v>
       </c>
-      <c r="I7">
+      <c r="J20">
         <v>0.9</v>
       </c>
-      <c r="P7">
+      <c r="Q20">
         <v>0.91</v>
       </c>
-      <c r="W7">
+      <c r="X20">
         <v>0.99</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>82</v>
-      </c>
-      <c r="D8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" t="s">
-        <v>118</v>
-      </c>
-      <c r="G8" t="s">
-        <v>81</v>
-      </c>
-      <c r="H8" t="s">
-        <v>155</v>
-      </c>
-      <c r="I8">
-        <v>1.2</v>
-      </c>
-      <c r="P8">
-        <v>1</v>
-      </c>
-      <c r="X8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>85</v>
-      </c>
-      <c r="D9" t="s">
-        <v>84</v>
-      </c>
-      <c r="E9" t="s">
-        <v>83</v>
-      </c>
-      <c r="F9" t="s">
-        <v>119</v>
-      </c>
-      <c r="G9" t="s">
-        <v>71</v>
-      </c>
-      <c r="I9">
-        <v>0.89</v>
-      </c>
-      <c r="N9">
-        <v>0.7</v>
-      </c>
-      <c r="S9">
-        <v>0.99</v>
-      </c>
-      <c r="X9">
-        <v>1.04</v>
-      </c>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>125</v>
-      </c>
-      <c r="D10" t="s">
-        <v>121</v>
-      </c>
-      <c r="E10" t="s">
-        <v>120</v>
-      </c>
-      <c r="F10" t="s">
-        <v>122</v>
-      </c>
-      <c r="G10" t="s">
-        <v>124</v>
-      </c>
-      <c r="H10" t="s">
-        <v>123</v>
-      </c>
-      <c r="I10">
-        <v>1.47</v>
-      </c>
-      <c r="N10">
-        <v>1.25</v>
-      </c>
-      <c r="S10">
-        <v>1.36</v>
-      </c>
-      <c r="X10">
-        <v>1.42</v>
-      </c>
-      <c r="AC10">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>152</v>
-      </c>
-      <c r="C11" t="s">
-        <v>131</v>
-      </c>
-      <c r="D11" t="s">
-        <v>126</v>
-      </c>
-      <c r="E11" t="s">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
+        <v>145</v>
+      </c>
+      <c r="D21" t="s">
+        <v>134</v>
+      </c>
+      <c r="E21" t="s">
         <v>129</v>
       </c>
-      <c r="F11" t="s">
-        <v>127</v>
-      </c>
-      <c r="G11" t="s">
-        <v>128</v>
-      </c>
-      <c r="H11" t="s">
-        <v>130</v>
-      </c>
-      <c r="I11">
-        <v>2.0499999999999998</v>
-      </c>
-      <c r="P11">
-        <v>1.96</v>
-      </c>
-      <c r="U11">
-        <v>1.92</v>
-      </c>
-      <c r="Y11">
-        <v>2</v>
-      </c>
-      <c r="AC11">
-        <v>2.0699999999999998</v>
-      </c>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" t="s">
-        <v>133</v>
-      </c>
-      <c r="D12" t="s">
-        <v>134</v>
-      </c>
-      <c r="E12" t="s">
-        <v>129</v>
-      </c>
-      <c r="F12" t="s">
-        <v>127</v>
-      </c>
-      <c r="G12" t="s">
-        <v>135</v>
-      </c>
-      <c r="H12" t="s">
-        <v>136</v>
-      </c>
-      <c r="I12">
-        <v>3.31</v>
-      </c>
-      <c r="S12">
-        <v>3.19</v>
-      </c>
-      <c r="AC12">
-        <v>3.38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" t="s">
-        <v>138</v>
-      </c>
-      <c r="D13" t="s">
-        <v>134</v>
-      </c>
-      <c r="E13" t="s">
-        <v>129</v>
-      </c>
-      <c r="F13" t="s">
-        <v>127</v>
-      </c>
-      <c r="G13" t="s">
-        <v>137</v>
-      </c>
-      <c r="H13" t="s">
-        <v>136</v>
-      </c>
-      <c r="I13">
-        <v>1.41</v>
-      </c>
-      <c r="S13">
-        <v>1.36</v>
-      </c>
-      <c r="U13">
-        <v>1.35</v>
-      </c>
-      <c r="W13">
-        <v>1.44</v>
-      </c>
-      <c r="Y13">
-        <v>1.46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" t="s">
-        <v>139</v>
-      </c>
-      <c r="D14" t="s">
-        <v>142</v>
-      </c>
-      <c r="E14" t="s">
-        <v>129</v>
-      </c>
-      <c r="F14" t="s">
-        <v>127</v>
-      </c>
-      <c r="G14" t="s">
-        <v>140</v>
-      </c>
-      <c r="H14" t="s">
-        <v>141</v>
-      </c>
-      <c r="I14">
-        <v>3.16</v>
-      </c>
-      <c r="AC14">
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" t="s">
-        <v>143</v>
-      </c>
-      <c r="D15" t="s">
-        <v>144</v>
-      </c>
-      <c r="E15" t="s">
-        <v>129</v>
-      </c>
-      <c r="F15" t="s">
-        <v>127</v>
-      </c>
-      <c r="G15" t="s">
-        <v>140</v>
-      </c>
-      <c r="H15" t="s">
-        <v>141</v>
-      </c>
-      <c r="I15">
-        <v>3.16</v>
-      </c>
-      <c r="AC15">
-        <v>2.98</v>
-      </c>
-    </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" t="s">
-        <v>145</v>
-      </c>
-      <c r="D16" t="s">
-        <v>134</v>
-      </c>
-      <c r="E16" t="s">
-        <v>129</v>
-      </c>
-      <c r="F16" t="s">
-        <v>151</v>
-      </c>
-      <c r="G16" t="s">
+      <c r="F21" t="s">
+        <v>186</v>
+      </c>
+      <c r="G21" t="s">
+        <v>150</v>
+      </c>
+      <c r="H21" t="s">
         <v>147</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I21" t="s">
         <v>146</v>
       </c>
-      <c r="I16">
+      <c r="J21">
         <f>1/1.08</f>
         <v>0.92592592592592582</v>
       </c>
-      <c r="K16">
+      <c r="L21">
         <f>1/1.12</f>
         <v>0.89285714285714279</v>
       </c>
-      <c r="M16">
+      <c r="N21">
         <f>1/1.08</f>
         <v>0.92592592592592582</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>194</v>
+      </c>
+      <c r="C22" t="s">
         <v>148</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D22" t="s">
         <v>149</v>
       </c>
-      <c r="D17" t="s">
+      <c r="F22" t="s">
+        <v>186</v>
+      </c>
+      <c r="G22" t="s">
         <v>150</v>
       </c>
-      <c r="F17" t="s">
-        <v>151</v>
-      </c>
-      <c r="G17" t="s">
+      <c r="H22" t="s">
         <v>147</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I22" t="s">
         <v>146</v>
       </c>
-      <c r="I17">
+      <c r="J22">
         <f>1/1.08</f>
         <v>0.92592592592592582</v>
       </c>
-      <c r="K17">
+      <c r="L22">
         <f>1/1.14</f>
         <v>0.87719298245614041</v>
       </c>
-      <c r="M17">
+      <c r="N22">
         <f>1/1.06</f>
         <v>0.94339622641509424</v>
       </c>
-      <c r="Q17">
+      <c r="R22">
         <f>1/0.89</f>
         <v>1.1235955056179776</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" t="s">
-        <v>152</v>
-      </c>
-      <c r="C18" t="s">
-        <v>149</v>
-      </c>
-      <c r="D18" t="s">
-        <v>156</v>
-      </c>
-      <c r="E18" t="s">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>151</v>
+      </c>
+      <c r="C23" t="s">
+        <v>148</v>
+      </c>
+      <c r="D23" t="s">
+        <v>155</v>
+      </c>
+      <c r="E23" t="s">
         <v>129</v>
       </c>
-      <c r="F18" t="s">
-        <v>151</v>
-      </c>
-      <c r="G18" t="s">
+      <c r="F23" t="s">
+        <v>186</v>
+      </c>
+      <c r="G23" t="s">
+        <v>150</v>
+      </c>
+      <c r="H23" t="s">
         <v>147</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I23" t="s">
         <v>146</v>
       </c>
-      <c r="I18">
+      <c r="J23">
         <f>1/1.08</f>
         <v>0.92592592592592582</v>
       </c>
-      <c r="K18">
+      <c r="L23">
         <f>1/1.15</f>
         <v>0.86956521739130443</v>
       </c>
-      <c r="M18">
+      <c r="N23">
         <f>1/0.94</f>
         <v>1.0638297872340425</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" t="s">
-        <v>153</v>
-      </c>
-      <c r="D19" t="s">
-        <v>154</v>
-      </c>
-      <c r="F19" t="s">
-        <v>118</v>
-      </c>
-      <c r="G19" t="s">
-        <v>81</v>
-      </c>
-      <c r="H19" t="s">
-        <v>155</v>
-      </c>
-      <c r="I19">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" t="s">
+        <v>170</v>
+      </c>
+      <c r="D24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" t="s">
+        <v>160</v>
+      </c>
+      <c r="F24" t="s">
+        <v>186</v>
+      </c>
+      <c r="G24" t="s">
+        <v>173</v>
+      </c>
+      <c r="H24" t="s">
+        <v>172</v>
+      </c>
+      <c r="I24" t="s">
+        <v>171</v>
+      </c>
+      <c r="J24">
+        <v>0.76</v>
+      </c>
+      <c r="N24">
+        <v>0.76</v>
+      </c>
+      <c r="Q24">
+        <v>0.82</v>
+      </c>
+      <c r="T24">
+        <v>0.86</v>
+      </c>
+      <c r="X24">
         <v>0.98</v>
       </c>
-    </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" t="s">
-        <v>159</v>
-      </c>
-      <c r="D20" t="s">
-        <v>160</v>
-      </c>
-      <c r="E20" t="s">
-        <v>161</v>
-      </c>
-      <c r="F20" t="s">
-        <v>31</v>
-      </c>
-      <c r="G20" t="s">
-        <v>158</v>
-      </c>
-      <c r="H20" t="s">
-        <v>157</v>
-      </c>
-      <c r="I20">
-        <f>1/1.48</f>
-        <v>0.67567567567567566</v>
-      </c>
-      <c r="AC20">
-        <f>1/1.68</f>
-        <v>0.59523809523809523</v>
-      </c>
-    </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" t="s">
-        <v>162</v>
-      </c>
-      <c r="D21" t="s">
-        <v>160</v>
-      </c>
-      <c r="E21" t="s">
-        <v>161</v>
-      </c>
-      <c r="F21" t="s">
-        <v>118</v>
-      </c>
-      <c r="G21" t="s">
-        <v>81</v>
-      </c>
-      <c r="H21" t="s">
-        <v>155</v>
-      </c>
-      <c r="I21">
-        <v>1.2</v>
-      </c>
-      <c r="N21">
-        <v>1</v>
-      </c>
-      <c r="S21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" t="s">
-        <v>163</v>
-      </c>
-      <c r="D22" t="s">
-        <v>164</v>
-      </c>
-      <c r="E22" t="s">
-        <v>161</v>
-      </c>
-      <c r="F22" t="s">
-        <v>118</v>
-      </c>
-      <c r="G22" t="s">
-        <v>81</v>
-      </c>
-      <c r="H22" t="s">
-        <v>155</v>
-      </c>
-      <c r="I22">
-        <v>1.2</v>
-      </c>
-      <c r="N22">
-        <v>1</v>
-      </c>
-      <c r="S22">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" t="s">
-        <v>165</v>
-      </c>
-      <c r="D23" t="s">
-        <v>29</v>
-      </c>
-      <c r="E23" t="s">
-        <v>161</v>
-      </c>
-      <c r="F23" t="s">
-        <v>118</v>
-      </c>
-      <c r="G23" t="s">
-        <v>81</v>
-      </c>
-      <c r="H23" t="s">
-        <v>155</v>
-      </c>
-      <c r="I23">
-        <v>1.18</v>
-      </c>
-      <c r="P23">
-        <v>1.22</v>
-      </c>
-      <c r="U23">
-        <v>1.47</v>
-      </c>
-    </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" t="s">
-        <v>166</v>
-      </c>
-      <c r="D24" t="s">
-        <v>175</v>
-      </c>
-      <c r="E24" t="s">
-        <v>176</v>
-      </c>
-      <c r="F24" t="s">
-        <v>118</v>
-      </c>
-      <c r="G24" t="s">
-        <v>81</v>
-      </c>
-      <c r="H24" t="s">
-        <v>155</v>
-      </c>
-      <c r="I24">
-        <v>1.18</v>
-      </c>
-      <c r="N24">
-        <v>1.22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="Z24">
+        <v>1.21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -2896,218 +3128,1163 @@
         <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="D25" t="s">
         <v>29</v>
       </c>
       <c r="E25" t="s">
+        <v>160</v>
+      </c>
+      <c r="F25" t="s">
+        <v>186</v>
+      </c>
+      <c r="G25" t="s">
+        <v>173</v>
+      </c>
+      <c r="H25" t="s">
+        <v>172</v>
+      </c>
+      <c r="I25" t="s">
+        <v>171</v>
+      </c>
+      <c r="J25">
+        <f>1/2.4</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="M25">
+        <f>1/2.4</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="P25">
+        <f>1/2.3</f>
+        <v>0.43478260869565222</v>
+      </c>
+      <c r="T25">
+        <f>1/2.2</f>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="W25">
+        <f>1/1.9</f>
+        <v>0.52631578947368418</v>
+      </c>
+      <c r="Y25">
+        <f>1/1.6</f>
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" t="s">
+        <v>186</v>
+      </c>
+      <c r="G26" t="s">
+        <v>118</v>
+      </c>
+      <c r="H26" t="s">
+        <v>81</v>
+      </c>
+      <c r="I26" t="s">
+        <v>154</v>
+      </c>
+      <c r="J26">
+        <v>1.2</v>
+      </c>
+      <c r="Q26">
+        <v>1</v>
+      </c>
+      <c r="Y26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" t="s">
+        <v>152</v>
+      </c>
+      <c r="D27" t="s">
+        <v>153</v>
+      </c>
+      <c r="F27" t="s">
+        <v>186</v>
+      </c>
+      <c r="G27" t="s">
+        <v>118</v>
+      </c>
+      <c r="H27" t="s">
+        <v>81</v>
+      </c>
+      <c r="I27" t="s">
+        <v>154</v>
+      </c>
+      <c r="J27">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" t="s">
         <v>161</v>
       </c>
-      <c r="F25" t="s">
+      <c r="D28" t="s">
+        <v>159</v>
+      </c>
+      <c r="E28" t="s">
+        <v>160</v>
+      </c>
+      <c r="F28" t="s">
+        <v>186</v>
+      </c>
+      <c r="G28" t="s">
         <v>118</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H28" t="s">
+        <v>81</v>
+      </c>
+      <c r="I28" t="s">
+        <v>154</v>
+      </c>
+      <c r="J28">
+        <v>1.2</v>
+      </c>
+      <c r="O28">
+        <v>1</v>
+      </c>
+      <c r="T28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" t="s">
+        <v>162</v>
+      </c>
+      <c r="D29" t="s">
+        <v>163</v>
+      </c>
+      <c r="E29" t="s">
+        <v>160</v>
+      </c>
+      <c r="F29" t="s">
+        <v>186</v>
+      </c>
+      <c r="G29" t="s">
+        <v>118</v>
+      </c>
+      <c r="H29" t="s">
+        <v>81</v>
+      </c>
+      <c r="I29" t="s">
+        <v>154</v>
+      </c>
+      <c r="J29">
+        <v>1.2</v>
+      </c>
+      <c r="O29">
+        <v>1</v>
+      </c>
+      <c r="T29">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" t="s">
+        <v>164</v>
+      </c>
+      <c r="D30" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30" t="s">
+        <v>160</v>
+      </c>
+      <c r="F30" t="s">
+        <v>186</v>
+      </c>
+      <c r="G30" t="s">
+        <v>118</v>
+      </c>
+      <c r="H30" t="s">
+        <v>81</v>
+      </c>
+      <c r="I30" t="s">
+        <v>154</v>
+      </c>
+      <c r="J30">
+        <v>1.18</v>
+      </c>
+      <c r="Q30">
+        <v>1.22</v>
+      </c>
+      <c r="V30">
+        <v>1.47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" t="s">
+        <v>165</v>
+      </c>
+      <c r="D31" t="s">
+        <v>174</v>
+      </c>
+      <c r="E31" t="s">
+        <v>175</v>
+      </c>
+      <c r="F31" t="s">
+        <v>186</v>
+      </c>
+      <c r="G31" t="s">
+        <v>118</v>
+      </c>
+      <c r="H31" t="s">
+        <v>81</v>
+      </c>
+      <c r="I31" t="s">
+        <v>154</v>
+      </c>
+      <c r="J31">
+        <v>1.18</v>
+      </c>
+      <c r="O31">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" t="s">
+        <v>166</v>
+      </c>
+      <c r="D32" t="s">
+        <v>29</v>
+      </c>
+      <c r="E32" t="s">
+        <v>160</v>
+      </c>
+      <c r="F32" t="s">
+        <v>186</v>
+      </c>
+      <c r="G32" t="s">
+        <v>118</v>
+      </c>
+      <c r="H32" t="s">
+        <v>167</v>
+      </c>
+      <c r="I32" t="s">
         <v>168</v>
       </c>
-      <c r="H25" t="s">
+      <c r="J32">
+        <v>1.25</v>
+      </c>
+      <c r="O32">
+        <v>1.24</v>
+      </c>
+      <c r="T32">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="AD32">
+        <v>1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" t="s">
         <v>169</v>
       </c>
-      <c r="I25">
+      <c r="D33" t="s">
+        <v>29</v>
+      </c>
+      <c r="E33" t="s">
+        <v>160</v>
+      </c>
+      <c r="F33" t="s">
+        <v>186</v>
+      </c>
+      <c r="G33" t="s">
+        <v>118</v>
+      </c>
+      <c r="H33" t="s">
+        <v>167</v>
+      </c>
+      <c r="I33" t="s">
+        <v>168</v>
+      </c>
+      <c r="J33">
         <v>1.25</v>
       </c>
-      <c r="N25">
-        <v>1.24</v>
-      </c>
-      <c r="S25">
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="AC25">
+      <c r="O33">
+        <v>0.98</v>
+      </c>
+      <c r="AD33">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" t="s">
+        <v>125</v>
+      </c>
+      <c r="D34" t="s">
+        <v>121</v>
+      </c>
+      <c r="E34" t="s">
+        <v>120</v>
+      </c>
+      <c r="F34" t="s">
+        <v>186</v>
+      </c>
+      <c r="G34" t="s">
+        <v>122</v>
+      </c>
+      <c r="H34" t="s">
+        <v>124</v>
+      </c>
+      <c r="I34" t="s">
+        <v>123</v>
+      </c>
+      <c r="J34">
+        <v>1.47</v>
+      </c>
+      <c r="O34">
+        <v>1.25</v>
+      </c>
+      <c r="T34">
+        <v>1.36</v>
+      </c>
+      <c r="Y34">
+        <v>1.42</v>
+      </c>
+      <c r="AD34">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" t="s">
+        <v>176</v>
+      </c>
+      <c r="D35" t="s">
+        <v>174</v>
+      </c>
+      <c r="E35" t="s">
+        <v>175</v>
+      </c>
+      <c r="F35" t="s">
+        <v>186</v>
+      </c>
+      <c r="G35" t="s">
+        <v>122</v>
+      </c>
+      <c r="H35" t="s">
+        <v>124</v>
+      </c>
+      <c r="I35" t="s">
+        <v>123</v>
+      </c>
+      <c r="J35">
         <v>1.1399999999999999</v>
       </c>
-    </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>1</v>
-      </c>
-      <c r="B26" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" t="s">
-        <v>170</v>
-      </c>
-      <c r="D26" t="s">
-        <v>29</v>
-      </c>
-      <c r="E26" t="s">
-        <v>161</v>
-      </c>
-      <c r="F26" t="s">
+      <c r="P35">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="S35">
+        <v>1.05</v>
+      </c>
+      <c r="V35">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Y35">
+        <v>1.06</v>
+      </c>
+      <c r="AA35">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="AD35">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" t="s">
+        <v>177</v>
+      </c>
+      <c r="D36" t="s">
+        <v>174</v>
+      </c>
+      <c r="E36" t="s">
+        <v>175</v>
+      </c>
+      <c r="F36" t="s">
+        <v>186</v>
+      </c>
+      <c r="G36" t="s">
+        <v>122</v>
+      </c>
+      <c r="H36" t="s">
+        <v>124</v>
+      </c>
+      <c r="I36" t="s">
+        <v>123</v>
+      </c>
+      <c r="J36">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P36">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="S36">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="V36">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Y36">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AA36">
+        <v>1.2</v>
+      </c>
+      <c r="AD36">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" t="s">
+        <v>183</v>
+      </c>
+      <c r="D37" t="s">
+        <v>174</v>
+      </c>
+      <c r="E37" t="s">
+        <v>175</v>
+      </c>
+      <c r="F37" t="s">
+        <v>186</v>
+      </c>
+      <c r="G37" t="s">
+        <v>122</v>
+      </c>
+      <c r="H37" t="s">
+        <v>124</v>
+      </c>
+      <c r="I37" t="s">
+        <v>123</v>
+      </c>
+      <c r="J37">
+        <v>1.36</v>
+      </c>
+      <c r="P37">
+        <v>1.45</v>
+      </c>
+      <c r="U37">
+        <v>1.45</v>
+      </c>
+      <c r="Z37">
+        <v>1.32</v>
+      </c>
+      <c r="AD37">
+        <v>1.86</v>
+      </c>
+    </row>
+    <row r="38" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" t="s">
+        <v>184</v>
+      </c>
+      <c r="D38" t="s">
+        <v>174</v>
+      </c>
+      <c r="E38" t="s">
+        <v>175</v>
+      </c>
+      <c r="F38" t="s">
+        <v>186</v>
+      </c>
+      <c r="G38" t="s">
+        <v>122</v>
+      </c>
+      <c r="H38" t="s">
+        <v>124</v>
+      </c>
+      <c r="I38" t="s">
+        <v>123</v>
+      </c>
+      <c r="J38">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="O38">
+        <v>1.29</v>
+      </c>
+      <c r="T38">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" t="s">
+        <v>187</v>
+      </c>
+      <c r="C39" t="s">
+        <v>191</v>
+      </c>
+      <c r="D39" t="s">
+        <v>190</v>
+      </c>
+      <c r="E39" t="s">
+        <v>189</v>
+      </c>
+      <c r="F39" t="s">
+        <v>188</v>
+      </c>
+      <c r="G39" t="s">
+        <v>150</v>
+      </c>
+      <c r="H39" t="s">
+        <v>192</v>
+      </c>
+      <c r="I39" t="s">
+        <v>193</v>
+      </c>
+      <c r="J39">
+        <v>0.93</v>
+      </c>
+      <c r="R39">
+        <v>0.93</v>
+      </c>
+      <c r="AD39">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" t="s">
+        <v>187</v>
+      </c>
+      <c r="C40" t="s">
+        <v>195</v>
+      </c>
+      <c r="D40" t="s">
+        <v>190</v>
+      </c>
+      <c r="E40" t="s">
+        <v>189</v>
+      </c>
+      <c r="F40" t="s">
+        <v>188</v>
+      </c>
+      <c r="G40" t="s">
+        <v>150</v>
+      </c>
+      <c r="H40" t="s">
+        <v>192</v>
+      </c>
+      <c r="I40" t="s">
+        <v>193</v>
+      </c>
+      <c r="J40">
+        <v>0.93</v>
+      </c>
+      <c r="R40">
+        <v>0.93</v>
+      </c>
+      <c r="AD40">
+        <v>1.1200000000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" t="s">
+        <v>187</v>
+      </c>
+      <c r="C41" t="s">
+        <v>199</v>
+      </c>
+      <c r="D41" t="s">
+        <v>190</v>
+      </c>
+      <c r="E41" t="s">
+        <v>200</v>
+      </c>
+      <c r="F41" t="s">
+        <v>186</v>
+      </c>
+      <c r="G41" t="s">
+        <v>197</v>
+      </c>
+      <c r="H41" t="s">
+        <v>198</v>
+      </c>
+      <c r="I41" t="s">
+        <v>196</v>
+      </c>
+      <c r="J41">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="M41">
+        <v>2.13</v>
+      </c>
+      <c r="O41">
+        <v>2.21</v>
+      </c>
+      <c r="R41">
+        <v>2.27</v>
+      </c>
+      <c r="T41">
+        <v>2.2200000000000002</v>
+      </c>
+    </row>
+    <row r="42" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" t="s">
+        <v>151</v>
+      </c>
+      <c r="C42" t="s">
+        <v>201</v>
+      </c>
+      <c r="D42" t="s">
+        <v>202</v>
+      </c>
+      <c r="E42" t="s">
+        <v>200</v>
+      </c>
+      <c r="F42" t="s">
+        <v>186</v>
+      </c>
+      <c r="G42" t="s">
+        <v>212</v>
+      </c>
+      <c r="H42" t="s">
+        <v>203</v>
+      </c>
+      <c r="I42" t="s">
+        <v>204</v>
+      </c>
+      <c r="J42">
+        <v>0.8</v>
+      </c>
+      <c r="K42">
+        <v>0.8</v>
+      </c>
+      <c r="L42">
+        <v>0.8</v>
+      </c>
+      <c r="M42">
+        <v>0.8</v>
+      </c>
+      <c r="N42">
+        <v>0.8</v>
+      </c>
+      <c r="AE42" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="43" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43" t="s">
+        <v>187</v>
+      </c>
+      <c r="C43" t="s">
+        <v>209</v>
+      </c>
+      <c r="D43" t="s">
+        <v>190</v>
+      </c>
+      <c r="E43" t="s">
+        <v>208</v>
+      </c>
+      <c r="F43" t="s">
+        <v>186</v>
+      </c>
+      <c r="G43" t="s">
+        <v>150</v>
+      </c>
+      <c r="H43" t="s">
+        <v>206</v>
+      </c>
+      <c r="I43" t="s">
+        <v>207</v>
+      </c>
+      <c r="J43">
+        <v>1.17</v>
+      </c>
+      <c r="M43">
+        <v>3.86</v>
+      </c>
+    </row>
+    <row r="44" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>1</v>
+      </c>
+      <c r="B44" t="s">
+        <v>187</v>
+      </c>
+      <c r="C44" t="s">
+        <v>211</v>
+      </c>
+      <c r="D44" t="s">
+        <v>190</v>
+      </c>
+      <c r="E44" t="s">
+        <v>210</v>
+      </c>
+      <c r="F44" t="s">
+        <v>186</v>
+      </c>
+      <c r="G44" t="s">
+        <v>150</v>
+      </c>
+      <c r="H44" t="s">
+        <v>206</v>
+      </c>
+      <c r="I44" t="s">
+        <v>207</v>
+      </c>
+      <c r="J44">
+        <v>1.21</v>
+      </c>
+      <c r="M44">
+        <v>1.25</v>
+      </c>
+      <c r="P44">
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="45" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>1</v>
+      </c>
+      <c r="B45" t="s">
+        <v>187</v>
+      </c>
+      <c r="C45" t="s">
+        <v>215</v>
+      </c>
+      <c r="D45" t="s">
+        <v>190</v>
+      </c>
+      <c r="E45" t="s">
+        <v>213</v>
+      </c>
+      <c r="F45" t="s">
+        <v>186</v>
+      </c>
+      <c r="G45" t="s">
         <v>118</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H45" t="s">
+        <v>167</v>
+      </c>
+      <c r="I45" t="s">
         <v>168</v>
       </c>
-      <c r="H26" t="s">
-        <v>169</v>
-      </c>
-      <c r="I26">
+      <c r="J45">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="M45">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="P45">
         <v>1.25</v>
       </c>
-      <c r="N26">
-        <v>0.98</v>
-      </c>
-      <c r="AC26">
-        <v>1.45</v>
-      </c>
-    </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" t="s">
-        <v>171</v>
-      </c>
-      <c r="D27" t="s">
-        <v>29</v>
-      </c>
-      <c r="E27" t="s">
-        <v>161</v>
-      </c>
-      <c r="F27" t="s">
-        <v>174</v>
-      </c>
-      <c r="G27" t="s">
+    </row>
+    <row r="46" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46" t="s">
+        <v>187</v>
+      </c>
+      <c r="C46" t="s">
+        <v>216</v>
+      </c>
+      <c r="D46" t="s">
+        <v>190</v>
+      </c>
+      <c r="E46" t="s">
+        <v>214</v>
+      </c>
+      <c r="F46" t="s">
+        <v>186</v>
+      </c>
+      <c r="G46" t="s">
+        <v>118</v>
+      </c>
+      <c r="H46" t="s">
+        <v>167</v>
+      </c>
+      <c r="I46" t="s">
+        <v>168</v>
+      </c>
+      <c r="J46">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="M46">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="P46">
+        <v>1.17</v>
+      </c>
+    </row>
+    <row r="47" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>1</v>
+      </c>
+      <c r="B47" t="s">
+        <v>187</v>
+      </c>
+      <c r="C47" t="s">
+        <v>215</v>
+      </c>
+      <c r="D47" t="s">
+        <v>190</v>
+      </c>
+      <c r="E47" t="s">
+        <v>213</v>
+      </c>
+      <c r="F47" t="s">
+        <v>186</v>
+      </c>
+      <c r="G47" t="s">
+        <v>127</v>
+      </c>
+      <c r="H47" t="s">
+        <v>135</v>
+      </c>
+      <c r="I47" t="s">
+        <v>136</v>
+      </c>
+      <c r="J47">
+        <v>1.46</v>
+      </c>
+      <c r="M47">
+        <v>1.7</v>
+      </c>
+      <c r="P47">
+        <v>1.64</v>
+      </c>
+    </row>
+    <row r="48" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>1</v>
+      </c>
+      <c r="B48" t="s">
+        <v>187</v>
+      </c>
+      <c r="C48" t="s">
+        <v>216</v>
+      </c>
+      <c r="D48" t="s">
+        <v>190</v>
+      </c>
+      <c r="E48" t="s">
+        <v>214</v>
+      </c>
+      <c r="F48" t="s">
+        <v>186</v>
+      </c>
+      <c r="G48" t="s">
+        <v>127</v>
+      </c>
+      <c r="H48" t="s">
+        <v>135</v>
+      </c>
+      <c r="I48" t="s">
+        <v>136</v>
+      </c>
+      <c r="J48">
+        <v>1.46</v>
+      </c>
+      <c r="M48">
+        <v>1.52</v>
+      </c>
+      <c r="P48">
+        <v>1.43</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>1</v>
+      </c>
+      <c r="B49" t="s">
+        <v>187</v>
+      </c>
+      <c r="C49" t="s">
+        <v>215</v>
+      </c>
+      <c r="D49" t="s">
+        <v>190</v>
+      </c>
+      <c r="E49" t="s">
+        <v>213</v>
+      </c>
+      <c r="F49" t="s">
+        <v>186</v>
+      </c>
+      <c r="G49" t="s">
+        <v>197</v>
+      </c>
+      <c r="H49" t="s">
+        <v>217</v>
+      </c>
+      <c r="I49" t="s">
+        <v>196</v>
+      </c>
+      <c r="J49">
+        <v>1.91</v>
+      </c>
+      <c r="M49">
+        <v>1.6</v>
+      </c>
+      <c r="P49">
+        <v>1.57</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>1</v>
+      </c>
+      <c r="B50" t="s">
+        <v>187</v>
+      </c>
+      <c r="C50" t="s">
+        <v>216</v>
+      </c>
+      <c r="D50" t="s">
+        <v>190</v>
+      </c>
+      <c r="E50" t="s">
+        <v>214</v>
+      </c>
+      <c r="F50" t="s">
+        <v>186</v>
+      </c>
+      <c r="G50" t="s">
+        <v>197</v>
+      </c>
+      <c r="H50" t="s">
+        <v>217</v>
+      </c>
+      <c r="I50" t="s">
+        <v>196</v>
+      </c>
+      <c r="J50">
+        <v>1.91</v>
+      </c>
+      <c r="M50">
+        <v>1.82</v>
+      </c>
+      <c r="P50">
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>1</v>
+      </c>
+      <c r="B51" t="s">
+        <v>187</v>
+      </c>
+      <c r="C51" t="s">
+        <v>219</v>
+      </c>
+      <c r="D51" t="s">
+        <v>190</v>
+      </c>
+      <c r="E51" t="s">
+        <v>220</v>
+      </c>
+      <c r="F51" t="s">
+        <v>221</v>
+      </c>
+      <c r="G51" t="s">
+        <v>150</v>
+      </c>
+      <c r="H51" t="s">
+        <v>116</v>
+      </c>
+      <c r="I51" t="s">
+        <v>77</v>
+      </c>
+      <c r="J51">
+        <v>1.92</v>
+      </c>
+      <c r="M51">
+        <v>2.11</v>
+      </c>
+      <c r="O51">
+        <v>1.7</v>
+      </c>
+      <c r="P51">
+        <v>1.86</v>
+      </c>
+      <c r="S51">
+        <v>1.91</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>1</v>
+      </c>
+      <c r="B52" t="s">
+        <v>187</v>
+      </c>
+      <c r="C52" t="s">
+        <v>222</v>
+      </c>
+      <c r="D52" t="s">
+        <v>190</v>
+      </c>
+      <c r="E52" t="s">
+        <v>220</v>
+      </c>
+      <c r="F52" t="s">
+        <v>221</v>
+      </c>
+      <c r="G52" t="s">
+        <v>150</v>
+      </c>
+      <c r="H52" t="s">
+        <v>116</v>
+      </c>
+      <c r="I52" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B53" t="s">
+        <v>187</v>
+      </c>
+      <c r="C53" t="s">
+        <v>226</v>
+      </c>
+      <c r="D53" t="s">
+        <v>190</v>
+      </c>
+      <c r="E53" t="s">
+        <v>225</v>
+      </c>
+      <c r="F53" t="s">
+        <v>221</v>
+      </c>
+      <c r="G53" t="s">
         <v>173</v>
       </c>
-      <c r="H27" t="s">
-        <v>172</v>
-      </c>
-      <c r="I27">
-        <v>0.76</v>
-      </c>
-      <c r="M27">
-        <v>0.76</v>
-      </c>
-      <c r="P27">
-        <v>0.82</v>
-      </c>
-      <c r="S27">
-        <v>0.86</v>
-      </c>
-      <c r="W27">
-        <v>0.98</v>
-      </c>
-      <c r="Y27">
-        <v>1.21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>1</v>
-      </c>
-      <c r="B28" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28" t="s">
-        <v>177</v>
-      </c>
-      <c r="D28" t="s">
-        <v>175</v>
-      </c>
-      <c r="E28" t="s">
-        <v>176</v>
-      </c>
-      <c r="F28" t="s">
-        <v>122</v>
-      </c>
-      <c r="G28" t="s">
-        <v>124</v>
-      </c>
-      <c r="H28" t="s">
-        <v>123</v>
-      </c>
-      <c r="I28">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="O28">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="R28">
-        <v>1.05</v>
-      </c>
-      <c r="U28">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="X28">
-        <v>1.06</v>
-      </c>
-      <c r="Z28">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="AC28">
-        <v>1.22</v>
-      </c>
-    </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>1</v>
-      </c>
-      <c r="B29" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" t="s">
-        <v>178</v>
-      </c>
-      <c r="D29" t="s">
-        <v>175</v>
-      </c>
-      <c r="E29" t="s">
-        <v>176</v>
-      </c>
-      <c r="F29" t="s">
-        <v>122</v>
-      </c>
-      <c r="G29" t="s">
-        <v>124</v>
-      </c>
-      <c r="H29" t="s">
-        <v>123</v>
-      </c>
-      <c r="I29">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="O29">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="R29">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="U29">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="X29">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="Z29">
-        <v>1.2</v>
-      </c>
-      <c r="AC29">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" t="s">
-        <v>10</v>
+      <c r="H53" t="s">
+        <v>223</v>
+      </c>
+      <c r="I53" t="s">
+        <v>224</v>
+      </c>
+      <c r="J53">
+        <v>2.25</v>
+      </c>
+      <c r="K53">
+        <v>1.98</v>
+      </c>
+      <c r="L53">
+        <v>2.23</v>
+      </c>
+      <c r="M53">
+        <v>2.27</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="C60" t="s">
+        <v>218</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:AD37">
+    <sortCondition ref="G2:G37"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>

</xml_diff>

<commit_message>
End of Algae FCR done. Dowloaded yeast. Start of MS - first push.
</commit_message>
<xml_diff>
--- a/alternativefeeddata.xlsx
+++ b/alternativefeeddata.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="254">
   <si>
     <t xml:space="preserve">Taxon </t>
   </si>
@@ -448,9 +448,6 @@
     <t xml:space="preserve">Rangcharyulu et al 2003 </t>
   </si>
   <si>
-    <t xml:space="preserve">Mutliple: Silver, mrigal, rohu, catla </t>
-  </si>
-  <si>
     <t xml:space="preserve">Hypophthalmychthys molitrix, Cirrhinus mrigala, Labeo rohita, and catla catla </t>
   </si>
   <si>
@@ -643,9 +640,6 @@
     <t xml:space="preserve">Seriola rivoliana </t>
   </si>
   <si>
-    <t xml:space="preserve">%of algae as proetin source </t>
-  </si>
-  <si>
     <t>Atlantic cod </t>
   </si>
   <si>
@@ -676,9 +670,6 @@
     <t xml:space="preserve">Kiron et al 2012 </t>
   </si>
   <si>
-    <t>Kiron et al 2013</t>
-  </si>
-  <si>
     <t>Whiteleg shrimp</t>
   </si>
   <si>
@@ -707,6 +698,96 @@
   </si>
   <si>
     <t>Kim et al 2013</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0044848617315132?via%3Dihub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">See perez-velasquez </t>
+  </si>
+  <si>
+    <t>Appler and Kelley 1983</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cladophora glomerata </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bawdy 2008 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Algal meal </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chlorella spp </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year </t>
+  </si>
+  <si>
+    <t>Catla</t>
+  </si>
+  <si>
+    <t>Rohu</t>
+  </si>
+  <si>
+    <t>Catla catla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mixed: Silver, mrigal, rohu, catla </t>
+  </si>
+  <si>
+    <t>Nandeesha et al 2001</t>
+  </si>
+  <si>
+    <t>Spirulina platensis</t>
+  </si>
+  <si>
+    <t>Nandeesha et al 2002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ameiurus melas </t>
+  </si>
+  <si>
+    <t>Spirulina maxima</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olivera-Novoa </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oreochromis mossambicus </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isocrysis sp. </t>
+  </si>
+  <si>
+    <t>Palmegianao et al 2009</t>
+  </si>
+  <si>
+    <t>*Not clear values for replacement percentages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poryphora dioica </t>
+  </si>
+  <si>
+    <t>Solar-Vila 2009</t>
+  </si>
+  <si>
+    <t>Tetraselmis suecica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tulli et al 2002 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fish trimmings </t>
+  </si>
+  <si>
+    <t>Poryphora sp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Walker et al 2009 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">%of algae as protein source </t>
   </si>
 </sst>
 </file>
@@ -1036,7 +1117,7 @@
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A44" sqref="A44"/>
@@ -2086,34 +2167,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE60"/>
+  <dimension ref="A1:AF75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="9" ySplit="1" topLeftCell="J12" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="10" ySplit="1" topLeftCell="K37" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B53" sqref="B53"/>
+      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="27.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.453125" customWidth="1"/>
-    <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.1796875" customWidth="1"/>
-    <col min="11" max="11" width="12" customWidth="1"/>
-    <col min="12" max="12" width="8.1796875" customWidth="1"/>
-    <col min="13" max="13" width="8.54296875" customWidth="1"/>
-    <col min="14" max="14" width="8.7265625" customWidth="1"/>
-    <col min="15" max="15" width="10.1796875" customWidth="1"/>
-    <col min="16" max="16" width="8.54296875" customWidth="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.453125" customWidth="1"/>
+    <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.08984375" customWidth="1"/>
+    <col min="11" max="11" width="12.1796875" customWidth="1"/>
+    <col min="12" max="12" width="12" customWidth="1"/>
+    <col min="13" max="13" width="8.1796875" customWidth="1"/>
+    <col min="14" max="14" width="8.54296875" customWidth="1"/>
+    <col min="15" max="15" width="8.7265625" customWidth="1"/>
+    <col min="16" max="16" width="10.1796875" customWidth="1"/>
+    <col min="17" max="17" width="8.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>90</v>
       </c>
@@ -2124,132 +2206,138 @@
         <v>114</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>185</v>
-      </c>
       <c r="G1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C2" t="s">
         <v>131</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2">
+        <v>1994</v>
+      </c>
+      <c r="E2" t="s">
         <v>126</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>129</v>
       </c>
-      <c r="F2" t="s">
-        <v>186</v>
-      </c>
       <c r="G2" t="s">
+        <v>185</v>
+      </c>
+      <c r="H2" t="s">
         <v>127</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>128</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>130</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>2.0499999999999998</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>1.96</v>
       </c>
-      <c r="V2">
+      <c r="W2">
         <v>1.92</v>
       </c>
-      <c r="Z2">
+      <c r="AA2">
         <v>2</v>
       </c>
-      <c r="AD2">
+      <c r="AE2">
         <v>2.0699999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2259,35 +2347,38 @@
       <c r="C3" t="s">
         <v>133</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3">
+        <v>1990</v>
+      </c>
+      <c r="E3" t="s">
         <v>134</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>129</v>
       </c>
-      <c r="F3" t="s">
-        <v>186</v>
-      </c>
       <c r="G3" t="s">
+        <v>185</v>
+      </c>
+      <c r="H3" t="s">
         <v>127</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>135</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>136</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>3.31</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <v>3.19</v>
       </c>
-      <c r="AD3">
+      <c r="AE3">
         <v>3.38</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -2297,41 +2388,44 @@
       <c r="C4" t="s">
         <v>138</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4">
+        <v>2013</v>
+      </c>
+      <c r="E4" t="s">
         <v>134</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>129</v>
       </c>
-      <c r="F4" t="s">
-        <v>186</v>
-      </c>
       <c r="G4" t="s">
+        <v>185</v>
+      </c>
+      <c r="H4" t="s">
         <v>127</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>137</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>136</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>1.41</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>1.36</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>1.35</v>
       </c>
-      <c r="X4">
+      <c r="Y4">
         <v>1.44</v>
       </c>
-      <c r="Z4">
+      <c r="AA4">
         <v>1.46</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -2341,67 +2435,73 @@
       <c r="C5" t="s">
         <v>139</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5">
+        <v>2003</v>
+      </c>
+      <c r="E5" t="s">
+        <v>141</v>
+      </c>
+      <c r="F5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G5" t="s">
+        <v>185</v>
+      </c>
+      <c r="H5" t="s">
+        <v>127</v>
+      </c>
+      <c r="I5" t="s">
+        <v>235</v>
+      </c>
+      <c r="J5" t="s">
+        <v>140</v>
+      </c>
+      <c r="K5">
+        <v>3.16</v>
+      </c>
+      <c r="AE5">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
         <v>142</v>
       </c>
-      <c r="E5" t="s">
+      <c r="D6">
+        <v>2004</v>
+      </c>
+      <c r="E6" t="s">
+        <v>143</v>
+      </c>
+      <c r="F6" t="s">
         <v>129</v>
       </c>
-      <c r="F5" t="s">
-        <v>186</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="G6" t="s">
+        <v>185</v>
+      </c>
+      <c r="H6" t="s">
         <v>127</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I6" t="s">
+        <v>235</v>
+      </c>
+      <c r="J6" t="s">
         <v>140</v>
       </c>
-      <c r="I5" t="s">
-        <v>141</v>
-      </c>
-      <c r="J5">
+      <c r="K6">
         <v>3.16</v>
       </c>
-      <c r="AD5">
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>143</v>
-      </c>
-      <c r="D6" t="s">
-        <v>144</v>
-      </c>
-      <c r="E6" t="s">
-        <v>129</v>
-      </c>
-      <c r="F6" t="s">
-        <v>186</v>
-      </c>
-      <c r="G6" t="s">
-        <v>127</v>
-      </c>
-      <c r="H6" t="s">
-        <v>140</v>
-      </c>
-      <c r="I6" t="s">
-        <v>141</v>
-      </c>
-      <c r="J6">
-        <v>3.16</v>
-      </c>
-      <c r="AD6">
+      <c r="AE6">
         <v>2.98</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -2411,49 +2511,52 @@
       <c r="C7" t="s">
         <v>34</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7">
+        <v>2001</v>
+      </c>
+      <c r="E7" t="s">
         <v>17</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>4</v>
       </c>
-      <c r="F7" t="s">
-        <v>186</v>
-      </c>
       <c r="G7" t="s">
+        <v>185</v>
+      </c>
+      <c r="H7" t="s">
         <v>31</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>32</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>91</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>0.76</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <f>1/1.33</f>
         <v>0.75187969924812026</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <f>1/1.19</f>
         <v>0.84033613445378152</v>
       </c>
-      <c r="V7">
+      <c r="W7">
         <f>1/1.02</f>
         <v>0.98039215686274506</v>
       </c>
-      <c r="Z7">
+      <c r="AA7">
         <f>1/1.12</f>
         <v>0.89285714285714279</v>
       </c>
-      <c r="AD7">
+      <c r="AE7">
         <f>1/0.89</f>
         <v>1.1235955056179776</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -2463,41 +2566,44 @@
       <c r="C8" t="s">
         <v>69</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8">
+        <v>2011</v>
+      </c>
+      <c r="E8" t="s">
         <v>68</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>70</v>
       </c>
-      <c r="F8" t="s">
-        <v>186</v>
-      </c>
       <c r="G8" t="s">
+        <v>185</v>
+      </c>
+      <c r="H8" t="s">
         <v>31</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>32</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>91</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>1.51</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>1.46</v>
       </c>
-      <c r="T8">
+      <c r="U8">
         <v>1.81</v>
       </c>
-      <c r="Y8">
+      <c r="Z8">
         <v>1.72</v>
       </c>
-      <c r="AD8">
+      <c r="AE8">
         <v>1.91</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -2507,41 +2613,44 @@
       <c r="C9" t="s">
         <v>74</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9">
+        <v>2009</v>
+      </c>
+      <c r="E9" t="s">
         <v>72</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>73</v>
       </c>
-      <c r="F9" t="s">
-        <v>186</v>
-      </c>
       <c r="G9" t="s">
+        <v>185</v>
+      </c>
+      <c r="H9" t="s">
         <v>31</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>71</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>91</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>2.96</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>3.09</v>
       </c>
-      <c r="T9">
+      <c r="U9">
         <v>2.88</v>
       </c>
-      <c r="Y9">
+      <c r="Z9">
         <v>3.67</v>
       </c>
-      <c r="AD9">
+      <c r="AE9">
         <v>3.44</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -2551,29 +2660,35 @@
       <c r="C10" t="s">
         <v>75</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10">
+        <v>2015</v>
+      </c>
+      <c r="E10" t="s">
         <v>17</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>4</v>
       </c>
-      <c r="F10" t="s">
-        <v>186</v>
-      </c>
       <c r="G10" t="s">
+        <v>185</v>
+      </c>
+      <c r="H10" t="s">
         <v>31</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>76</v>
       </c>
-      <c r="J10">
+      <c r="J10" t="s">
+        <v>239</v>
+      </c>
+      <c r="K10">
         <v>3.8</v>
       </c>
-      <c r="T10">
+      <c r="U10">
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -2581,36 +2696,39 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
+        <v>157</v>
+      </c>
+      <c r="D11">
+        <v>2005</v>
+      </c>
+      <c r="E11" t="s">
         <v>158</v>
       </c>
-      <c r="D11" t="s">
+      <c r="F11" t="s">
         <v>159</v>
       </c>
-      <c r="E11" t="s">
-        <v>160</v>
-      </c>
-      <c r="F11" t="s">
-        <v>186</v>
-      </c>
       <c r="G11" t="s">
+        <v>185</v>
+      </c>
+      <c r="H11" t="s">
         <v>31</v>
-      </c>
-      <c r="H11" t="s">
-        <v>157</v>
       </c>
       <c r="I11" t="s">
         <v>156</v>
       </c>
-      <c r="J11">
+      <c r="J11" t="s">
+        <v>155</v>
+      </c>
+      <c r="K11">
         <f>1/1.48</f>
         <v>0.67567567567567566</v>
       </c>
-      <c r="AD11">
+      <c r="AE11">
         <f>1/1.68</f>
         <v>0.59523809523809523</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -2618,221 +2736,239 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
+        <v>178</v>
+      </c>
+      <c r="D12">
+        <v>2009</v>
+      </c>
+      <c r="E12" t="s">
+        <v>173</v>
+      </c>
+      <c r="F12" t="s">
+        <v>174</v>
+      </c>
+      <c r="G12" t="s">
+        <v>185</v>
+      </c>
+      <c r="H12" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" t="s">
+        <v>32</v>
+      </c>
+      <c r="J12" t="s">
+        <v>91</v>
+      </c>
+      <c r="K12">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="U12">
+        <v>1.17</v>
+      </c>
+      <c r="AE12">
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
         <v>179</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13">
+        <v>2003</v>
+      </c>
+      <c r="E13" t="s">
+        <v>173</v>
+      </c>
+      <c r="F13" t="s">
         <v>174</v>
       </c>
-      <c r="E12" t="s">
-        <v>175</v>
-      </c>
-      <c r="F12" t="s">
-        <v>186</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="G13" t="s">
+        <v>185</v>
+      </c>
+      <c r="H13" t="s">
         <v>31</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I13" t="s">
         <v>32</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J13" t="s">
         <v>91</v>
       </c>
-      <c r="J12">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="T12">
-        <v>1.17</v>
-      </c>
-      <c r="AD12">
-        <v>1.1599999999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="K13">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="AE13">
+        <v>2.58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>179</v>
+      </c>
+      <c r="D14">
+        <v>2003</v>
+      </c>
+      <c r="E14" t="s">
+        <v>173</v>
+      </c>
+      <c r="F14" t="s">
+        <v>174</v>
+      </c>
+      <c r="G14" t="s">
+        <v>185</v>
+      </c>
+      <c r="H14" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" t="s">
+        <v>32</v>
+      </c>
+      <c r="J14" t="s">
+        <v>91</v>
+      </c>
+      <c r="K14">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="AE14">
+        <v>3.52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
+        <v>179</v>
+      </c>
+      <c r="D15">
+        <v>2003</v>
+      </c>
+      <c r="E15" t="s">
+        <v>173</v>
+      </c>
+      <c r="F15" t="s">
+        <v>174</v>
+      </c>
+      <c r="G15" t="s">
+        <v>185</v>
+      </c>
+      <c r="H15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I15" t="s">
+        <v>32</v>
+      </c>
+      <c r="J15" t="s">
+        <v>91</v>
+      </c>
+      <c r="K15">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="AE15">
+        <v>2.2400000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>179</v>
+      </c>
+      <c r="D16">
+        <v>2003</v>
+      </c>
+      <c r="E16" t="s">
+        <v>173</v>
+      </c>
+      <c r="F16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G16" t="s">
+        <v>185</v>
+      </c>
+      <c r="H16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" t="s">
+        <v>32</v>
+      </c>
+      <c r="J16" t="s">
+        <v>91</v>
+      </c>
+      <c r="K16">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="AE16">
+        <v>2.65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>150</v>
+      </c>
+      <c r="C17" t="s">
+        <v>181</v>
+      </c>
+      <c r="D17">
+        <v>2010</v>
+      </c>
+      <c r="E17" t="s">
         <v>180</v>
       </c>
-      <c r="D13" t="s">
+      <c r="F17" t="s">
         <v>174</v>
       </c>
-      <c r="E13" t="s">
-        <v>175</v>
-      </c>
-      <c r="F13" t="s">
-        <v>186</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="G17" t="s">
+        <v>185</v>
+      </c>
+      <c r="H17" t="s">
         <v>31</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I17" t="s">
         <v>32</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J17" t="s">
         <v>91</v>
       </c>
-      <c r="J13">
-        <v>2.2599999999999998</v>
-      </c>
-      <c r="AD13">
-        <v>2.58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" t="s">
-        <v>180</v>
-      </c>
-      <c r="D14" t="s">
-        <v>174</v>
-      </c>
-      <c r="E14" t="s">
-        <v>175</v>
-      </c>
-      <c r="F14" t="s">
-        <v>186</v>
-      </c>
-      <c r="G14" t="s">
-        <v>31</v>
-      </c>
-      <c r="H14" t="s">
-        <v>32</v>
-      </c>
-      <c r="I14" t="s">
-        <v>91</v>
-      </c>
-      <c r="J14">
-        <v>2.2599999999999998</v>
-      </c>
-      <c r="AD14">
-        <v>3.52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" t="s">
-        <v>180</v>
-      </c>
-      <c r="D15" t="s">
-        <v>174</v>
-      </c>
-      <c r="E15" t="s">
-        <v>175</v>
-      </c>
-      <c r="F15" t="s">
-        <v>186</v>
-      </c>
-      <c r="G15" t="s">
-        <v>31</v>
-      </c>
-      <c r="H15" t="s">
-        <v>32</v>
-      </c>
-      <c r="I15" t="s">
-        <v>91</v>
-      </c>
-      <c r="J15">
-        <v>2.2599999999999998</v>
-      </c>
-      <c r="AD15">
-        <v>2.2400000000000002</v>
-      </c>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" t="s">
-        <v>180</v>
-      </c>
-      <c r="D16" t="s">
-        <v>174</v>
-      </c>
-      <c r="E16" t="s">
-        <v>175</v>
-      </c>
-      <c r="F16" t="s">
-        <v>186</v>
-      </c>
-      <c r="G16" t="s">
-        <v>31</v>
-      </c>
-      <c r="H16" t="s">
-        <v>32</v>
-      </c>
-      <c r="I16" t="s">
-        <v>91</v>
-      </c>
-      <c r="J16">
-        <v>2.2599999999999998</v>
-      </c>
-      <c r="AD16">
-        <v>2.65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" t="s">
-        <v>151</v>
-      </c>
-      <c r="C17" t="s">
-        <v>182</v>
-      </c>
-      <c r="D17" t="s">
-        <v>181</v>
-      </c>
-      <c r="E17" t="s">
-        <v>175</v>
-      </c>
-      <c r="F17" t="s">
-        <v>186</v>
-      </c>
-      <c r="G17" t="s">
-        <v>31</v>
-      </c>
-      <c r="H17" t="s">
-        <v>32</v>
-      </c>
-      <c r="I17" t="s">
-        <v>91</v>
-      </c>
-      <c r="J17">
+      <c r="K17">
         <v>1.34</v>
       </c>
-      <c r="O17">
+      <c r="P17">
         <v>1.36</v>
       </c>
-      <c r="T17">
+      <c r="U17">
         <v>1.44</v>
       </c>
-      <c r="Y17">
+      <c r="Z17">
         <v>1.61</v>
       </c>
-      <c r="AD17">
+      <c r="AE17">
         <v>1.67</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -2842,38 +2978,41 @@
       <c r="C18" t="s">
         <v>85</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18">
+        <v>2010</v>
+      </c>
+      <c r="E18" t="s">
         <v>84</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>83</v>
       </c>
-      <c r="F18" t="s">
-        <v>186</v>
-      </c>
       <c r="G18" t="s">
+        <v>185</v>
+      </c>
+      <c r="H18" t="s">
         <v>119</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>71</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>91</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>0.89</v>
       </c>
-      <c r="O18">
+      <c r="P18">
         <v>0.7</v>
       </c>
-      <c r="T18">
+      <c r="U18">
         <v>0.99</v>
       </c>
-      <c r="Y18">
+      <c r="Z18">
         <v>1.04</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -2883,35 +3022,38 @@
       <c r="C19" t="s">
         <v>79</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19">
+        <v>2018</v>
+      </c>
+      <c r="E19" t="s">
         <v>17</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>4</v>
       </c>
-      <c r="F19" t="s">
-        <v>186</v>
-      </c>
       <c r="G19" t="s">
-        <v>150</v>
+        <v>185</v>
       </c>
       <c r="H19" t="s">
+        <v>149</v>
+      </c>
+      <c r="I19" t="s">
         <v>116</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>77</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>1.34</v>
       </c>
-      <c r="Q19">
+      <c r="R19">
         <v>1.02</v>
       </c>
-      <c r="X19">
+      <c r="Y19">
         <v>1.28</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -2921,35 +3063,38 @@
       <c r="C20" t="s">
         <v>80</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20">
+        <v>2016</v>
+      </c>
+      <c r="E20" t="s">
         <v>17</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>4</v>
       </c>
-      <c r="F20" t="s">
-        <v>186</v>
-      </c>
       <c r="G20" t="s">
-        <v>150</v>
+        <v>185</v>
       </c>
       <c r="H20" t="s">
+        <v>149</v>
+      </c>
+      <c r="I20" t="s">
         <v>78</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>117</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>0.9</v>
       </c>
-      <c r="Q20">
+      <c r="R20">
         <v>0.91</v>
       </c>
-      <c r="X20">
+      <c r="Y20">
         <v>0.99</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -2957,123 +3102,132 @@
         <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>145</v>
-      </c>
-      <c r="D21" t="s">
+        <v>144</v>
+      </c>
+      <c r="D21">
+        <v>2012</v>
+      </c>
+      <c r="E21" t="s">
         <v>134</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>129</v>
       </c>
-      <c r="F21" t="s">
-        <v>186</v>
-      </c>
       <c r="G21" t="s">
-        <v>150</v>
+        <v>185</v>
       </c>
       <c r="H21" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="I21" t="s">
         <v>146</v>
       </c>
-      <c r="J21">
+      <c r="J21" t="s">
+        <v>145</v>
+      </c>
+      <c r="K21">
         <f>1/1.08</f>
         <v>0.92592592592592582</v>
       </c>
-      <c r="L21">
+      <c r="M21">
         <f>1/1.12</f>
         <v>0.89285714285714279</v>
       </c>
-      <c r="N21">
+      <c r="O21">
         <f>1/1.08</f>
         <v>0.92592592592592582</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C22" t="s">
+        <v>147</v>
+      </c>
+      <c r="D22">
+        <v>2013</v>
+      </c>
+      <c r="E22" t="s">
         <v>148</v>
       </c>
-      <c r="D22" t="s">
+      <c r="G22" t="s">
+        <v>185</v>
+      </c>
+      <c r="H22" t="s">
         <v>149</v>
-      </c>
-      <c r="F22" t="s">
-        <v>186</v>
-      </c>
-      <c r="G22" t="s">
-        <v>150</v>
-      </c>
-      <c r="H22" t="s">
-        <v>147</v>
       </c>
       <c r="I22" t="s">
         <v>146</v>
       </c>
-      <c r="J22">
+      <c r="J22" t="s">
+        <v>145</v>
+      </c>
+      <c r="K22">
         <f>1/1.08</f>
         <v>0.92592592592592582</v>
       </c>
-      <c r="L22">
+      <c r="M22">
         <f>1/1.14</f>
         <v>0.87719298245614041</v>
       </c>
-      <c r="N22">
+      <c r="O22">
         <f>1/1.06</f>
         <v>0.94339622641509424</v>
       </c>
-      <c r="R22">
+      <c r="S22">
         <f>1/0.89</f>
         <v>1.1235955056179776</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C23" t="s">
-        <v>148</v>
-      </c>
-      <c r="D23" t="s">
-        <v>155</v>
+        <v>147</v>
+      </c>
+      <c r="D23">
+        <v>2013</v>
       </c>
       <c r="E23" t="s">
+        <v>154</v>
+      </c>
+      <c r="F23" t="s">
         <v>129</v>
       </c>
-      <c r="F23" t="s">
-        <v>186</v>
-      </c>
       <c r="G23" t="s">
-        <v>150</v>
+        <v>185</v>
       </c>
       <c r="H23" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="I23" t="s">
         <v>146</v>
       </c>
-      <c r="J23">
+      <c r="J23" t="s">
+        <v>145</v>
+      </c>
+      <c r="K23">
         <f>1/1.08</f>
         <v>0.92592592592592582</v>
       </c>
-      <c r="L23">
+      <c r="M23">
         <f>1/1.15</f>
         <v>0.86956521739130443</v>
       </c>
-      <c r="N23">
+      <c r="O23">
         <f>1/0.94</f>
         <v>1.0638297872340425</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -3081,19 +3235,19 @@
         <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>170</v>
-      </c>
-      <c r="D24" t="s">
+        <v>169</v>
+      </c>
+      <c r="D24">
+        <v>2018</v>
+      </c>
+      <c r="E24" t="s">
         <v>29</v>
       </c>
-      <c r="E24" t="s">
-        <v>160</v>
-      </c>
       <c r="F24" t="s">
-        <v>186</v>
+        <v>159</v>
       </c>
       <c r="G24" t="s">
-        <v>173</v>
+        <v>185</v>
       </c>
       <c r="H24" t="s">
         <v>172</v>
@@ -3101,26 +3255,29 @@
       <c r="I24" t="s">
         <v>171</v>
       </c>
-      <c r="J24">
+      <c r="J24" t="s">
+        <v>170</v>
+      </c>
+      <c r="K24">
         <v>0.76</v>
       </c>
-      <c r="N24">
+      <c r="O24">
         <v>0.76</v>
       </c>
-      <c r="Q24">
+      <c r="R24">
         <v>0.82</v>
       </c>
-      <c r="T24">
+      <c r="U24">
         <v>0.86</v>
       </c>
-      <c r="X24">
+      <c r="Y24">
         <v>0.98</v>
       </c>
-      <c r="Z24">
+      <c r="AA24">
         <v>1.21</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -3128,19 +3285,19 @@
         <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>178</v>
-      </c>
-      <c r="D25" t="s">
+        <v>177</v>
+      </c>
+      <c r="D25">
+        <v>2013</v>
+      </c>
+      <c r="E25" t="s">
         <v>29</v>
       </c>
-      <c r="E25" t="s">
-        <v>160</v>
-      </c>
       <c r="F25" t="s">
-        <v>186</v>
+        <v>159</v>
       </c>
       <c r="G25" t="s">
-        <v>173</v>
+        <v>185</v>
       </c>
       <c r="H25" t="s">
         <v>172</v>
@@ -3148,32 +3305,35 @@
       <c r="I25" t="s">
         <v>171</v>
       </c>
-      <c r="J25">
+      <c r="J25" t="s">
+        <v>170</v>
+      </c>
+      <c r="K25">
         <f>1/2.4</f>
         <v>0.41666666666666669</v>
       </c>
-      <c r="M25">
+      <c r="N25">
         <f>1/2.4</f>
         <v>0.41666666666666669</v>
       </c>
-      <c r="P25">
+      <c r="Q25">
         <f>1/2.3</f>
         <v>0.43478260869565222</v>
       </c>
-      <c r="T25">
+      <c r="U25">
         <f>1/2.2</f>
         <v>0.45454545454545453</v>
       </c>
-      <c r="W25">
+      <c r="X25">
         <f>1/1.9</f>
         <v>0.52631578947368418</v>
       </c>
-      <c r="Y25">
+      <c r="Z25">
         <f>1/1.6</f>
         <v>0.625</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -3183,35 +3343,38 @@
       <c r="C26" t="s">
         <v>82</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26">
+        <v>2015</v>
+      </c>
+      <c r="E26" t="s">
         <v>17</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>4</v>
       </c>
-      <c r="F26" t="s">
-        <v>186</v>
-      </c>
       <c r="G26" t="s">
+        <v>185</v>
+      </c>
+      <c r="H26" t="s">
         <v>118</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>81</v>
       </c>
-      <c r="I26" t="s">
-        <v>154</v>
-      </c>
-      <c r="J26">
+      <c r="J26" t="s">
+        <v>153</v>
+      </c>
+      <c r="K26">
         <v>1.2</v>
       </c>
-      <c r="Q26">
-        <v>1</v>
-      </c>
-      <c r="Y26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="R26">
+        <v>1</v>
+      </c>
+      <c r="Z26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -3219,256 +3382,277 @@
         <v>10</v>
       </c>
       <c r="C27" t="s">
+        <v>151</v>
+      </c>
+      <c r="D27">
+        <v>2011</v>
+      </c>
+      <c r="E27" t="s">
         <v>152</v>
       </c>
-      <c r="D27" t="s">
+      <c r="G27" t="s">
+        <v>185</v>
+      </c>
+      <c r="H27" t="s">
+        <v>118</v>
+      </c>
+      <c r="I27" t="s">
+        <v>81</v>
+      </c>
+      <c r="J27" t="s">
         <v>153</v>
       </c>
-      <c r="F27" t="s">
-        <v>186</v>
-      </c>
-      <c r="G27" t="s">
+      <c r="K27">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" t="s">
+        <v>160</v>
+      </c>
+      <c r="D28">
+        <v>2011</v>
+      </c>
+      <c r="E28" t="s">
+        <v>158</v>
+      </c>
+      <c r="F28" t="s">
+        <v>159</v>
+      </c>
+      <c r="G28" t="s">
+        <v>185</v>
+      </c>
+      <c r="H28" t="s">
         <v>118</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I28" t="s">
         <v>81</v>
       </c>
-      <c r="I27" t="s">
-        <v>154</v>
-      </c>
-      <c r="J27">
+      <c r="J28" t="s">
+        <v>153</v>
+      </c>
+      <c r="K28">
+        <v>1.2</v>
+      </c>
+      <c r="P28">
+        <v>1</v>
+      </c>
+      <c r="U28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" t="s">
+        <v>161</v>
+      </c>
+      <c r="D29">
+        <v>2012</v>
+      </c>
+      <c r="E29" t="s">
+        <v>162</v>
+      </c>
+      <c r="F29" t="s">
+        <v>159</v>
+      </c>
+      <c r="G29" t="s">
+        <v>185</v>
+      </c>
+      <c r="H29" t="s">
+        <v>118</v>
+      </c>
+      <c r="I29" t="s">
+        <v>81</v>
+      </c>
+      <c r="J29" t="s">
+        <v>153</v>
+      </c>
+      <c r="K29">
+        <v>1.2</v>
+      </c>
+      <c r="P29">
+        <v>1</v>
+      </c>
+      <c r="U29">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" t="s">
+        <v>163</v>
+      </c>
+      <c r="D30">
+        <v>2007</v>
+      </c>
+      <c r="E30" t="s">
+        <v>29</v>
+      </c>
+      <c r="F30" t="s">
+        <v>159</v>
+      </c>
+      <c r="G30" t="s">
+        <v>185</v>
+      </c>
+      <c r="H30" t="s">
+        <v>118</v>
+      </c>
+      <c r="I30" t="s">
+        <v>81</v>
+      </c>
+      <c r="J30" t="s">
+        <v>153</v>
+      </c>
+      <c r="K30">
+        <v>1.18</v>
+      </c>
+      <c r="R30">
+        <v>1.22</v>
+      </c>
+      <c r="W30">
+        <v>1.47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" t="s">
+        <v>164</v>
+      </c>
+      <c r="D31">
+        <v>2008</v>
+      </c>
+      <c r="E31" t="s">
+        <v>173</v>
+      </c>
+      <c r="F31" t="s">
+        <v>174</v>
+      </c>
+      <c r="G31" t="s">
+        <v>185</v>
+      </c>
+      <c r="H31" t="s">
+        <v>118</v>
+      </c>
+      <c r="I31" t="s">
+        <v>81</v>
+      </c>
+      <c r="J31" t="s">
+        <v>153</v>
+      </c>
+      <c r="K31">
+        <v>1.18</v>
+      </c>
+      <c r="P31">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" t="s">
+        <v>165</v>
+      </c>
+      <c r="D32">
+        <v>2016</v>
+      </c>
+      <c r="E32" t="s">
+        <v>29</v>
+      </c>
+      <c r="F32" t="s">
+        <v>159</v>
+      </c>
+      <c r="G32" t="s">
+        <v>185</v>
+      </c>
+      <c r="H32" t="s">
+        <v>118</v>
+      </c>
+      <c r="I32" t="s">
+        <v>166</v>
+      </c>
+      <c r="J32" t="s">
+        <v>167</v>
+      </c>
+      <c r="K32">
+        <v>1.25</v>
+      </c>
+      <c r="P32">
+        <v>1.24</v>
+      </c>
+      <c r="U32">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="AE32">
+        <v>1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" t="s">
+        <v>168</v>
+      </c>
+      <c r="D33">
+        <v>2017</v>
+      </c>
+      <c r="E33" t="s">
+        <v>29</v>
+      </c>
+      <c r="F33" t="s">
+        <v>159</v>
+      </c>
+      <c r="G33" t="s">
+        <v>185</v>
+      </c>
+      <c r="H33" t="s">
+        <v>118</v>
+      </c>
+      <c r="I33" t="s">
+        <v>166</v>
+      </c>
+      <c r="J33" t="s">
+        <v>167</v>
+      </c>
+      <c r="K33">
+        <v>1.25</v>
+      </c>
+      <c r="P33">
         <v>0.98</v>
       </c>
-    </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>1</v>
-      </c>
-      <c r="B28" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28" t="s">
-        <v>161</v>
-      </c>
-      <c r="D28" t="s">
-        <v>159</v>
-      </c>
-      <c r="E28" t="s">
-        <v>160</v>
-      </c>
-      <c r="F28" t="s">
-        <v>186</v>
-      </c>
-      <c r="G28" t="s">
-        <v>118</v>
-      </c>
-      <c r="H28" t="s">
-        <v>81</v>
-      </c>
-      <c r="I28" t="s">
-        <v>154</v>
-      </c>
-      <c r="J28">
-        <v>1.2</v>
-      </c>
-      <c r="O28">
-        <v>1</v>
-      </c>
-      <c r="T28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>1</v>
-      </c>
-      <c r="B29" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" t="s">
-        <v>162</v>
-      </c>
-      <c r="D29" t="s">
-        <v>163</v>
-      </c>
-      <c r="E29" t="s">
-        <v>160</v>
-      </c>
-      <c r="F29" t="s">
-        <v>186</v>
-      </c>
-      <c r="G29" t="s">
-        <v>118</v>
-      </c>
-      <c r="H29" t="s">
-        <v>81</v>
-      </c>
-      <c r="I29" t="s">
-        <v>154</v>
-      </c>
-      <c r="J29">
-        <v>1.2</v>
-      </c>
-      <c r="O29">
-        <v>1</v>
-      </c>
-      <c r="T29">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" t="s">
-        <v>164</v>
-      </c>
-      <c r="D30" t="s">
-        <v>29</v>
-      </c>
-      <c r="E30" t="s">
-        <v>160</v>
-      </c>
-      <c r="F30" t="s">
-        <v>186</v>
-      </c>
-      <c r="G30" t="s">
-        <v>118</v>
-      </c>
-      <c r="H30" t="s">
-        <v>81</v>
-      </c>
-      <c r="I30" t="s">
-        <v>154</v>
-      </c>
-      <c r="J30">
-        <v>1.18</v>
-      </c>
-      <c r="Q30">
-        <v>1.22</v>
-      </c>
-      <c r="V30">
-        <v>1.47</v>
-      </c>
-    </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>1</v>
-      </c>
-      <c r="B31" t="s">
-        <v>10</v>
-      </c>
-      <c r="C31" t="s">
-        <v>165</v>
-      </c>
-      <c r="D31" t="s">
-        <v>174</v>
-      </c>
-      <c r="E31" t="s">
-        <v>175</v>
-      </c>
-      <c r="F31" t="s">
-        <v>186</v>
-      </c>
-      <c r="G31" t="s">
-        <v>118</v>
-      </c>
-      <c r="H31" t="s">
-        <v>81</v>
-      </c>
-      <c r="I31" t="s">
-        <v>154</v>
-      </c>
-      <c r="J31">
-        <v>1.18</v>
-      </c>
-      <c r="O31">
-        <v>1.22</v>
-      </c>
-    </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>1</v>
-      </c>
-      <c r="B32" t="s">
-        <v>10</v>
-      </c>
-      <c r="C32" t="s">
-        <v>166</v>
-      </c>
-      <c r="D32" t="s">
-        <v>29</v>
-      </c>
-      <c r="E32" t="s">
-        <v>160</v>
-      </c>
-      <c r="F32" t="s">
-        <v>186</v>
-      </c>
-      <c r="G32" t="s">
-        <v>118</v>
-      </c>
-      <c r="H32" t="s">
-        <v>167</v>
-      </c>
-      <c r="I32" t="s">
-        <v>168</v>
-      </c>
-      <c r="J32">
-        <v>1.25</v>
-      </c>
-      <c r="O32">
-        <v>1.24</v>
-      </c>
-      <c r="T32">
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="AD32">
-        <v>1.1399999999999999</v>
-      </c>
-    </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>1</v>
-      </c>
-      <c r="B33" t="s">
-        <v>10</v>
-      </c>
-      <c r="C33" t="s">
-        <v>169</v>
-      </c>
-      <c r="D33" t="s">
-        <v>29</v>
-      </c>
-      <c r="E33" t="s">
-        <v>160</v>
-      </c>
-      <c r="F33" t="s">
-        <v>186</v>
-      </c>
-      <c r="G33" t="s">
-        <v>118</v>
-      </c>
-      <c r="H33" t="s">
-        <v>167</v>
-      </c>
-      <c r="I33" t="s">
-        <v>168</v>
-      </c>
-      <c r="J33">
-        <v>1.25</v>
-      </c>
-      <c r="O33">
-        <v>0.98</v>
-      </c>
-      <c r="AD33">
+      <c r="AE33">
         <v>1.45</v>
       </c>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>1</v>
       </c>
@@ -3478,234 +3662,249 @@
       <c r="C34" t="s">
         <v>125</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34">
+        <v>2012</v>
+      </c>
+      <c r="E34" t="s">
         <v>121</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>120</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
+        <v>185</v>
+      </c>
+      <c r="H34" t="s">
+        <v>122</v>
+      </c>
+      <c r="I34" t="s">
+        <v>124</v>
+      </c>
+      <c r="J34" t="s">
+        <v>123</v>
+      </c>
+      <c r="K34">
+        <v>1.47</v>
+      </c>
+      <c r="P34">
+        <v>1.25</v>
+      </c>
+      <c r="U34">
+        <v>1.36</v>
+      </c>
+      <c r="Z34">
+        <v>1.42</v>
+      </c>
+      <c r="AE34">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" t="s">
+        <v>175</v>
+      </c>
+      <c r="D35">
+        <v>2008</v>
+      </c>
+      <c r="E35" t="s">
+        <v>173</v>
+      </c>
+      <c r="F35" t="s">
+        <v>174</v>
+      </c>
+      <c r="G35" t="s">
+        <v>185</v>
+      </c>
+      <c r="H35" t="s">
+        <v>122</v>
+      </c>
+      <c r="I35" t="s">
+        <v>124</v>
+      </c>
+      <c r="J35" t="s">
+        <v>123</v>
+      </c>
+      <c r="K35">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="Q35">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="T35">
+        <v>1.05</v>
+      </c>
+      <c r="W35">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Z35">
+        <v>1.06</v>
+      </c>
+      <c r="AB35">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="AE35">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" t="s">
+        <v>176</v>
+      </c>
+      <c r="D36">
+        <v>2007</v>
+      </c>
+      <c r="E36" t="s">
+        <v>173</v>
+      </c>
+      <c r="F36" t="s">
+        <v>174</v>
+      </c>
+      <c r="G36" t="s">
+        <v>185</v>
+      </c>
+      <c r="H36" t="s">
+        <v>122</v>
+      </c>
+      <c r="I36" t="s">
+        <v>124</v>
+      </c>
+      <c r="J36" t="s">
+        <v>123</v>
+      </c>
+      <c r="K36">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Q36">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="T36">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="W36">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Z36">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AB36">
+        <v>1.2</v>
+      </c>
+      <c r="AE36">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" t="s">
+        <v>182</v>
+      </c>
+      <c r="D37">
+        <v>2017</v>
+      </c>
+      <c r="E37" t="s">
+        <v>173</v>
+      </c>
+      <c r="F37" t="s">
+        <v>174</v>
+      </c>
+      <c r="G37" t="s">
+        <v>185</v>
+      </c>
+      <c r="H37" t="s">
+        <v>122</v>
+      </c>
+      <c r="I37" t="s">
+        <v>124</v>
+      </c>
+      <c r="J37" t="s">
+        <v>123</v>
+      </c>
+      <c r="K37">
+        <v>1.36</v>
+      </c>
+      <c r="Q37">
+        <v>1.45</v>
+      </c>
+      <c r="V37">
+        <v>1.45</v>
+      </c>
+      <c r="AA37">
+        <v>1.32</v>
+      </c>
+      <c r="AE37">
+        <v>1.86</v>
+      </c>
+    </row>
+    <row r="38" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" t="s">
+        <v>183</v>
+      </c>
+      <c r="D38">
+        <v>2009</v>
+      </c>
+      <c r="E38" t="s">
+        <v>173</v>
+      </c>
+      <c r="F38" t="s">
+        <v>174</v>
+      </c>
+      <c r="G38" t="s">
+        <v>185</v>
+      </c>
+      <c r="H38" t="s">
+        <v>122</v>
+      </c>
+      <c r="I38" t="s">
+        <v>124</v>
+      </c>
+      <c r="J38" t="s">
+        <v>123</v>
+      </c>
+      <c r="K38">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="P38">
+        <v>1.29</v>
+      </c>
+      <c r="U38">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" t="s">
         <v>186</v>
       </c>
-      <c r="G34" t="s">
-        <v>122</v>
-      </c>
-      <c r="H34" t="s">
-        <v>124</v>
-      </c>
-      <c r="I34" t="s">
-        <v>123</v>
-      </c>
-      <c r="J34">
-        <v>1.47</v>
-      </c>
-      <c r="O34">
-        <v>1.25</v>
-      </c>
-      <c r="T34">
-        <v>1.36</v>
-      </c>
-      <c r="Y34">
-        <v>1.42</v>
-      </c>
-      <c r="AD34">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>1</v>
-      </c>
-      <c r="B35" t="s">
-        <v>10</v>
-      </c>
-      <c r="C35" t="s">
-        <v>176</v>
-      </c>
-      <c r="D35" t="s">
-        <v>174</v>
-      </c>
-      <c r="E35" t="s">
-        <v>175</v>
-      </c>
-      <c r="F35" t="s">
-        <v>186</v>
-      </c>
-      <c r="G35" t="s">
-        <v>122</v>
-      </c>
-      <c r="H35" t="s">
-        <v>124</v>
-      </c>
-      <c r="I35" t="s">
-        <v>123</v>
-      </c>
-      <c r="J35">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="P35">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="S35">
-        <v>1.05</v>
-      </c>
-      <c r="V35">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="Y35">
-        <v>1.06</v>
-      </c>
-      <c r="AA35">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="AD35">
-        <v>1.22</v>
-      </c>
-    </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>1</v>
-      </c>
-      <c r="B36" t="s">
-        <v>10</v>
-      </c>
-      <c r="C36" t="s">
-        <v>177</v>
-      </c>
-      <c r="D36" t="s">
-        <v>174</v>
-      </c>
-      <c r="E36" t="s">
-        <v>175</v>
-      </c>
-      <c r="F36" t="s">
-        <v>186</v>
-      </c>
-      <c r="G36" t="s">
-        <v>122</v>
-      </c>
-      <c r="H36" t="s">
-        <v>124</v>
-      </c>
-      <c r="I36" t="s">
-        <v>123</v>
-      </c>
-      <c r="J36">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="P36">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="S36">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="V36">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="Y36">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="AA36">
-        <v>1.2</v>
-      </c>
-      <c r="AD36">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>1</v>
-      </c>
-      <c r="B37" t="s">
-        <v>10</v>
-      </c>
-      <c r="C37" t="s">
-        <v>183</v>
-      </c>
-      <c r="D37" t="s">
-        <v>174</v>
-      </c>
-      <c r="E37" t="s">
-        <v>175</v>
-      </c>
-      <c r="F37" t="s">
-        <v>186</v>
-      </c>
-      <c r="G37" t="s">
-        <v>122</v>
-      </c>
-      <c r="H37" t="s">
-        <v>124</v>
-      </c>
-      <c r="I37" t="s">
-        <v>123</v>
-      </c>
-      <c r="J37">
-        <v>1.36</v>
-      </c>
-      <c r="P37">
-        <v>1.45</v>
-      </c>
-      <c r="U37">
-        <v>1.45</v>
-      </c>
-      <c r="Z37">
-        <v>1.32</v>
-      </c>
-      <c r="AD37">
-        <v>1.86</v>
-      </c>
-    </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>1</v>
-      </c>
-      <c r="B38" t="s">
-        <v>10</v>
-      </c>
-      <c r="C38" t="s">
-        <v>184</v>
-      </c>
-      <c r="D38" t="s">
-        <v>174</v>
-      </c>
-      <c r="E38" t="s">
-        <v>175</v>
-      </c>
-      <c r="F38" t="s">
-        <v>186</v>
-      </c>
-      <c r="G38" t="s">
-        <v>122</v>
-      </c>
-      <c r="H38" t="s">
-        <v>124</v>
-      </c>
-      <c r="I38" t="s">
-        <v>123</v>
-      </c>
-      <c r="J38">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="O38">
-        <v>1.29</v>
-      </c>
-      <c r="T38">
-        <v>1.45</v>
-      </c>
-    </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>1</v>
-      </c>
-      <c r="B39" t="s">
-        <v>187</v>
-      </c>
       <c r="C39" t="s">
-        <v>191</v>
-      </c>
-      <c r="D39" t="s">
         <v>190</v>
+      </c>
+      <c r="D39">
+        <v>2016</v>
       </c>
       <c r="E39" t="s">
         <v>189</v>
@@ -3714,36 +3913,39 @@
         <v>188</v>
       </c>
       <c r="G39" t="s">
-        <v>150</v>
+        <v>187</v>
       </c>
       <c r="H39" t="s">
+        <v>149</v>
+      </c>
+      <c r="I39" t="s">
+        <v>191</v>
+      </c>
+      <c r="J39" t="s">
         <v>192</v>
       </c>
-      <c r="I39" t="s">
-        <v>193</v>
-      </c>
-      <c r="J39">
+      <c r="K39">
         <v>0.93</v>
       </c>
-      <c r="R39">
+      <c r="S39">
         <v>0.93</v>
       </c>
-      <c r="AD39">
+      <c r="AE39">
         <v>0.95</v>
       </c>
     </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C40" t="s">
-        <v>195</v>
-      </c>
-      <c r="D40" t="s">
-        <v>190</v>
+        <v>194</v>
+      </c>
+      <c r="D40">
+        <v>2017</v>
       </c>
       <c r="E40" t="s">
         <v>189</v>
@@ -3752,98 +3954,104 @@
         <v>188</v>
       </c>
       <c r="G40" t="s">
+        <v>187</v>
+      </c>
+      <c r="H40" t="s">
+        <v>149</v>
+      </c>
+      <c r="I40" t="s">
+        <v>191</v>
+      </c>
+      <c r="J40" t="s">
+        <v>192</v>
+      </c>
+      <c r="K40">
+        <v>0.93</v>
+      </c>
+      <c r="S40">
+        <v>0.93</v>
+      </c>
+      <c r="AE40">
+        <v>1.1200000000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" t="s">
+        <v>186</v>
+      </c>
+      <c r="C41" t="s">
+        <v>198</v>
+      </c>
+      <c r="D41">
+        <v>2012</v>
+      </c>
+      <c r="E41" t="s">
+        <v>189</v>
+      </c>
+      <c r="F41" t="s">
+        <v>199</v>
+      </c>
+      <c r="G41" t="s">
+        <v>185</v>
+      </c>
+      <c r="H41" t="s">
+        <v>196</v>
+      </c>
+      <c r="I41" t="s">
+        <v>197</v>
+      </c>
+      <c r="J41" t="s">
+        <v>195</v>
+      </c>
+      <c r="K41">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="N41">
+        <v>2.13</v>
+      </c>
+      <c r="P41">
+        <v>2.21</v>
+      </c>
+      <c r="S41">
+        <v>2.27</v>
+      </c>
+      <c r="U41">
+        <v>2.2200000000000002</v>
+      </c>
+    </row>
+    <row r="42" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" t="s">
         <v>150</v>
       </c>
-      <c r="H40" t="s">
-        <v>192</v>
-      </c>
-      <c r="I40" t="s">
-        <v>193</v>
-      </c>
-      <c r="J40">
-        <v>0.93</v>
-      </c>
-      <c r="R40">
-        <v>0.93</v>
-      </c>
-      <c r="AD40">
-        <v>1.1200000000000001</v>
-      </c>
-    </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>1</v>
-      </c>
-      <c r="B41" t="s">
-        <v>187</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
+        <v>200</v>
+      </c>
+      <c r="D42">
+        <v>2016</v>
+      </c>
+      <c r="E42" t="s">
+        <v>201</v>
+      </c>
+      <c r="F42" t="s">
         <v>199</v>
       </c>
-      <c r="D41" t="s">
-        <v>190</v>
-      </c>
-      <c r="E41" t="s">
-        <v>200</v>
-      </c>
-      <c r="F41" t="s">
-        <v>186</v>
-      </c>
-      <c r="G41" t="s">
-        <v>197</v>
-      </c>
-      <c r="H41" t="s">
-        <v>198</v>
-      </c>
-      <c r="I41" t="s">
-        <v>196</v>
-      </c>
-      <c r="J41">
-        <v>2.2799999999999998</v>
-      </c>
-      <c r="M41">
-        <v>2.13</v>
-      </c>
-      <c r="O41">
-        <v>2.21</v>
-      </c>
-      <c r="R41">
-        <v>2.27</v>
-      </c>
-      <c r="T41">
-        <v>2.2200000000000002</v>
-      </c>
-    </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>1</v>
-      </c>
-      <c r="B42" t="s">
-        <v>151</v>
-      </c>
-      <c r="C42" t="s">
-        <v>201</v>
-      </c>
-      <c r="D42" t="s">
+      <c r="G42" t="s">
+        <v>185</v>
+      </c>
+      <c r="H42" t="s">
+        <v>210</v>
+      </c>
+      <c r="I42" t="s">
         <v>202</v>
       </c>
-      <c r="E42" t="s">
-        <v>200</v>
-      </c>
-      <c r="F42" t="s">
-        <v>186</v>
-      </c>
-      <c r="G42" t="s">
-        <v>212</v>
-      </c>
-      <c r="H42" t="s">
+      <c r="J42" t="s">
         <v>203</v>
-      </c>
-      <c r="I42" t="s">
-        <v>204</v>
-      </c>
-      <c r="J42">
-        <v>0.8</v>
       </c>
       <c r="K42">
         <v>0.8</v>
@@ -3857,433 +4065,917 @@
       <c r="N42">
         <v>0.8</v>
       </c>
-      <c r="AE42" t="s">
+      <c r="O42">
+        <v>0.8</v>
+      </c>
+      <c r="AF42" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="43" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43" t="s">
+        <v>186</v>
+      </c>
+      <c r="C43" t="s">
+        <v>207</v>
+      </c>
+      <c r="D43">
+        <v>2011</v>
+      </c>
+      <c r="E43" t="s">
+        <v>189</v>
+      </c>
+      <c r="F43" t="s">
+        <v>206</v>
+      </c>
+      <c r="G43" t="s">
+        <v>185</v>
+      </c>
+      <c r="H43" t="s">
+        <v>149</v>
+      </c>
+      <c r="I43" t="s">
+        <v>204</v>
+      </c>
+      <c r="J43" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>1</v>
-      </c>
-      <c r="B43" t="s">
-        <v>187</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="K43">
+        <v>1.17</v>
+      </c>
+      <c r="N43">
+        <v>3.86</v>
+      </c>
+    </row>
+    <row r="44" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>1</v>
+      </c>
+      <c r="B44" t="s">
+        <v>186</v>
+      </c>
+      <c r="C44" t="s">
         <v>209</v>
       </c>
-      <c r="D43" t="s">
-        <v>190</v>
-      </c>
-      <c r="E43" t="s">
+      <c r="D44">
+        <v>2011</v>
+      </c>
+      <c r="E44" t="s">
+        <v>189</v>
+      </c>
+      <c r="F44" t="s">
         <v>208</v>
       </c>
-      <c r="F43" t="s">
+      <c r="G44" t="s">
+        <v>185</v>
+      </c>
+      <c r="H44" t="s">
+        <v>149</v>
+      </c>
+      <c r="I44" t="s">
+        <v>204</v>
+      </c>
+      <c r="J44" t="s">
+        <v>205</v>
+      </c>
+      <c r="K44">
+        <v>1.21</v>
+      </c>
+      <c r="N44">
+        <v>1.25</v>
+      </c>
+      <c r="Q44">
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="45" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>1</v>
+      </c>
+      <c r="B45" t="s">
         <v>186</v>
       </c>
-      <c r="G43" t="s">
-        <v>150</v>
-      </c>
-      <c r="H43" t="s">
-        <v>206</v>
-      </c>
-      <c r="I43" t="s">
-        <v>207</v>
-      </c>
-      <c r="J43">
+      <c r="C45" t="s">
+        <v>213</v>
+      </c>
+      <c r="D45">
+        <v>2012</v>
+      </c>
+      <c r="E45" t="s">
+        <v>189</v>
+      </c>
+      <c r="F45" t="s">
+        <v>211</v>
+      </c>
+      <c r="G45" t="s">
+        <v>185</v>
+      </c>
+      <c r="H45" t="s">
+        <v>118</v>
+      </c>
+      <c r="I45" t="s">
+        <v>166</v>
+      </c>
+      <c r="J45" t="s">
+        <v>167</v>
+      </c>
+      <c r="K45">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="N45">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="Q45">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46" t="s">
+        <v>186</v>
+      </c>
+      <c r="C46" t="s">
+        <v>213</v>
+      </c>
+      <c r="D46">
+        <v>2012</v>
+      </c>
+      <c r="E46" t="s">
+        <v>189</v>
+      </c>
+      <c r="F46" t="s">
+        <v>212</v>
+      </c>
+      <c r="G46" t="s">
+        <v>185</v>
+      </c>
+      <c r="H46" t="s">
+        <v>118</v>
+      </c>
+      <c r="I46" t="s">
+        <v>166</v>
+      </c>
+      <c r="J46" t="s">
+        <v>167</v>
+      </c>
+      <c r="K46">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="N46">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="Q46">
         <v>1.17</v>
       </c>
-      <c r="M43">
-        <v>3.86</v>
-      </c>
-    </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>1</v>
-      </c>
-      <c r="B44" t="s">
-        <v>187</v>
-      </c>
-      <c r="C44" t="s">
+    </row>
+    <row r="47" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>1</v>
+      </c>
+      <c r="B47" t="s">
+        <v>186</v>
+      </c>
+      <c r="C47" t="s">
+        <v>213</v>
+      </c>
+      <c r="D47">
+        <v>2012</v>
+      </c>
+      <c r="E47" t="s">
+        <v>189</v>
+      </c>
+      <c r="F47" t="s">
         <v>211</v>
       </c>
-      <c r="D44" t="s">
-        <v>190</v>
-      </c>
-      <c r="E44" t="s">
-        <v>210</v>
-      </c>
-      <c r="F44" t="s">
+      <c r="G47" t="s">
+        <v>185</v>
+      </c>
+      <c r="H47" t="s">
+        <v>127</v>
+      </c>
+      <c r="I47" t="s">
+        <v>135</v>
+      </c>
+      <c r="J47" t="s">
+        <v>136</v>
+      </c>
+      <c r="K47">
+        <v>1.46</v>
+      </c>
+      <c r="N47">
+        <v>1.7</v>
+      </c>
+      <c r="Q47">
+        <v>1.64</v>
+      </c>
+    </row>
+    <row r="48" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>1</v>
+      </c>
+      <c r="B48" t="s">
         <v>186</v>
       </c>
-      <c r="G44" t="s">
-        <v>150</v>
-      </c>
-      <c r="H44" t="s">
-        <v>206</v>
-      </c>
-      <c r="I44" t="s">
-        <v>207</v>
-      </c>
-      <c r="J44">
+      <c r="C48" t="s">
+        <v>213</v>
+      </c>
+      <c r="D48">
+        <v>2012</v>
+      </c>
+      <c r="E48" t="s">
+        <v>189</v>
+      </c>
+      <c r="F48" t="s">
+        <v>212</v>
+      </c>
+      <c r="G48" t="s">
+        <v>185</v>
+      </c>
+      <c r="H48" t="s">
+        <v>127</v>
+      </c>
+      <c r="I48" t="s">
+        <v>135</v>
+      </c>
+      <c r="J48" t="s">
+        <v>136</v>
+      </c>
+      <c r="K48">
+        <v>1.46</v>
+      </c>
+      <c r="N48">
+        <v>1.52</v>
+      </c>
+      <c r="Q48">
+        <v>1.43</v>
+      </c>
+    </row>
+    <row r="49" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>1</v>
+      </c>
+      <c r="B49" t="s">
+        <v>186</v>
+      </c>
+      <c r="C49" t="s">
+        <v>213</v>
+      </c>
+      <c r="D49">
+        <v>2012</v>
+      </c>
+      <c r="E49" t="s">
+        <v>189</v>
+      </c>
+      <c r="F49" t="s">
+        <v>211</v>
+      </c>
+      <c r="G49" t="s">
+        <v>185</v>
+      </c>
+      <c r="H49" t="s">
+        <v>196</v>
+      </c>
+      <c r="I49" t="s">
+        <v>214</v>
+      </c>
+      <c r="J49" t="s">
+        <v>195</v>
+      </c>
+      <c r="K49">
+        <v>1.91</v>
+      </c>
+      <c r="N49">
+        <v>1.6</v>
+      </c>
+      <c r="Q49">
+        <v>1.57</v>
+      </c>
+    </row>
+    <row r="50" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>1</v>
+      </c>
+      <c r="B50" t="s">
+        <v>186</v>
+      </c>
+      <c r="C50" t="s">
+        <v>213</v>
+      </c>
+      <c r="D50">
+        <v>2012</v>
+      </c>
+      <c r="E50" t="s">
+        <v>189</v>
+      </c>
+      <c r="F50" t="s">
+        <v>212</v>
+      </c>
+      <c r="G50" t="s">
+        <v>185</v>
+      </c>
+      <c r="H50" t="s">
+        <v>196</v>
+      </c>
+      <c r="I50" t="s">
+        <v>214</v>
+      </c>
+      <c r="J50" t="s">
+        <v>195</v>
+      </c>
+      <c r="K50">
+        <v>1.91</v>
+      </c>
+      <c r="N50">
+        <v>1.82</v>
+      </c>
+      <c r="Q50">
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="51" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>1</v>
+      </c>
+      <c r="B51" t="s">
+        <v>186</v>
+      </c>
+      <c r="C51" t="s">
+        <v>216</v>
+      </c>
+      <c r="D51">
+        <v>2014</v>
+      </c>
+      <c r="E51" t="s">
+        <v>189</v>
+      </c>
+      <c r="F51" t="s">
+        <v>217</v>
+      </c>
+      <c r="G51" t="s">
+        <v>218</v>
+      </c>
+      <c r="H51" t="s">
+        <v>149</v>
+      </c>
+      <c r="I51" t="s">
+        <v>116</v>
+      </c>
+      <c r="J51" t="s">
+        <v>77</v>
+      </c>
+      <c r="K51">
+        <v>1.92</v>
+      </c>
+      <c r="N51">
+        <v>2.11</v>
+      </c>
+      <c r="P51">
+        <v>1.7</v>
+      </c>
+      <c r="Q51">
+        <v>1.86</v>
+      </c>
+      <c r="T51">
+        <v>1.91</v>
+      </c>
+    </row>
+    <row r="52" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>1</v>
+      </c>
+      <c r="B52" t="s">
+        <v>186</v>
+      </c>
+      <c r="C52" t="s">
+        <v>219</v>
+      </c>
+      <c r="D52">
+        <v>2015</v>
+      </c>
+      <c r="E52" t="s">
+        <v>189</v>
+      </c>
+      <c r="F52" t="s">
+        <v>217</v>
+      </c>
+      <c r="G52" t="s">
+        <v>218</v>
+      </c>
+      <c r="H52" t="s">
+        <v>149</v>
+      </c>
+      <c r="I52" t="s">
+        <v>116</v>
+      </c>
+      <c r="J52" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="53" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B53" t="s">
+        <v>186</v>
+      </c>
+      <c r="C53" t="s">
+        <v>223</v>
+      </c>
+      <c r="D53">
+        <v>2013</v>
+      </c>
+      <c r="E53" t="s">
+        <v>189</v>
+      </c>
+      <c r="F53" t="s">
+        <v>222</v>
+      </c>
+      <c r="G53" t="s">
+        <v>218</v>
+      </c>
+      <c r="H53" t="s">
+        <v>172</v>
+      </c>
+      <c r="I53" t="s">
+        <v>220</v>
+      </c>
+      <c r="J53" t="s">
+        <v>221</v>
+      </c>
+      <c r="K53">
+        <v>2.25</v>
+      </c>
+      <c r="L53">
+        <v>1.98</v>
+      </c>
+      <c r="M53">
+        <v>2.23</v>
+      </c>
+      <c r="N53">
+        <v>2.27</v>
+      </c>
+    </row>
+    <row r="54" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>1</v>
+      </c>
+      <c r="B54" t="s">
+        <v>186</v>
+      </c>
+      <c r="C54" t="s">
+        <v>226</v>
+      </c>
+      <c r="D54">
+        <v>1983</v>
+      </c>
+      <c r="E54" t="s">
+        <v>189</v>
+      </c>
+      <c r="F54" t="s">
+        <v>227</v>
+      </c>
+      <c r="G54" t="s">
+        <v>218</v>
+      </c>
+      <c r="H54" t="s">
+        <v>122</v>
+      </c>
+      <c r="I54" t="s">
+        <v>124</v>
+      </c>
+      <c r="J54" t="s">
+        <v>123</v>
+      </c>
+      <c r="K54">
+        <v>1.26</v>
+      </c>
+      <c r="N54">
         <v>1.21</v>
       </c>
-      <c r="M44">
+      <c r="Q54">
+        <v>1.42</v>
+      </c>
+      <c r="T54">
+        <v>1.51</v>
+      </c>
+      <c r="W54">
+        <v>2.09</v>
+      </c>
+      <c r="AC54">
+        <v>2.33</v>
+      </c>
+    </row>
+    <row r="55" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>1</v>
+      </c>
+      <c r="B55" t="s">
+        <v>186</v>
+      </c>
+      <c r="C55" t="s">
+        <v>228</v>
+      </c>
+      <c r="D55">
+        <v>2008</v>
+      </c>
+      <c r="E55" t="s">
+        <v>229</v>
+      </c>
+      <c r="F55" t="s">
+        <v>230</v>
+      </c>
+      <c r="G55" t="s">
+        <v>218</v>
+      </c>
+      <c r="H55" t="s">
+        <v>122</v>
+      </c>
+      <c r="I55" t="s">
+        <v>124</v>
+      </c>
+      <c r="J55" t="s">
+        <v>123</v>
+      </c>
+      <c r="K55">
+        <v>2.68</v>
+      </c>
+      <c r="M55">
+        <v>2.56</v>
+      </c>
+      <c r="P55">
+        <v>2.56</v>
+      </c>
+      <c r="T55">
+        <v>2.0299999999999998</v>
+      </c>
+    </row>
+    <row r="56" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B56" t="s">
+        <v>186</v>
+      </c>
+      <c r="C56" t="s">
+        <v>228</v>
+      </c>
+      <c r="D56">
+        <v>2008</v>
+      </c>
+      <c r="E56" t="s">
+        <v>229</v>
+      </c>
+      <c r="F56" t="s">
+        <v>217</v>
+      </c>
+      <c r="G56" t="s">
+        <v>218</v>
+      </c>
+      <c r="H56" t="s">
+        <v>122</v>
+      </c>
+      <c r="I56" t="s">
+        <v>124</v>
+      </c>
+      <c r="J56" t="s">
+        <v>123</v>
+      </c>
+      <c r="K56">
+        <v>2.68</v>
+      </c>
+      <c r="M56">
+        <v>2.59</v>
+      </c>
+      <c r="P56">
+        <v>2.57</v>
+      </c>
+      <c r="T56">
+        <v>1.76</v>
+      </c>
+    </row>
+    <row r="57" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>1</v>
+      </c>
+      <c r="B57" t="s">
+        <v>186</v>
+      </c>
+      <c r="C57" t="s">
+        <v>236</v>
+      </c>
+      <c r="D57">
+        <v>2001</v>
+      </c>
+      <c r="E57" t="s">
+        <v>189</v>
+      </c>
+      <c r="F57" t="s">
+        <v>237</v>
+      </c>
+      <c r="G57" t="s">
+        <v>218</v>
+      </c>
+      <c r="H57" t="s">
+        <v>127</v>
+      </c>
+      <c r="I57" t="s">
+        <v>232</v>
+      </c>
+      <c r="J57" t="s">
+        <v>234</v>
+      </c>
+      <c r="K57">
+        <v>2.14</v>
+      </c>
+      <c r="P57">
+        <v>2.31</v>
+      </c>
+      <c r="U57">
+        <v>2.5</v>
+      </c>
+      <c r="Z57">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="AE57">
+        <v>2.2799999999999998</v>
+      </c>
+    </row>
+    <row r="58" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>1</v>
+      </c>
+      <c r="B58" t="s">
+        <v>186</v>
+      </c>
+      <c r="C58" t="s">
+        <v>238</v>
+      </c>
+      <c r="D58">
+        <v>2002</v>
+      </c>
+      <c r="E58" t="s">
+        <v>189</v>
+      </c>
+      <c r="F58" t="s">
+        <v>237</v>
+      </c>
+      <c r="G58" t="s">
+        <v>218</v>
+      </c>
+      <c r="H58" t="s">
+        <v>127</v>
+      </c>
+      <c r="I58" t="s">
+        <v>233</v>
+      </c>
+      <c r="J58" t="s">
+        <v>130</v>
+      </c>
+      <c r="K58">
+        <v>2.1</v>
+      </c>
+      <c r="P58">
+        <v>2.06</v>
+      </c>
+      <c r="U58">
+        <v>2.12</v>
+      </c>
+      <c r="Z58">
+        <v>2.56</v>
+      </c>
+      <c r="AE58">
+        <v>2.5099999999999998</v>
+      </c>
+    </row>
+    <row r="59" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>1</v>
+      </c>
+      <c r="B59" t="s">
+        <v>186</v>
+      </c>
+      <c r="C59" t="s">
+        <v>241</v>
+      </c>
+      <c r="D59">
+        <v>1998</v>
+      </c>
+      <c r="E59" t="s">
+        <v>189</v>
+      </c>
+      <c r="F59" t="s">
+        <v>240</v>
+      </c>
+      <c r="G59" t="s">
+        <v>218</v>
+      </c>
+      <c r="H59" t="s">
+        <v>122</v>
+      </c>
+      <c r="I59" t="s">
+        <v>124</v>
+      </c>
+      <c r="J59" t="s">
+        <v>242</v>
+      </c>
+      <c r="K59">
+        <v>1.03</v>
+      </c>
+      <c r="O59">
+        <v>1.07</v>
+      </c>
+      <c r="S59">
+        <v>1.28</v>
+      </c>
+      <c r="W59">
+        <v>1.45</v>
+      </c>
+      <c r="AA59">
+        <v>1.91</v>
+      </c>
+      <c r="AE59">
+        <v>1.96</v>
+      </c>
+    </row>
+    <row r="60" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>1</v>
+      </c>
+      <c r="B60" t="s">
+        <v>186</v>
+      </c>
+      <c r="C60" t="s">
+        <v>244</v>
+      </c>
+      <c r="D60">
+        <v>2009</v>
+      </c>
+      <c r="E60" t="s">
+        <v>189</v>
+      </c>
+      <c r="F60" t="s">
+        <v>243</v>
+      </c>
+      <c r="G60" t="s">
+        <v>218</v>
+      </c>
+      <c r="H60" t="s">
+        <v>149</v>
+      </c>
+      <c r="I60" t="s">
+        <v>116</v>
+      </c>
+      <c r="J60" t="s">
+        <v>77</v>
+      </c>
+      <c r="K60" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="61" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>1</v>
+      </c>
+      <c r="B61" t="s">
+        <v>186</v>
+      </c>
+      <c r="C61" t="s">
+        <v>247</v>
+      </c>
+      <c r="D61">
+        <v>2009</v>
+      </c>
+      <c r="E61" t="s">
+        <v>189</v>
+      </c>
+      <c r="F61" t="s">
+        <v>246</v>
+      </c>
+      <c r="G61" t="s">
+        <v>218</v>
+      </c>
+      <c r="H61" t="s">
+        <v>118</v>
+      </c>
+      <c r="I61" t="s">
+        <v>81</v>
+      </c>
+      <c r="J61" t="s">
+        <v>153</v>
+      </c>
+      <c r="K61">
+        <v>0.83</v>
+      </c>
+      <c r="L61">
+        <v>0.82</v>
+      </c>
+      <c r="M61">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="62" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>1</v>
+      </c>
+      <c r="B62" t="s">
+        <v>186</v>
+      </c>
+      <c r="C62" t="s">
+        <v>249</v>
+      </c>
+      <c r="D62">
+        <v>2002</v>
+      </c>
+      <c r="E62" t="s">
+        <v>189</v>
+      </c>
+      <c r="F62" t="s">
+        <v>248</v>
+      </c>
+      <c r="G62" t="s">
+        <v>250</v>
+      </c>
+      <c r="H62" t="s">
+        <v>149</v>
+      </c>
+      <c r="I62" t="s">
+        <v>78</v>
+      </c>
+      <c r="J62" t="s">
+        <v>117</v>
+      </c>
+      <c r="K62">
+        <v>1.35</v>
+      </c>
+      <c r="M62">
+        <v>1.41</v>
+      </c>
+      <c r="O62">
+        <v>1.43</v>
+      </c>
+    </row>
+    <row r="63" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>1</v>
+      </c>
+      <c r="B63" t="s">
+        <v>186</v>
+      </c>
+      <c r="C63" t="s">
+        <v>252</v>
+      </c>
+      <c r="D63">
+        <v>2002</v>
+      </c>
+      <c r="E63" t="s">
+        <v>189</v>
+      </c>
+      <c r="F63" t="s">
+        <v>251</v>
+      </c>
+      <c r="G63" t="s">
+        <v>185</v>
+      </c>
+      <c r="H63" t="s">
+        <v>149</v>
+      </c>
+      <c r="I63" t="s">
+        <v>204</v>
+      </c>
+      <c r="J63" t="s">
+        <v>205</v>
+      </c>
+      <c r="K63">
+        <v>1.21</v>
+      </c>
+      <c r="N63">
         <v>1.25</v>
       </c>
-      <c r="P44">
+      <c r="Q63">
         <v>1.32</v>
       </c>
     </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>1</v>
-      </c>
-      <c r="B45" t="s">
-        <v>187</v>
-      </c>
-      <c r="C45" t="s">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>225</v>
+      </c>
+      <c r="C72" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C75" t="s">
         <v>215</v>
       </c>
-      <c r="D45" t="s">
-        <v>190</v>
-      </c>
-      <c r="E45" t="s">
-        <v>213</v>
-      </c>
-      <c r="F45" t="s">
-        <v>186</v>
-      </c>
-      <c r="G45" t="s">
-        <v>118</v>
-      </c>
-      <c r="H45" t="s">
-        <v>167</v>
-      </c>
-      <c r="I45" t="s">
-        <v>168</v>
-      </c>
-      <c r="J45">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="M45">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="P45">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>1</v>
-      </c>
-      <c r="B46" t="s">
-        <v>187</v>
-      </c>
-      <c r="C46" t="s">
-        <v>216</v>
-      </c>
-      <c r="D46" t="s">
-        <v>190</v>
-      </c>
-      <c r="E46" t="s">
-        <v>214</v>
-      </c>
-      <c r="F46" t="s">
-        <v>186</v>
-      </c>
-      <c r="G46" t="s">
-        <v>118</v>
-      </c>
-      <c r="H46" t="s">
-        <v>167</v>
-      </c>
-      <c r="I46" t="s">
-        <v>168</v>
-      </c>
-      <c r="J46">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="M46">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="P46">
-        <v>1.17</v>
-      </c>
-    </row>
-    <row r="47" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>1</v>
-      </c>
-      <c r="B47" t="s">
-        <v>187</v>
-      </c>
-      <c r="C47" t="s">
-        <v>215</v>
-      </c>
-      <c r="D47" t="s">
-        <v>190</v>
-      </c>
-      <c r="E47" t="s">
-        <v>213</v>
-      </c>
-      <c r="F47" t="s">
-        <v>186</v>
-      </c>
-      <c r="G47" t="s">
-        <v>127</v>
-      </c>
-      <c r="H47" t="s">
-        <v>135</v>
-      </c>
-      <c r="I47" t="s">
-        <v>136</v>
-      </c>
-      <c r="J47">
-        <v>1.46</v>
-      </c>
-      <c r="M47">
-        <v>1.7</v>
-      </c>
-      <c r="P47">
-        <v>1.64</v>
-      </c>
-    </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>1</v>
-      </c>
-      <c r="B48" t="s">
-        <v>187</v>
-      </c>
-      <c r="C48" t="s">
-        <v>216</v>
-      </c>
-      <c r="D48" t="s">
-        <v>190</v>
-      </c>
-      <c r="E48" t="s">
-        <v>214</v>
-      </c>
-      <c r="F48" t="s">
-        <v>186</v>
-      </c>
-      <c r="G48" t="s">
-        <v>127</v>
-      </c>
-      <c r="H48" t="s">
-        <v>135</v>
-      </c>
-      <c r="I48" t="s">
-        <v>136</v>
-      </c>
-      <c r="J48">
-        <v>1.46</v>
-      </c>
-      <c r="M48">
-        <v>1.52</v>
-      </c>
-      <c r="P48">
-        <v>1.43</v>
-      </c>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>1</v>
-      </c>
-      <c r="B49" t="s">
-        <v>187</v>
-      </c>
-      <c r="C49" t="s">
-        <v>215</v>
-      </c>
-      <c r="D49" t="s">
-        <v>190</v>
-      </c>
-      <c r="E49" t="s">
-        <v>213</v>
-      </c>
-      <c r="F49" t="s">
-        <v>186</v>
-      </c>
-      <c r="G49" t="s">
-        <v>197</v>
-      </c>
-      <c r="H49" t="s">
-        <v>217</v>
-      </c>
-      <c r="I49" t="s">
-        <v>196</v>
-      </c>
-      <c r="J49">
-        <v>1.91</v>
-      </c>
-      <c r="M49">
-        <v>1.6</v>
-      </c>
-      <c r="P49">
-        <v>1.57</v>
-      </c>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>1</v>
-      </c>
-      <c r="B50" t="s">
-        <v>187</v>
-      </c>
-      <c r="C50" t="s">
-        <v>216</v>
-      </c>
-      <c r="D50" t="s">
-        <v>190</v>
-      </c>
-      <c r="E50" t="s">
-        <v>214</v>
-      </c>
-      <c r="F50" t="s">
-        <v>186</v>
-      </c>
-      <c r="G50" t="s">
-        <v>197</v>
-      </c>
-      <c r="H50" t="s">
-        <v>217</v>
-      </c>
-      <c r="I50" t="s">
-        <v>196</v>
-      </c>
-      <c r="J50">
-        <v>1.91</v>
-      </c>
-      <c r="M50">
-        <v>1.82</v>
-      </c>
-      <c r="P50">
-        <v>1.81</v>
-      </c>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>1</v>
-      </c>
-      <c r="B51" t="s">
-        <v>187</v>
-      </c>
-      <c r="C51" t="s">
-        <v>219</v>
-      </c>
-      <c r="D51" t="s">
-        <v>190</v>
-      </c>
-      <c r="E51" t="s">
-        <v>220</v>
-      </c>
-      <c r="F51" t="s">
-        <v>221</v>
-      </c>
-      <c r="G51" t="s">
-        <v>150</v>
-      </c>
-      <c r="H51" t="s">
-        <v>116</v>
-      </c>
-      <c r="I51" t="s">
-        <v>77</v>
-      </c>
-      <c r="J51">
-        <v>1.92</v>
-      </c>
-      <c r="M51">
-        <v>2.11</v>
-      </c>
-      <c r="O51">
-        <v>1.7</v>
-      </c>
-      <c r="P51">
-        <v>1.86</v>
-      </c>
-      <c r="S51">
-        <v>1.91</v>
-      </c>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>1</v>
-      </c>
-      <c r="B52" t="s">
-        <v>187</v>
-      </c>
-      <c r="C52" t="s">
-        <v>222</v>
-      </c>
-      <c r="D52" t="s">
-        <v>190</v>
-      </c>
-      <c r="E52" t="s">
-        <v>220</v>
-      </c>
-      <c r="F52" t="s">
-        <v>221</v>
-      </c>
-      <c r="G52" t="s">
-        <v>150</v>
-      </c>
-      <c r="H52" t="s">
-        <v>116</v>
-      </c>
-      <c r="I52" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>1</v>
-      </c>
-      <c r="B53" t="s">
-        <v>187</v>
-      </c>
-      <c r="C53" t="s">
-        <v>226</v>
-      </c>
-      <c r="D53" t="s">
-        <v>190</v>
-      </c>
-      <c r="E53" t="s">
-        <v>225</v>
-      </c>
-      <c r="F53" t="s">
-        <v>221</v>
-      </c>
-      <c r="G53" t="s">
-        <v>173</v>
-      </c>
-      <c r="H53" t="s">
-        <v>223</v>
-      </c>
-      <c r="I53" t="s">
-        <v>224</v>
-      </c>
-      <c r="J53">
-        <v>2.25</v>
-      </c>
-      <c r="K53">
-        <v>1.98</v>
-      </c>
-      <c r="L53">
-        <v>2.23</v>
-      </c>
-      <c r="M53">
-        <v>2.27</v>
-      </c>
-    </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="C60" t="s">
-        <v>218</v>
-      </c>
     </row>
   </sheetData>
-  <sortState ref="A2:AD37">
-    <sortCondition ref="G2:G37"/>
+  <sortState ref="A2:AF69">
+    <sortCondition ref="H2:H37"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Small changes to word doc and link add to excel
</commit_message>
<xml_diff>
--- a/alternativefeeddata.xlsx
+++ b/alternativefeeddata.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="255">
   <si>
     <t xml:space="preserve">Taxon </t>
   </si>
@@ -673,9 +673,6 @@
     <t>Whiteleg shrimp</t>
   </si>
   <si>
-    <t>Start on salze 2010</t>
-  </si>
-  <si>
     <t>Vizcaino et al 2014</t>
   </si>
   <si>
@@ -788,6 +785,12 @@
   </si>
   <si>
     <t xml:space="preserve">%of algae as protein source </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saee de cruz 2018 </t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0044848617313704?via%3Dihub</t>
   </si>
 </sst>
 </file>
@@ -1120,7 +1123,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A44" sqref="A44"/>
+      <selection pane="bottomRight" activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2167,13 +2170,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF75"/>
+  <dimension ref="A1:AF73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="10" ySplit="1" topLeftCell="K37" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="1" topLeftCell="K51" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomRight" activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2206,7 +2209,7 @@
         <v>114</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>87</v>
@@ -2451,7 +2454,7 @@
         <v>127</v>
       </c>
       <c r="I5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J5" t="s">
         <v>140</v>
@@ -2489,7 +2492,7 @@
         <v>127</v>
       </c>
       <c r="I6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J6" t="s">
         <v>140</v>
@@ -2679,7 +2682,7 @@
         <v>76</v>
       </c>
       <c r="J10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K10">
         <v>3.8</v>
@@ -4069,7 +4072,7 @@
         <v>0.8</v>
       </c>
       <c r="AF42" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="43" spans="1:32" x14ac:dyDescent="0.35">
@@ -4405,7 +4408,7 @@
         <v>186</v>
       </c>
       <c r="C51" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D51">
         <v>2014</v>
@@ -4414,10 +4417,10 @@
         <v>189</v>
       </c>
       <c r="F51" t="s">
+        <v>216</v>
+      </c>
+      <c r="G51" t="s">
         <v>217</v>
-      </c>
-      <c r="G51" t="s">
-        <v>218</v>
       </c>
       <c r="H51" t="s">
         <v>149</v>
@@ -4452,7 +4455,7 @@
         <v>186</v>
       </c>
       <c r="C52" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D52">
         <v>2015</v>
@@ -4461,10 +4464,10 @@
         <v>189</v>
       </c>
       <c r="F52" t="s">
+        <v>216</v>
+      </c>
+      <c r="G52" t="s">
         <v>217</v>
-      </c>
-      <c r="G52" t="s">
-        <v>218</v>
       </c>
       <c r="H52" t="s">
         <v>149</v>
@@ -4481,10 +4484,10 @@
         <v>1</v>
       </c>
       <c r="B53" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="C53" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D53">
         <v>2013</v>
@@ -4493,19 +4496,19 @@
         <v>189</v>
       </c>
       <c r="F53" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G53" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H53" t="s">
         <v>172</v>
       </c>
       <c r="I53" t="s">
+        <v>219</v>
+      </c>
+      <c r="J53" t="s">
         <v>220</v>
-      </c>
-      <c r="J53" t="s">
-        <v>221</v>
       </c>
       <c r="K53">
         <v>2.25</v>
@@ -4528,7 +4531,7 @@
         <v>186</v>
       </c>
       <c r="C54" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D54">
         <v>1983</v>
@@ -4537,10 +4540,10 @@
         <v>189</v>
       </c>
       <c r="F54" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G54" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H54" t="s">
         <v>122</v>
@@ -4578,19 +4581,19 @@
         <v>186</v>
       </c>
       <c r="C55" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D55">
         <v>2008</v>
       </c>
       <c r="E55" t="s">
+        <v>228</v>
+      </c>
+      <c r="F55" t="s">
         <v>229</v>
       </c>
-      <c r="F55" t="s">
-        <v>230</v>
-      </c>
       <c r="G55" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H55" t="s">
         <v>122</v>
@@ -4622,19 +4625,19 @@
         <v>186</v>
       </c>
       <c r="C56" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D56">
         <v>2008</v>
       </c>
       <c r="E56" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F56" t="s">
+        <v>216</v>
+      </c>
+      <c r="G56" t="s">
         <v>217</v>
-      </c>
-      <c r="G56" t="s">
-        <v>218</v>
       </c>
       <c r="H56" t="s">
         <v>122</v>
@@ -4663,10 +4666,10 @@
         <v>1</v>
       </c>
       <c r="B57" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="C57" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D57">
         <v>2001</v>
@@ -4675,19 +4678,19 @@
         <v>189</v>
       </c>
       <c r="F57" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G57" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H57" t="s">
         <v>127</v>
       </c>
       <c r="I57" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J57" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K57">
         <v>2.14</v>
@@ -4710,10 +4713,10 @@
         <v>1</v>
       </c>
       <c r="B58" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="C58" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D58">
         <v>2002</v>
@@ -4722,16 +4725,16 @@
         <v>189</v>
       </c>
       <c r="F58" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G58" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H58" t="s">
         <v>127</v>
       </c>
       <c r="I58" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="J58" t="s">
         <v>130</v>
@@ -4757,10 +4760,10 @@
         <v>1</v>
       </c>
       <c r="B59" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="C59" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D59">
         <v>1998</v>
@@ -4769,10 +4772,10 @@
         <v>189</v>
       </c>
       <c r="F59" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G59" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H59" t="s">
         <v>122</v>
@@ -4781,7 +4784,7 @@
         <v>124</v>
       </c>
       <c r="J59" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K59">
         <v>1.03</v>
@@ -4810,7 +4813,7 @@
         <v>186</v>
       </c>
       <c r="C60" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D60">
         <v>2009</v>
@@ -4819,10 +4822,10 @@
         <v>189</v>
       </c>
       <c r="F60" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G60" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H60" t="s">
         <v>149</v>
@@ -4834,7 +4837,7 @@
         <v>77</v>
       </c>
       <c r="K60" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="61" spans="1:31" x14ac:dyDescent="0.35">
@@ -4845,7 +4848,7 @@
         <v>186</v>
       </c>
       <c r="C61" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D61">
         <v>2009</v>
@@ -4854,10 +4857,10 @@
         <v>189</v>
       </c>
       <c r="F61" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G61" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H61" t="s">
         <v>118</v>
@@ -4886,7 +4889,7 @@
         <v>186</v>
       </c>
       <c r="C62" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D62">
         <v>2002</v>
@@ -4895,10 +4898,10 @@
         <v>189</v>
       </c>
       <c r="F62" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G62" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H62" t="s">
         <v>149</v>
@@ -4927,7 +4930,7 @@
         <v>186</v>
       </c>
       <c r="C63" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D63">
         <v>2002</v>
@@ -4936,7 +4939,7 @@
         <v>189</v>
       </c>
       <c r="F63" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G63" t="s">
         <v>185</v>
@@ -4962,15 +4965,18 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C72" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C75" t="s">
-        <v>215</v>
+        <v>223</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>253</v>
+      </c>
+      <c r="C73" t="s">
+        <v>254</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Small mods to both word and excel
</commit_message>
<xml_diff>
--- a/alternativefeeddata.xlsx
+++ b/alternativefeeddata.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="254">
   <si>
     <t xml:space="preserve">Taxon </t>
   </si>
@@ -680,9 +680,6 @@
   </si>
   <si>
     <t xml:space="preserve">Fishmeal </t>
-  </si>
-  <si>
-    <t>Vizcaino et al 2015</t>
   </si>
   <si>
     <t>Parrot fish</t>
@@ -1120,7 +1117,7 @@
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="C41" sqref="C41"/>
@@ -2173,10 +2170,10 @@
   <dimension ref="A1:AF73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="10" ySplit="1" topLeftCell="K51" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E77" sqref="E77"/>
+      <selection pane="bottomRight" activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2209,7 +2206,7 @@
         <v>114</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>87</v>
@@ -2298,19 +2295,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>150</v>
+        <v>186</v>
       </c>
       <c r="C2" t="s">
-        <v>131</v>
+        <v>213</v>
       </c>
       <c r="D2">
-        <v>1994</v>
+        <v>2012</v>
       </c>
       <c r="E2" t="s">
-        <v>126</v>
+        <v>189</v>
       </c>
       <c r="F2" t="s">
-        <v>129</v>
+        <v>211</v>
       </c>
       <c r="G2" t="s">
         <v>185</v>
@@ -2319,25 +2316,19 @@
         <v>127</v>
       </c>
       <c r="I2" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="J2" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="K2">
-        <v>2.0499999999999998</v>
-      </c>
-      <c r="R2">
-        <v>1.96</v>
-      </c>
-      <c r="W2">
-        <v>1.92</v>
-      </c>
-      <c r="AA2">
-        <v>2</v>
-      </c>
-      <c r="AE2">
-        <v>2.0699999999999998</v>
+        <v>1.46</v>
+      </c>
+      <c r="N2">
+        <v>1.7</v>
+      </c>
+      <c r="Q2">
+        <v>1.64</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.35">
@@ -2345,19 +2336,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>186</v>
       </c>
       <c r="C3" t="s">
-        <v>133</v>
+        <v>213</v>
       </c>
       <c r="D3">
-        <v>1990</v>
+        <v>2012</v>
       </c>
       <c r="E3" t="s">
-        <v>134</v>
+        <v>189</v>
       </c>
       <c r="F3" t="s">
-        <v>129</v>
+        <v>212</v>
       </c>
       <c r="G3" t="s">
         <v>185</v>
@@ -2372,13 +2363,13 @@
         <v>136</v>
       </c>
       <c r="K3">
-        <v>3.31</v>
-      </c>
-      <c r="U3">
-        <v>3.19</v>
-      </c>
-      <c r="AE3">
-        <v>3.38</v>
+        <v>1.46</v>
+      </c>
+      <c r="N3">
+        <v>1.52</v>
+      </c>
+      <c r="Q3">
+        <v>1.43</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.35">
@@ -2386,46 +2377,40 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>186</v>
       </c>
       <c r="C4" t="s">
-        <v>138</v>
+        <v>190</v>
       </c>
       <c r="D4">
-        <v>2013</v>
+        <v>2016</v>
       </c>
       <c r="E4" t="s">
-        <v>134</v>
+        <v>189</v>
       </c>
       <c r="F4" t="s">
-        <v>129</v>
+        <v>188</v>
       </c>
       <c r="G4" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="H4" t="s">
-        <v>127</v>
+        <v>149</v>
       </c>
       <c r="I4" t="s">
-        <v>137</v>
+        <v>191</v>
       </c>
       <c r="J4" t="s">
-        <v>136</v>
+        <v>192</v>
       </c>
       <c r="K4">
-        <v>1.41</v>
-      </c>
-      <c r="U4">
-        <v>1.36</v>
-      </c>
-      <c r="W4">
-        <v>1.35</v>
-      </c>
-      <c r="Y4">
-        <v>1.44</v>
-      </c>
-      <c r="AA4">
-        <v>1.46</v>
+        <v>0.93</v>
+      </c>
+      <c r="S4">
+        <v>0.93</v>
+      </c>
+      <c r="AE4">
+        <v>0.95</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.35">
@@ -2433,37 +2418,40 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>186</v>
       </c>
       <c r="C5" t="s">
-        <v>139</v>
+        <v>194</v>
       </c>
       <c r="D5">
-        <v>2003</v>
+        <v>2017</v>
       </c>
       <c r="E5" t="s">
-        <v>141</v>
+        <v>189</v>
       </c>
       <c r="F5" t="s">
-        <v>129</v>
+        <v>188</v>
       </c>
       <c r="G5" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="H5" t="s">
-        <v>127</v>
+        <v>149</v>
       </c>
       <c r="I5" t="s">
-        <v>234</v>
+        <v>191</v>
       </c>
       <c r="J5" t="s">
-        <v>140</v>
+        <v>192</v>
       </c>
       <c r="K5">
-        <v>3.16</v>
+        <v>0.93</v>
+      </c>
+      <c r="S5">
+        <v>0.93</v>
       </c>
       <c r="AE5">
-        <v>2.1</v>
+        <v>1.1200000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.35">
@@ -2471,37 +2459,37 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>186</v>
       </c>
       <c r="C6" t="s">
-        <v>142</v>
+        <v>207</v>
       </c>
       <c r="D6">
-        <v>2004</v>
+        <v>2011</v>
       </c>
       <c r="E6" t="s">
-        <v>143</v>
+        <v>189</v>
       </c>
       <c r="F6" t="s">
-        <v>129</v>
+        <v>206</v>
       </c>
       <c r="G6" t="s">
         <v>185</v>
       </c>
       <c r="H6" t="s">
-        <v>127</v>
+        <v>149</v>
       </c>
       <c r="I6" t="s">
-        <v>234</v>
+        <v>204</v>
       </c>
       <c r="J6" t="s">
-        <v>140</v>
+        <v>205</v>
       </c>
       <c r="K6">
-        <v>3.16</v>
-      </c>
-      <c r="AE6">
-        <v>2.98</v>
+        <v>1.17</v>
+      </c>
+      <c r="N6">
+        <v>3.86</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.35">
@@ -2509,1942 +2497,1948 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>186</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>209</v>
       </c>
       <c r="D7">
-        <v>2001</v>
+        <v>2011</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>189</v>
       </c>
       <c r="F7" t="s">
-        <v>4</v>
+        <v>208</v>
       </c>
       <c r="G7" t="s">
         <v>185</v>
       </c>
       <c r="H7" t="s">
+        <v>149</v>
+      </c>
+      <c r="I7" t="s">
+        <v>204</v>
+      </c>
+      <c r="J7" t="s">
+        <v>205</v>
+      </c>
+      <c r="K7">
+        <v>1.21</v>
+      </c>
+      <c r="N7">
+        <v>1.25</v>
+      </c>
+      <c r="Q7">
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>186</v>
+      </c>
+      <c r="C8" t="s">
+        <v>215</v>
+      </c>
+      <c r="D8">
+        <v>2014</v>
+      </c>
+      <c r="E8" t="s">
+        <v>189</v>
+      </c>
+      <c r="F8" t="s">
+        <v>216</v>
+      </c>
+      <c r="G8" t="s">
+        <v>217</v>
+      </c>
+      <c r="H8" t="s">
+        <v>149</v>
+      </c>
+      <c r="I8" t="s">
+        <v>116</v>
+      </c>
+      <c r="J8" t="s">
+        <v>77</v>
+      </c>
+      <c r="K8">
+        <v>1.92</v>
+      </c>
+      <c r="N8">
+        <v>2.11</v>
+      </c>
+      <c r="P8">
+        <v>1.7</v>
+      </c>
+      <c r="Q8">
+        <v>1.86</v>
+      </c>
+      <c r="T8">
+        <v>1.91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C9" t="s">
+        <v>215</v>
+      </c>
+      <c r="D9">
+        <v>2015</v>
+      </c>
+      <c r="E9" t="s">
+        <v>189</v>
+      </c>
+      <c r="F9" t="s">
+        <v>216</v>
+      </c>
+      <c r="G9" t="s">
+        <v>217</v>
+      </c>
+      <c r="H9" t="s">
+        <v>149</v>
+      </c>
+      <c r="I9" t="s">
+        <v>116</v>
+      </c>
+      <c r="J9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>186</v>
+      </c>
+      <c r="C10" t="s">
+        <v>242</v>
+      </c>
+      <c r="D10">
+        <v>2009</v>
+      </c>
+      <c r="E10" t="s">
+        <v>189</v>
+      </c>
+      <c r="F10" t="s">
+        <v>241</v>
+      </c>
+      <c r="G10" t="s">
+        <v>217</v>
+      </c>
+      <c r="H10" t="s">
+        <v>149</v>
+      </c>
+      <c r="I10" t="s">
+        <v>116</v>
+      </c>
+      <c r="J10" t="s">
+        <v>77</v>
+      </c>
+      <c r="K10" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>186</v>
+      </c>
+      <c r="C11" t="s">
+        <v>247</v>
+      </c>
+      <c r="D11">
+        <v>2002</v>
+      </c>
+      <c r="E11" t="s">
+        <v>189</v>
+      </c>
+      <c r="F11" t="s">
+        <v>246</v>
+      </c>
+      <c r="G11" t="s">
+        <v>248</v>
+      </c>
+      <c r="H11" t="s">
+        <v>149</v>
+      </c>
+      <c r="I11" t="s">
+        <v>78</v>
+      </c>
+      <c r="J11" t="s">
+        <v>117</v>
+      </c>
+      <c r="K11">
+        <v>1.35</v>
+      </c>
+      <c r="M11">
+        <v>1.41</v>
+      </c>
+      <c r="O11">
+        <v>1.43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>186</v>
+      </c>
+      <c r="C12" t="s">
+        <v>250</v>
+      </c>
+      <c r="D12">
+        <v>2002</v>
+      </c>
+      <c r="E12" t="s">
+        <v>189</v>
+      </c>
+      <c r="F12" t="s">
+        <v>249</v>
+      </c>
+      <c r="G12" t="s">
+        <v>185</v>
+      </c>
+      <c r="H12" t="s">
+        <v>149</v>
+      </c>
+      <c r="I12" t="s">
+        <v>204</v>
+      </c>
+      <c r="J12" t="s">
+        <v>205</v>
+      </c>
+      <c r="K12">
+        <v>1.21</v>
+      </c>
+      <c r="N12">
+        <v>1.25</v>
+      </c>
+      <c r="Q12">
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>186</v>
+      </c>
+      <c r="C13" t="s">
+        <v>213</v>
+      </c>
+      <c r="D13">
+        <v>2012</v>
+      </c>
+      <c r="E13" t="s">
+        <v>189</v>
+      </c>
+      <c r="F13" t="s">
+        <v>211</v>
+      </c>
+      <c r="G13" t="s">
+        <v>185</v>
+      </c>
+      <c r="H13" t="s">
+        <v>118</v>
+      </c>
+      <c r="I13" t="s">
+        <v>166</v>
+      </c>
+      <c r="J13" t="s">
+        <v>167</v>
+      </c>
+      <c r="K13">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="N13">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="Q13">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>186</v>
+      </c>
+      <c r="C14" t="s">
+        <v>213</v>
+      </c>
+      <c r="D14">
+        <v>2012</v>
+      </c>
+      <c r="E14" t="s">
+        <v>189</v>
+      </c>
+      <c r="F14" t="s">
+        <v>212</v>
+      </c>
+      <c r="G14" t="s">
+        <v>185</v>
+      </c>
+      <c r="H14" t="s">
+        <v>118</v>
+      </c>
+      <c r="I14" t="s">
+        <v>166</v>
+      </c>
+      <c r="J14" t="s">
+        <v>167</v>
+      </c>
+      <c r="K14">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="N14">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="Q14">
+        <v>1.17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>186</v>
+      </c>
+      <c r="C15" t="s">
+        <v>245</v>
+      </c>
+      <c r="D15">
+        <v>2009</v>
+      </c>
+      <c r="E15" t="s">
+        <v>189</v>
+      </c>
+      <c r="F15" t="s">
+        <v>244</v>
+      </c>
+      <c r="G15" t="s">
+        <v>217</v>
+      </c>
+      <c r="H15" t="s">
+        <v>118</v>
+      </c>
+      <c r="I15" t="s">
+        <v>81</v>
+      </c>
+      <c r="J15" t="s">
+        <v>153</v>
+      </c>
+      <c r="K15">
+        <v>0.83</v>
+      </c>
+      <c r="L15">
+        <v>0.82</v>
+      </c>
+      <c r="M15">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>186</v>
+      </c>
+      <c r="C16" t="s">
+        <v>198</v>
+      </c>
+      <c r="D16">
+        <v>2012</v>
+      </c>
+      <c r="E16" t="s">
+        <v>189</v>
+      </c>
+      <c r="F16" t="s">
+        <v>199</v>
+      </c>
+      <c r="G16" t="s">
+        <v>185</v>
+      </c>
+      <c r="H16" t="s">
+        <v>196</v>
+      </c>
+      <c r="I16" t="s">
+        <v>197</v>
+      </c>
+      <c r="J16" t="s">
+        <v>195</v>
+      </c>
+      <c r="K16">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="N16">
+        <v>2.13</v>
+      </c>
+      <c r="P16">
+        <v>2.21</v>
+      </c>
+      <c r="S16">
+        <v>2.27</v>
+      </c>
+      <c r="U16">
+        <v>2.2200000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>186</v>
+      </c>
+      <c r="C17" t="s">
+        <v>213</v>
+      </c>
+      <c r="D17">
+        <v>2012</v>
+      </c>
+      <c r="E17" t="s">
+        <v>189</v>
+      </c>
+      <c r="F17" t="s">
+        <v>211</v>
+      </c>
+      <c r="G17" t="s">
+        <v>185</v>
+      </c>
+      <c r="H17" t="s">
+        <v>196</v>
+      </c>
+      <c r="I17" t="s">
+        <v>214</v>
+      </c>
+      <c r="J17" t="s">
+        <v>195</v>
+      </c>
+      <c r="K17">
+        <v>1.91</v>
+      </c>
+      <c r="N17">
+        <v>1.6</v>
+      </c>
+      <c r="Q17">
+        <v>1.57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>186</v>
+      </c>
+      <c r="C18" t="s">
+        <v>213</v>
+      </c>
+      <c r="D18">
+        <v>2012</v>
+      </c>
+      <c r="E18" t="s">
+        <v>189</v>
+      </c>
+      <c r="F18" t="s">
+        <v>212</v>
+      </c>
+      <c r="G18" t="s">
+        <v>185</v>
+      </c>
+      <c r="H18" t="s">
+        <v>196</v>
+      </c>
+      <c r="I18" t="s">
+        <v>214</v>
+      </c>
+      <c r="J18" t="s">
+        <v>195</v>
+      </c>
+      <c r="K18">
+        <v>1.91</v>
+      </c>
+      <c r="N18">
+        <v>1.82</v>
+      </c>
+      <c r="Q18">
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>186</v>
+      </c>
+      <c r="C19" t="s">
+        <v>224</v>
+      </c>
+      <c r="D19">
+        <v>1983</v>
+      </c>
+      <c r="E19" t="s">
+        <v>189</v>
+      </c>
+      <c r="F19" t="s">
+        <v>225</v>
+      </c>
+      <c r="G19" t="s">
+        <v>217</v>
+      </c>
+      <c r="H19" t="s">
+        <v>122</v>
+      </c>
+      <c r="I19" t="s">
+        <v>124</v>
+      </c>
+      <c r="J19" t="s">
+        <v>123</v>
+      </c>
+      <c r="K19">
+        <v>1.26</v>
+      </c>
+      <c r="N19">
+        <v>1.21</v>
+      </c>
+      <c r="Q19">
+        <v>1.42</v>
+      </c>
+      <c r="T19">
+        <v>1.51</v>
+      </c>
+      <c r="W19">
+        <v>2.09</v>
+      </c>
+      <c r="AC19">
+        <v>2.33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>186</v>
+      </c>
+      <c r="C20" t="s">
+        <v>226</v>
+      </c>
+      <c r="D20">
+        <v>2008</v>
+      </c>
+      <c r="E20" t="s">
+        <v>227</v>
+      </c>
+      <c r="F20" t="s">
+        <v>228</v>
+      </c>
+      <c r="G20" t="s">
+        <v>217</v>
+      </c>
+      <c r="H20" t="s">
+        <v>122</v>
+      </c>
+      <c r="I20" t="s">
+        <v>124</v>
+      </c>
+      <c r="J20" t="s">
+        <v>123</v>
+      </c>
+      <c r="K20">
+        <v>2.68</v>
+      </c>
+      <c r="M20">
+        <v>2.56</v>
+      </c>
+      <c r="P20">
+        <v>2.56</v>
+      </c>
+      <c r="T20">
+        <v>2.0299999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>186</v>
+      </c>
+      <c r="C21" t="s">
+        <v>226</v>
+      </c>
+      <c r="D21">
+        <v>2008</v>
+      </c>
+      <c r="E21" t="s">
+        <v>227</v>
+      </c>
+      <c r="F21" t="s">
+        <v>216</v>
+      </c>
+      <c r="G21" t="s">
+        <v>217</v>
+      </c>
+      <c r="H21" t="s">
+        <v>122</v>
+      </c>
+      <c r="I21" t="s">
+        <v>124</v>
+      </c>
+      <c r="J21" t="s">
+        <v>123</v>
+      </c>
+      <c r="K21">
+        <v>2.68</v>
+      </c>
+      <c r="M21">
+        <v>2.59</v>
+      </c>
+      <c r="P21">
+        <v>2.57</v>
+      </c>
+      <c r="T21">
+        <v>1.76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>193</v>
+      </c>
+      <c r="C22" t="s">
+        <v>234</v>
+      </c>
+      <c r="D22">
+        <v>2001</v>
+      </c>
+      <c r="E22" t="s">
+        <v>189</v>
+      </c>
+      <c r="F22" t="s">
+        <v>235</v>
+      </c>
+      <c r="G22" t="s">
+        <v>217</v>
+      </c>
+      <c r="H22" t="s">
+        <v>127</v>
+      </c>
+      <c r="I22" t="s">
+        <v>230</v>
+      </c>
+      <c r="J22" t="s">
+        <v>232</v>
+      </c>
+      <c r="K22">
+        <v>2.14</v>
+      </c>
+      <c r="P22">
+        <v>2.31</v>
+      </c>
+      <c r="U22">
+        <v>2.5</v>
+      </c>
+      <c r="Z22">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="AE22">
+        <v>2.2799999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>193</v>
+      </c>
+      <c r="C23" t="s">
+        <v>236</v>
+      </c>
+      <c r="D23">
+        <v>2002</v>
+      </c>
+      <c r="E23" t="s">
+        <v>189</v>
+      </c>
+      <c r="F23" t="s">
+        <v>235</v>
+      </c>
+      <c r="G23" t="s">
+        <v>217</v>
+      </c>
+      <c r="H23" t="s">
+        <v>127</v>
+      </c>
+      <c r="I23" t="s">
+        <v>231</v>
+      </c>
+      <c r="J23" t="s">
+        <v>130</v>
+      </c>
+      <c r="K23">
+        <v>2.1</v>
+      </c>
+      <c r="P23">
+        <v>2.06</v>
+      </c>
+      <c r="U23">
+        <v>2.12</v>
+      </c>
+      <c r="Z23">
+        <v>2.56</v>
+      </c>
+      <c r="AE23">
+        <v>2.5099999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>193</v>
+      </c>
+      <c r="C24" t="s">
+        <v>147</v>
+      </c>
+      <c r="D24">
+        <v>2013</v>
+      </c>
+      <c r="E24" t="s">
+        <v>148</v>
+      </c>
+      <c r="G24" t="s">
+        <v>185</v>
+      </c>
+      <c r="H24" t="s">
+        <v>149</v>
+      </c>
+      <c r="I24" t="s">
+        <v>146</v>
+      </c>
+      <c r="J24" t="s">
+        <v>145</v>
+      </c>
+      <c r="K24">
+        <f>1/1.08</f>
+        <v>0.92592592592592582</v>
+      </c>
+      <c r="M24">
+        <f>1/1.14</f>
+        <v>0.87719298245614041</v>
+      </c>
+      <c r="O24">
+        <f>1/1.06</f>
+        <v>0.94339622641509424</v>
+      </c>
+      <c r="S24">
+        <f>1/0.89</f>
+        <v>1.1235955056179776</v>
+      </c>
+    </row>
+    <row r="25" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>193</v>
+      </c>
+      <c r="C25" t="s">
+        <v>221</v>
+      </c>
+      <c r="D25">
+        <v>2013</v>
+      </c>
+      <c r="E25" t="s">
+        <v>189</v>
+      </c>
+      <c r="F25" t="s">
+        <v>220</v>
+      </c>
+      <c r="G25" t="s">
+        <v>217</v>
+      </c>
+      <c r="H25" t="s">
+        <v>172</v>
+      </c>
+      <c r="I25" t="s">
+        <v>218</v>
+      </c>
+      <c r="J25" t="s">
+        <v>219</v>
+      </c>
+      <c r="K25">
+        <v>2.25</v>
+      </c>
+      <c r="L25">
+        <v>1.98</v>
+      </c>
+      <c r="M25">
+        <v>2.23</v>
+      </c>
+      <c r="N25">
+        <v>2.27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>193</v>
+      </c>
+      <c r="C26" t="s">
+        <v>239</v>
+      </c>
+      <c r="D26">
+        <v>1998</v>
+      </c>
+      <c r="E26" t="s">
+        <v>189</v>
+      </c>
+      <c r="F26" t="s">
+        <v>238</v>
+      </c>
+      <c r="G26" t="s">
+        <v>217</v>
+      </c>
+      <c r="H26" t="s">
+        <v>122</v>
+      </c>
+      <c r="I26" t="s">
+        <v>124</v>
+      </c>
+      <c r="J26" t="s">
+        <v>240</v>
+      </c>
+      <c r="K26">
+        <v>1.03</v>
+      </c>
+      <c r="O26">
+        <v>1.07</v>
+      </c>
+      <c r="S26">
+        <v>1.28</v>
+      </c>
+      <c r="W26">
+        <v>1.45</v>
+      </c>
+      <c r="AA26">
+        <v>1.91</v>
+      </c>
+      <c r="AE26">
+        <v>1.96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>150</v>
+      </c>
+      <c r="C27" t="s">
+        <v>131</v>
+      </c>
+      <c r="D27">
+        <v>1994</v>
+      </c>
+      <c r="E27" t="s">
+        <v>126</v>
+      </c>
+      <c r="F27" t="s">
+        <v>129</v>
+      </c>
+      <c r="G27" t="s">
+        <v>185</v>
+      </c>
+      <c r="H27" t="s">
+        <v>127</v>
+      </c>
+      <c r="I27" t="s">
+        <v>128</v>
+      </c>
+      <c r="J27" t="s">
+        <v>130</v>
+      </c>
+      <c r="K27">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="R27">
+        <v>1.96</v>
+      </c>
+      <c r="W27">
+        <v>1.92</v>
+      </c>
+      <c r="AA27">
+        <v>2</v>
+      </c>
+      <c r="AE27">
+        <v>2.0699999999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>150</v>
+      </c>
+      <c r="C28" t="s">
+        <v>181</v>
+      </c>
+      <c r="D28">
+        <v>2010</v>
+      </c>
+      <c r="E28" t="s">
+        <v>180</v>
+      </c>
+      <c r="F28" t="s">
+        <v>174</v>
+      </c>
+      <c r="G28" t="s">
+        <v>185</v>
+      </c>
+      <c r="H28" t="s">
         <v>31</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I28" t="s">
         <v>32</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J28" t="s">
         <v>91</v>
       </c>
-      <c r="K7">
+      <c r="K28">
+        <v>1.34</v>
+      </c>
+      <c r="P28">
+        <v>1.36</v>
+      </c>
+      <c r="U28">
+        <v>1.44</v>
+      </c>
+      <c r="Z28">
+        <v>1.61</v>
+      </c>
+      <c r="AE28">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>150</v>
+      </c>
+      <c r="C29" t="s">
+        <v>147</v>
+      </c>
+      <c r="D29">
+        <v>2013</v>
+      </c>
+      <c r="E29" t="s">
+        <v>154</v>
+      </c>
+      <c r="F29" t="s">
+        <v>129</v>
+      </c>
+      <c r="G29" t="s">
+        <v>185</v>
+      </c>
+      <c r="H29" t="s">
+        <v>149</v>
+      </c>
+      <c r="I29" t="s">
+        <v>146</v>
+      </c>
+      <c r="J29" t="s">
+        <v>145</v>
+      </c>
+      <c r="K29">
+        <f>1/1.08</f>
+        <v>0.92592592592592582</v>
+      </c>
+      <c r="M29">
+        <f>1/1.15</f>
+        <v>0.86956521739130443</v>
+      </c>
+      <c r="O29">
+        <f>1/0.94</f>
+        <v>1.0638297872340425</v>
+      </c>
+    </row>
+    <row r="30" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
+        <v>150</v>
+      </c>
+      <c r="C30" t="s">
+        <v>200</v>
+      </c>
+      <c r="D30">
+        <v>2016</v>
+      </c>
+      <c r="E30" t="s">
+        <v>201</v>
+      </c>
+      <c r="F30" t="s">
+        <v>199</v>
+      </c>
+      <c r="G30" t="s">
+        <v>185</v>
+      </c>
+      <c r="H30" t="s">
+        <v>210</v>
+      </c>
+      <c r="I30" t="s">
+        <v>202</v>
+      </c>
+      <c r="J30" t="s">
+        <v>203</v>
+      </c>
+      <c r="K30">
+        <v>0.8</v>
+      </c>
+      <c r="L30">
+        <v>0.8</v>
+      </c>
+      <c r="M30">
+        <v>0.8</v>
+      </c>
+      <c r="N30">
+        <v>0.8</v>
+      </c>
+      <c r="O30">
+        <v>0.8</v>
+      </c>
+      <c r="AF30" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="31" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" t="s">
+        <v>133</v>
+      </c>
+      <c r="D31">
+        <v>1990</v>
+      </c>
+      <c r="E31" t="s">
+        <v>134</v>
+      </c>
+      <c r="F31" t="s">
+        <v>129</v>
+      </c>
+      <c r="G31" t="s">
+        <v>185</v>
+      </c>
+      <c r="H31" t="s">
+        <v>127</v>
+      </c>
+      <c r="I31" t="s">
+        <v>135</v>
+      </c>
+      <c r="J31" t="s">
+        <v>136</v>
+      </c>
+      <c r="K31">
+        <v>3.31</v>
+      </c>
+      <c r="U31">
+        <v>3.19</v>
+      </c>
+      <c r="AE31">
+        <v>3.38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" t="s">
+        <v>138</v>
+      </c>
+      <c r="D32">
+        <v>2013</v>
+      </c>
+      <c r="E32" t="s">
+        <v>134</v>
+      </c>
+      <c r="F32" t="s">
+        <v>129</v>
+      </c>
+      <c r="G32" t="s">
+        <v>185</v>
+      </c>
+      <c r="H32" t="s">
+        <v>127</v>
+      </c>
+      <c r="I32" t="s">
+        <v>137</v>
+      </c>
+      <c r="J32" t="s">
+        <v>136</v>
+      </c>
+      <c r="K32">
+        <v>1.41</v>
+      </c>
+      <c r="U32">
+        <v>1.36</v>
+      </c>
+      <c r="W32">
+        <v>1.35</v>
+      </c>
+      <c r="Y32">
+        <v>1.44</v>
+      </c>
+      <c r="AA32">
+        <v>1.46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" t="s">
+        <v>139</v>
+      </c>
+      <c r="D33">
+        <v>2003</v>
+      </c>
+      <c r="E33" t="s">
+        <v>141</v>
+      </c>
+      <c r="F33" t="s">
+        <v>129</v>
+      </c>
+      <c r="G33" t="s">
+        <v>185</v>
+      </c>
+      <c r="H33" t="s">
+        <v>127</v>
+      </c>
+      <c r="I33" t="s">
+        <v>233</v>
+      </c>
+      <c r="J33" t="s">
+        <v>140</v>
+      </c>
+      <c r="K33">
+        <v>3.16</v>
+      </c>
+      <c r="AE33">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" t="s">
+        <v>142</v>
+      </c>
+      <c r="D34">
+        <v>2004</v>
+      </c>
+      <c r="E34" t="s">
+        <v>143</v>
+      </c>
+      <c r="F34" t="s">
+        <v>129</v>
+      </c>
+      <c r="G34" t="s">
+        <v>185</v>
+      </c>
+      <c r="H34" t="s">
+        <v>127</v>
+      </c>
+      <c r="I34" t="s">
+        <v>233</v>
+      </c>
+      <c r="J34" t="s">
+        <v>140</v>
+      </c>
+      <c r="K34">
+        <v>3.16</v>
+      </c>
+      <c r="AE34">
+        <v>2.98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35">
+        <v>2001</v>
+      </c>
+      <c r="E35" t="s">
+        <v>17</v>
+      </c>
+      <c r="F35" t="s">
+        <v>4</v>
+      </c>
+      <c r="G35" t="s">
+        <v>185</v>
+      </c>
+      <c r="H35" t="s">
+        <v>31</v>
+      </c>
+      <c r="I35" t="s">
+        <v>32</v>
+      </c>
+      <c r="J35" t="s">
+        <v>91</v>
+      </c>
+      <c r="K35">
         <v>0.76</v>
       </c>
-      <c r="O7">
+      <c r="O35">
         <f>1/1.33</f>
         <v>0.75187969924812026</v>
       </c>
-      <c r="S7">
+      <c r="S35">
         <f>1/1.19</f>
         <v>0.84033613445378152</v>
       </c>
-      <c r="W7">
+      <c r="W35">
         <f>1/1.02</f>
         <v>0.98039215686274506</v>
       </c>
-      <c r="AA7">
+      <c r="AA35">
         <f>1/1.12</f>
         <v>0.89285714285714279</v>
       </c>
-      <c r="AE7">
+      <c r="AE35">
         <f>1/0.89</f>
         <v>1.1235955056179776</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" t="s">
         <v>69</v>
       </c>
-      <c r="D8">
+      <c r="D36">
         <v>2011</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E36" t="s">
         <v>68</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F36" t="s">
         <v>70</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G36" t="s">
         <v>185</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H36" t="s">
         <v>31</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I36" t="s">
         <v>32</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J36" t="s">
         <v>91</v>
       </c>
-      <c r="K8">
+      <c r="K36">
         <v>1.51</v>
       </c>
-      <c r="P8">
+      <c r="P36">
         <v>1.46</v>
       </c>
-      <c r="U8">
+      <c r="U36">
         <v>1.81</v>
       </c>
-      <c r="Z8">
+      <c r="Z36">
         <v>1.72</v>
       </c>
-      <c r="AE8">
+      <c r="AE36">
         <v>1.91</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" t="s">
         <v>74</v>
       </c>
-      <c r="D9">
+      <c r="D37">
         <v>2009</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E37" t="s">
         <v>72</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F37" t="s">
         <v>73</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G37" t="s">
         <v>185</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H37" t="s">
         <v>31</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I37" t="s">
         <v>71</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J37" t="s">
         <v>91</v>
       </c>
-      <c r="K9">
+      <c r="K37">
         <v>2.96</v>
       </c>
-      <c r="P9">
+      <c r="P37">
         <v>3.09</v>
       </c>
-      <c r="U9">
+      <c r="U37">
         <v>2.88</v>
       </c>
-      <c r="Z9">
+      <c r="Z37">
         <v>3.67</v>
       </c>
-      <c r="AE9">
+      <c r="AE37">
         <v>3.44</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" t="s">
         <v>75</v>
       </c>
-      <c r="D10">
+      <c r="D38">
         <v>2015</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E38" t="s">
         <v>17</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F38" t="s">
         <v>4</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G38" t="s">
         <v>185</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H38" t="s">
         <v>31</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I38" t="s">
         <v>76</v>
       </c>
-      <c r="J10" t="s">
-        <v>238</v>
-      </c>
-      <c r="K10">
+      <c r="J38" t="s">
+        <v>237</v>
+      </c>
+      <c r="K38">
         <v>3.8</v>
       </c>
-      <c r="U10">
+      <c r="U38">
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" t="s">
         <v>157</v>
       </c>
-      <c r="D11">
+      <c r="D39">
         <v>2005</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E39" t="s">
         <v>158</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F39" t="s">
         <v>159</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G39" t="s">
         <v>185</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H39" t="s">
         <v>31</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I39" t="s">
         <v>156</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J39" t="s">
         <v>155</v>
       </c>
-      <c r="K11">
+      <c r="K39">
         <f>1/1.48</f>
         <v>0.67567567567567566</v>
       </c>
-      <c r="AE11">
+      <c r="AE39">
         <f>1/1.68</f>
         <v>0.59523809523809523</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" t="s">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" t="s">
         <v>178</v>
       </c>
-      <c r="D12">
+      <c r="D40">
         <v>2009</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E40" t="s">
         <v>173</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F40" t="s">
         <v>174</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G40" t="s">
         <v>185</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H40" t="s">
         <v>31</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I40" t="s">
         <v>32</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J40" t="s">
         <v>91</v>
       </c>
-      <c r="K12">
+      <c r="K40">
         <v>1.1499999999999999</v>
       </c>
-      <c r="U12">
+      <c r="U40">
         <v>1.17</v>
       </c>
-      <c r="AE12">
+      <c r="AE40">
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" t="s">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" t="s">
         <v>179</v>
       </c>
-      <c r="D13">
+      <c r="D41">
         <v>2003</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E41" t="s">
         <v>173</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F41" t="s">
         <v>174</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G41" t="s">
         <v>185</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H41" t="s">
         <v>31</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I41" t="s">
         <v>32</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J41" t="s">
         <v>91</v>
       </c>
-      <c r="K13">
+      <c r="K41">
         <v>2.2599999999999998</v>
       </c>
-      <c r="AE13">
+      <c r="AE41">
         <v>2.58</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" t="s">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" t="s">
         <v>179</v>
       </c>
-      <c r="D14">
+      <c r="D42">
         <v>2003</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E42" t="s">
         <v>173</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F42" t="s">
         <v>174</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G42" t="s">
         <v>185</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H42" t="s">
         <v>31</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I42" t="s">
         <v>32</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J42" t="s">
         <v>91</v>
       </c>
-      <c r="K14">
+      <c r="K42">
         <v>2.2599999999999998</v>
       </c>
-      <c r="AE14">
+      <c r="AE42">
         <v>3.52</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" t="s">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" t="s">
         <v>179</v>
       </c>
-      <c r="D15">
+      <c r="D43">
         <v>2003</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E43" t="s">
         <v>173</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F43" t="s">
         <v>174</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G43" t="s">
         <v>185</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H43" t="s">
         <v>31</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I43" t="s">
         <v>32</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J43" t="s">
         <v>91</v>
       </c>
-      <c r="K15">
+      <c r="K43">
         <v>2.2599999999999998</v>
       </c>
-      <c r="AE15">
+      <c r="AE43">
         <v>2.2400000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" t="s">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>1</v>
+      </c>
+      <c r="B44" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" t="s">
         <v>179</v>
       </c>
-      <c r="D16">
+      <c r="D44">
         <v>2003</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E44" t="s">
         <v>173</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F44" t="s">
         <v>174</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G44" t="s">
         <v>185</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H44" t="s">
         <v>31</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I44" t="s">
         <v>32</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J44" t="s">
         <v>91</v>
       </c>
-      <c r="K16">
+      <c r="K44">
         <v>2.2599999999999998</v>
       </c>
-      <c r="AE16">
+      <c r="AE44">
         <v>2.65</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" t="s">
-        <v>150</v>
-      </c>
-      <c r="C17" t="s">
-        <v>181</v>
-      </c>
-      <c r="D17">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>1</v>
+      </c>
+      <c r="B45" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" t="s">
+        <v>85</v>
+      </c>
+      <c r="D45">
         <v>2010</v>
       </c>
-      <c r="E17" t="s">
-        <v>180</v>
-      </c>
-      <c r="F17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G17" t="s">
+      <c r="E45" t="s">
+        <v>84</v>
+      </c>
+      <c r="F45" t="s">
+        <v>83</v>
+      </c>
+      <c r="G45" t="s">
         <v>185</v>
       </c>
-      <c r="H17" t="s">
-        <v>31</v>
-      </c>
-      <c r="I17" t="s">
-        <v>32</v>
-      </c>
-      <c r="J17" t="s">
+      <c r="H45" t="s">
+        <v>119</v>
+      </c>
+      <c r="I45" t="s">
+        <v>71</v>
+      </c>
+      <c r="J45" t="s">
         <v>91</v>
       </c>
-      <c r="K17">
+      <c r="K45">
+        <v>0.89</v>
+      </c>
+      <c r="P45">
+        <v>0.7</v>
+      </c>
+      <c r="U45">
+        <v>0.99</v>
+      </c>
+      <c r="Z45">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="46" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" t="s">
+        <v>79</v>
+      </c>
+      <c r="D46">
+        <v>2018</v>
+      </c>
+      <c r="E46" t="s">
+        <v>17</v>
+      </c>
+      <c r="F46" t="s">
+        <v>4</v>
+      </c>
+      <c r="G46" t="s">
+        <v>185</v>
+      </c>
+      <c r="H46" t="s">
+        <v>149</v>
+      </c>
+      <c r="I46" t="s">
+        <v>116</v>
+      </c>
+      <c r="J46" t="s">
+        <v>77</v>
+      </c>
+      <c r="K46">
         <v>1.34</v>
       </c>
-      <c r="P17">
-        <v>1.36</v>
-      </c>
-      <c r="U17">
-        <v>1.44</v>
-      </c>
-      <c r="Z17">
-        <v>1.61</v>
-      </c>
-      <c r="AE17">
-        <v>1.67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" t="s">
-        <v>85</v>
-      </c>
-      <c r="D18">
-        <v>2010</v>
-      </c>
-      <c r="E18" t="s">
-        <v>84</v>
-      </c>
-      <c r="F18" t="s">
-        <v>83</v>
-      </c>
-      <c r="G18" t="s">
+      <c r="R46">
+        <v>1.02</v>
+      </c>
+      <c r="Y46">
+        <v>1.28</v>
+      </c>
+    </row>
+    <row r="47" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>1</v>
+      </c>
+      <c r="B47" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" t="s">
+        <v>80</v>
+      </c>
+      <c r="D47">
+        <v>2016</v>
+      </c>
+      <c r="E47" t="s">
+        <v>17</v>
+      </c>
+      <c r="F47" t="s">
+        <v>4</v>
+      </c>
+      <c r="G47" t="s">
         <v>185</v>
       </c>
-      <c r="H18" t="s">
-        <v>119</v>
-      </c>
-      <c r="I18" t="s">
-        <v>71</v>
-      </c>
-      <c r="J18" t="s">
-        <v>91</v>
-      </c>
-      <c r="K18">
-        <v>0.89</v>
-      </c>
-      <c r="P18">
-        <v>0.7</v>
-      </c>
-      <c r="U18">
+      <c r="H47" t="s">
+        <v>149</v>
+      </c>
+      <c r="I47" t="s">
+        <v>78</v>
+      </c>
+      <c r="J47" t="s">
+        <v>117</v>
+      </c>
+      <c r="K47">
+        <v>0.9</v>
+      </c>
+      <c r="R47">
+        <v>0.91</v>
+      </c>
+      <c r="Y47">
         <v>0.99</v>
       </c>
-      <c r="Z18">
-        <v>1.04</v>
-      </c>
-    </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" t="s">
-        <v>79</v>
-      </c>
-      <c r="D19">
-        <v>2018</v>
-      </c>
-      <c r="E19" t="s">
-        <v>17</v>
-      </c>
-      <c r="F19" t="s">
-        <v>4</v>
-      </c>
-      <c r="G19" t="s">
+    </row>
+    <row r="48" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>1</v>
+      </c>
+      <c r="B48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" t="s">
+        <v>144</v>
+      </c>
+      <c r="D48">
+        <v>2012</v>
+      </c>
+      <c r="E48" t="s">
+        <v>134</v>
+      </c>
+      <c r="F48" t="s">
+        <v>129</v>
+      </c>
+      <c r="G48" t="s">
         <v>185</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H48" t="s">
         <v>149</v>
       </c>
-      <c r="I19" t="s">
-        <v>116</v>
-      </c>
-      <c r="J19" t="s">
-        <v>77</v>
-      </c>
-      <c r="K19">
-        <v>1.34</v>
-      </c>
-      <c r="R19">
-        <v>1.02</v>
-      </c>
-      <c r="Y19">
-        <v>1.28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" t="s">
-        <v>80</v>
-      </c>
-      <c r="D20">
-        <v>2016</v>
-      </c>
-      <c r="E20" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" t="s">
-        <v>4</v>
-      </c>
-      <c r="G20" t="s">
-        <v>185</v>
-      </c>
-      <c r="H20" t="s">
-        <v>149</v>
-      </c>
-      <c r="I20" t="s">
-        <v>78</v>
-      </c>
-      <c r="J20" t="s">
-        <v>117</v>
-      </c>
-      <c r="K20">
-        <v>0.9</v>
-      </c>
-      <c r="R20">
-        <v>0.91</v>
-      </c>
-      <c r="Y20">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" t="s">
-        <v>144</v>
-      </c>
-      <c r="D21">
-        <v>2012</v>
-      </c>
-      <c r="E21" t="s">
-        <v>134</v>
-      </c>
-      <c r="F21" t="s">
-        <v>129</v>
-      </c>
-      <c r="G21" t="s">
-        <v>185</v>
-      </c>
-      <c r="H21" t="s">
-        <v>149</v>
-      </c>
-      <c r="I21" t="s">
+      <c r="I48" t="s">
         <v>146</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J48" t="s">
         <v>145</v>
       </c>
-      <c r="K21">
+      <c r="K48">
         <f>1/1.08</f>
         <v>0.92592592592592582</v>
       </c>
-      <c r="M21">
+      <c r="M48">
         <f>1/1.12</f>
         <v>0.89285714285714279</v>
       </c>
-      <c r="O21">
+      <c r="O48">
         <f>1/1.08</f>
         <v>0.92592592592592582</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" t="s">
-        <v>193</v>
-      </c>
-      <c r="C22" t="s">
-        <v>147</v>
-      </c>
-      <c r="D22">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>1</v>
+      </c>
+      <c r="B49" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" t="s">
+        <v>169</v>
+      </c>
+      <c r="D49">
+        <v>2018</v>
+      </c>
+      <c r="E49" t="s">
+        <v>29</v>
+      </c>
+      <c r="F49" t="s">
+        <v>159</v>
+      </c>
+      <c r="G49" t="s">
+        <v>185</v>
+      </c>
+      <c r="H49" t="s">
+        <v>172</v>
+      </c>
+      <c r="I49" t="s">
+        <v>171</v>
+      </c>
+      <c r="J49" t="s">
+        <v>170</v>
+      </c>
+      <c r="K49">
+        <v>0.76</v>
+      </c>
+      <c r="O49">
+        <v>0.76</v>
+      </c>
+      <c r="R49">
+        <v>0.82</v>
+      </c>
+      <c r="U49">
+        <v>0.86</v>
+      </c>
+      <c r="Y49">
+        <v>0.98</v>
+      </c>
+      <c r="AA49">
+        <v>1.21</v>
+      </c>
+    </row>
+    <row r="50" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>1</v>
+      </c>
+      <c r="B50" t="s">
+        <v>10</v>
+      </c>
+      <c r="C50" t="s">
+        <v>177</v>
+      </c>
+      <c r="D50">
         <v>2013</v>
       </c>
-      <c r="E22" t="s">
-        <v>148</v>
-      </c>
-      <c r="G22" t="s">
+      <c r="E50" t="s">
+        <v>29</v>
+      </c>
+      <c r="F50" t="s">
+        <v>159</v>
+      </c>
+      <c r="G50" t="s">
         <v>185</v>
       </c>
-      <c r="H22" t="s">
-        <v>149</v>
-      </c>
-      <c r="I22" t="s">
-        <v>146</v>
-      </c>
-      <c r="J22" t="s">
-        <v>145</v>
-      </c>
-      <c r="K22">
-        <f>1/1.08</f>
-        <v>0.92592592592592582</v>
-      </c>
-      <c r="M22">
-        <f>1/1.14</f>
-        <v>0.87719298245614041</v>
-      </c>
-      <c r="O22">
-        <f>1/1.06</f>
-        <v>0.94339622641509424</v>
-      </c>
-      <c r="S22">
-        <f>1/0.89</f>
-        <v>1.1235955056179776</v>
-      </c>
-    </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" t="s">
-        <v>150</v>
-      </c>
-      <c r="C23" t="s">
-        <v>147</v>
-      </c>
-      <c r="D23">
-        <v>2013</v>
-      </c>
-      <c r="E23" t="s">
-        <v>154</v>
-      </c>
-      <c r="F23" t="s">
-        <v>129</v>
-      </c>
-      <c r="G23" t="s">
-        <v>185</v>
-      </c>
-      <c r="H23" t="s">
-        <v>149</v>
-      </c>
-      <c r="I23" t="s">
-        <v>146</v>
-      </c>
-      <c r="J23" t="s">
-        <v>145</v>
-      </c>
-      <c r="K23">
-        <f>1/1.08</f>
-        <v>0.92592592592592582</v>
-      </c>
-      <c r="M23">
-        <f>1/1.15</f>
-        <v>0.86956521739130443</v>
-      </c>
-      <c r="O23">
-        <f>1/0.94</f>
-        <v>1.0638297872340425</v>
-      </c>
-    </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" t="s">
-        <v>169</v>
-      </c>
-      <c r="D24">
-        <v>2018</v>
-      </c>
-      <c r="E24" t="s">
-        <v>29</v>
-      </c>
-      <c r="F24" t="s">
-        <v>159</v>
-      </c>
-      <c r="G24" t="s">
-        <v>185</v>
-      </c>
-      <c r="H24" t="s">
+      <c r="H50" t="s">
         <v>172</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I50" t="s">
         <v>171</v>
       </c>
-      <c r="J24" t="s">
+      <c r="J50" t="s">
         <v>170</v>
       </c>
-      <c r="K24">
-        <v>0.76</v>
-      </c>
-      <c r="O24">
-        <v>0.76</v>
-      </c>
-      <c r="R24">
-        <v>0.82</v>
-      </c>
-      <c r="U24">
-        <v>0.86</v>
-      </c>
-      <c r="Y24">
-        <v>0.98</v>
-      </c>
-      <c r="AA24">
-        <v>1.21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" t="s">
-        <v>177</v>
-      </c>
-      <c r="D25">
-        <v>2013</v>
-      </c>
-      <c r="E25" t="s">
-        <v>29</v>
-      </c>
-      <c r="F25" t="s">
-        <v>159</v>
-      </c>
-      <c r="G25" t="s">
-        <v>185</v>
-      </c>
-      <c r="H25" t="s">
-        <v>172</v>
-      </c>
-      <c r="I25" t="s">
-        <v>171</v>
-      </c>
-      <c r="J25" t="s">
-        <v>170</v>
-      </c>
-      <c r="K25">
+      <c r="K50">
         <f>1/2.4</f>
         <v>0.41666666666666669</v>
       </c>
-      <c r="N25">
+      <c r="N50">
         <f>1/2.4</f>
         <v>0.41666666666666669</v>
       </c>
-      <c r="Q25">
+      <c r="Q50">
         <f>1/2.3</f>
         <v>0.43478260869565222</v>
       </c>
-      <c r="U25">
+      <c r="U50">
         <f>1/2.2</f>
         <v>0.45454545454545453</v>
       </c>
-      <c r="X25">
+      <c r="X50">
         <f>1/1.9</f>
         <v>0.52631578947368418</v>
       </c>
-      <c r="Z25">
+      <c r="Z50">
         <f>1/1.6</f>
         <v>0.625</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>1</v>
-      </c>
-      <c r="B26" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" t="s">
-        <v>82</v>
-      </c>
-      <c r="D26">
-        <v>2015</v>
-      </c>
-      <c r="E26" t="s">
-        <v>17</v>
-      </c>
-      <c r="F26" t="s">
-        <v>4</v>
-      </c>
-      <c r="G26" t="s">
-        <v>185</v>
-      </c>
-      <c r="H26" t="s">
-        <v>118</v>
-      </c>
-      <c r="I26" t="s">
-        <v>81</v>
-      </c>
-      <c r="J26" t="s">
-        <v>153</v>
-      </c>
-      <c r="K26">
-        <v>1.2</v>
-      </c>
-      <c r="R26">
-        <v>1</v>
-      </c>
-      <c r="Z26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" t="s">
-        <v>151</v>
-      </c>
-      <c r="D27">
-        <v>2011</v>
-      </c>
-      <c r="E27" t="s">
-        <v>152</v>
-      </c>
-      <c r="G27" t="s">
-        <v>185</v>
-      </c>
-      <c r="H27" t="s">
-        <v>118</v>
-      </c>
-      <c r="I27" t="s">
-        <v>81</v>
-      </c>
-      <c r="J27" t="s">
-        <v>153</v>
-      </c>
-      <c r="K27">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>1</v>
-      </c>
-      <c r="B28" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28" t="s">
-        <v>160</v>
-      </c>
-      <c r="D28">
-        <v>2011</v>
-      </c>
-      <c r="E28" t="s">
-        <v>158</v>
-      </c>
-      <c r="F28" t="s">
-        <v>159</v>
-      </c>
-      <c r="G28" t="s">
-        <v>185</v>
-      </c>
-      <c r="H28" t="s">
-        <v>118</v>
-      </c>
-      <c r="I28" t="s">
-        <v>81</v>
-      </c>
-      <c r="J28" t="s">
-        <v>153</v>
-      </c>
-      <c r="K28">
-        <v>1.2</v>
-      </c>
-      <c r="P28">
-        <v>1</v>
-      </c>
-      <c r="U28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>1</v>
-      </c>
-      <c r="B29" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" t="s">
-        <v>161</v>
-      </c>
-      <c r="D29">
-        <v>2012</v>
-      </c>
-      <c r="E29" t="s">
-        <v>162</v>
-      </c>
-      <c r="F29" t="s">
-        <v>159</v>
-      </c>
-      <c r="G29" t="s">
-        <v>185</v>
-      </c>
-      <c r="H29" t="s">
-        <v>118</v>
-      </c>
-      <c r="I29" t="s">
-        <v>81</v>
-      </c>
-      <c r="J29" t="s">
-        <v>153</v>
-      </c>
-      <c r="K29">
-        <v>1.2</v>
-      </c>
-      <c r="P29">
-        <v>1</v>
-      </c>
-      <c r="U29">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" t="s">
-        <v>163</v>
-      </c>
-      <c r="D30">
-        <v>2007</v>
-      </c>
-      <c r="E30" t="s">
-        <v>29</v>
-      </c>
-      <c r="F30" t="s">
-        <v>159</v>
-      </c>
-      <c r="G30" t="s">
-        <v>185</v>
-      </c>
-      <c r="H30" t="s">
-        <v>118</v>
-      </c>
-      <c r="I30" t="s">
-        <v>81</v>
-      </c>
-      <c r="J30" t="s">
-        <v>153</v>
-      </c>
-      <c r="K30">
-        <v>1.18</v>
-      </c>
-      <c r="R30">
-        <v>1.22</v>
-      </c>
-      <c r="W30">
-        <v>1.47</v>
-      </c>
-    </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>1</v>
-      </c>
-      <c r="B31" t="s">
-        <v>10</v>
-      </c>
-      <c r="C31" t="s">
-        <v>164</v>
-      </c>
-      <c r="D31">
-        <v>2008</v>
-      </c>
-      <c r="E31" t="s">
-        <v>173</v>
-      </c>
-      <c r="F31" t="s">
-        <v>174</v>
-      </c>
-      <c r="G31" t="s">
-        <v>185</v>
-      </c>
-      <c r="H31" t="s">
-        <v>118</v>
-      </c>
-      <c r="I31" t="s">
-        <v>81</v>
-      </c>
-      <c r="J31" t="s">
-        <v>153</v>
-      </c>
-      <c r="K31">
-        <v>1.18</v>
-      </c>
-      <c r="P31">
-        <v>1.22</v>
-      </c>
-    </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>1</v>
-      </c>
-      <c r="B32" t="s">
-        <v>10</v>
-      </c>
-      <c r="C32" t="s">
-        <v>165</v>
-      </c>
-      <c r="D32">
-        <v>2016</v>
-      </c>
-      <c r="E32" t="s">
-        <v>29</v>
-      </c>
-      <c r="F32" t="s">
-        <v>159</v>
-      </c>
-      <c r="G32" t="s">
-        <v>185</v>
-      </c>
-      <c r="H32" t="s">
-        <v>118</v>
-      </c>
-      <c r="I32" t="s">
-        <v>166</v>
-      </c>
-      <c r="J32" t="s">
-        <v>167</v>
-      </c>
-      <c r="K32">
-        <v>1.25</v>
-      </c>
-      <c r="P32">
-        <v>1.24</v>
-      </c>
-      <c r="U32">
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="AE32">
-        <v>1.1399999999999999</v>
-      </c>
-    </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>1</v>
-      </c>
-      <c r="B33" t="s">
-        <v>10</v>
-      </c>
-      <c r="C33" t="s">
-        <v>168</v>
-      </c>
-      <c r="D33">
-        <v>2017</v>
-      </c>
-      <c r="E33" t="s">
-        <v>29</v>
-      </c>
-      <c r="F33" t="s">
-        <v>159</v>
-      </c>
-      <c r="G33" t="s">
-        <v>185</v>
-      </c>
-      <c r="H33" t="s">
-        <v>118</v>
-      </c>
-      <c r="I33" t="s">
-        <v>166</v>
-      </c>
-      <c r="J33" t="s">
-        <v>167</v>
-      </c>
-      <c r="K33">
-        <v>1.25</v>
-      </c>
-      <c r="P33">
-        <v>0.98</v>
-      </c>
-      <c r="AE33">
-        <v>1.45</v>
-      </c>
-    </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>1</v>
-      </c>
-      <c r="B34" t="s">
-        <v>10</v>
-      </c>
-      <c r="C34" t="s">
-        <v>125</v>
-      </c>
-      <c r="D34">
-        <v>2012</v>
-      </c>
-      <c r="E34" t="s">
-        <v>121</v>
-      </c>
-      <c r="F34" t="s">
-        <v>120</v>
-      </c>
-      <c r="G34" t="s">
-        <v>185</v>
-      </c>
-      <c r="H34" t="s">
-        <v>122</v>
-      </c>
-      <c r="I34" t="s">
-        <v>124</v>
-      </c>
-      <c r="J34" t="s">
-        <v>123</v>
-      </c>
-      <c r="K34">
-        <v>1.47</v>
-      </c>
-      <c r="P34">
-        <v>1.25</v>
-      </c>
-      <c r="U34">
-        <v>1.36</v>
-      </c>
-      <c r="Z34">
-        <v>1.42</v>
-      </c>
-      <c r="AE34">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>1</v>
-      </c>
-      <c r="B35" t="s">
-        <v>10</v>
-      </c>
-      <c r="C35" t="s">
-        <v>175</v>
-      </c>
-      <c r="D35">
-        <v>2008</v>
-      </c>
-      <c r="E35" t="s">
-        <v>173</v>
-      </c>
-      <c r="F35" t="s">
-        <v>174</v>
-      </c>
-      <c r="G35" t="s">
-        <v>185</v>
-      </c>
-      <c r="H35" t="s">
-        <v>122</v>
-      </c>
-      <c r="I35" t="s">
-        <v>124</v>
-      </c>
-      <c r="J35" t="s">
-        <v>123</v>
-      </c>
-      <c r="K35">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="Q35">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="T35">
-        <v>1.05</v>
-      </c>
-      <c r="W35">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="Z35">
-        <v>1.06</v>
-      </c>
-      <c r="AB35">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="AE35">
-        <v>1.22</v>
-      </c>
-    </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>1</v>
-      </c>
-      <c r="B36" t="s">
-        <v>10</v>
-      </c>
-      <c r="C36" t="s">
-        <v>176</v>
-      </c>
-      <c r="D36">
-        <v>2007</v>
-      </c>
-      <c r="E36" t="s">
-        <v>173</v>
-      </c>
-      <c r="F36" t="s">
-        <v>174</v>
-      </c>
-      <c r="G36" t="s">
-        <v>185</v>
-      </c>
-      <c r="H36" t="s">
-        <v>122</v>
-      </c>
-      <c r="I36" t="s">
-        <v>124</v>
-      </c>
-      <c r="J36" t="s">
-        <v>123</v>
-      </c>
-      <c r="K36">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="Q36">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="T36">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="W36">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="Z36">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="AB36">
-        <v>1.2</v>
-      </c>
-      <c r="AE36">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>1</v>
-      </c>
-      <c r="B37" t="s">
-        <v>10</v>
-      </c>
-      <c r="C37" t="s">
-        <v>182</v>
-      </c>
-      <c r="D37">
-        <v>2017</v>
-      </c>
-      <c r="E37" t="s">
-        <v>173</v>
-      </c>
-      <c r="F37" t="s">
-        <v>174</v>
-      </c>
-      <c r="G37" t="s">
-        <v>185</v>
-      </c>
-      <c r="H37" t="s">
-        <v>122</v>
-      </c>
-      <c r="I37" t="s">
-        <v>124</v>
-      </c>
-      <c r="J37" t="s">
-        <v>123</v>
-      </c>
-      <c r="K37">
-        <v>1.36</v>
-      </c>
-      <c r="Q37">
-        <v>1.45</v>
-      </c>
-      <c r="V37">
-        <v>1.45</v>
-      </c>
-      <c r="AA37">
-        <v>1.32</v>
-      </c>
-      <c r="AE37">
-        <v>1.86</v>
-      </c>
-    </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>1</v>
-      </c>
-      <c r="B38" t="s">
-        <v>10</v>
-      </c>
-      <c r="C38" t="s">
-        <v>183</v>
-      </c>
-      <c r="D38">
-        <v>2009</v>
-      </c>
-      <c r="E38" t="s">
-        <v>173</v>
-      </c>
-      <c r="F38" t="s">
-        <v>174</v>
-      </c>
-      <c r="G38" t="s">
-        <v>185</v>
-      </c>
-      <c r="H38" t="s">
-        <v>122</v>
-      </c>
-      <c r="I38" t="s">
-        <v>124</v>
-      </c>
-      <c r="J38" t="s">
-        <v>123</v>
-      </c>
-      <c r="K38">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="P38">
-        <v>1.29</v>
-      </c>
-      <c r="U38">
-        <v>1.45</v>
-      </c>
-    </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>1</v>
-      </c>
-      <c r="B39" t="s">
-        <v>186</v>
-      </c>
-      <c r="C39" t="s">
-        <v>190</v>
-      </c>
-      <c r="D39">
-        <v>2016</v>
-      </c>
-      <c r="E39" t="s">
-        <v>189</v>
-      </c>
-      <c r="F39" t="s">
-        <v>188</v>
-      </c>
-      <c r="G39" t="s">
-        <v>187</v>
-      </c>
-      <c r="H39" t="s">
-        <v>149</v>
-      </c>
-      <c r="I39" t="s">
-        <v>191</v>
-      </c>
-      <c r="J39" t="s">
-        <v>192</v>
-      </c>
-      <c r="K39">
-        <v>0.93</v>
-      </c>
-      <c r="S39">
-        <v>0.93</v>
-      </c>
-      <c r="AE39">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>1</v>
-      </c>
-      <c r="B40" t="s">
-        <v>186</v>
-      </c>
-      <c r="C40" t="s">
-        <v>194</v>
-      </c>
-      <c r="D40">
-        <v>2017</v>
-      </c>
-      <c r="E40" t="s">
-        <v>189</v>
-      </c>
-      <c r="F40" t="s">
-        <v>188</v>
-      </c>
-      <c r="G40" t="s">
-        <v>187</v>
-      </c>
-      <c r="H40" t="s">
-        <v>149</v>
-      </c>
-      <c r="I40" t="s">
-        <v>191</v>
-      </c>
-      <c r="J40" t="s">
-        <v>192</v>
-      </c>
-      <c r="K40">
-        <v>0.93</v>
-      </c>
-      <c r="S40">
-        <v>0.93</v>
-      </c>
-      <c r="AE40">
-        <v>1.1200000000000001</v>
-      </c>
-    </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>1</v>
-      </c>
-      <c r="B41" t="s">
-        <v>186</v>
-      </c>
-      <c r="C41" t="s">
-        <v>198</v>
-      </c>
-      <c r="D41">
-        <v>2012</v>
-      </c>
-      <c r="E41" t="s">
-        <v>189</v>
-      </c>
-      <c r="F41" t="s">
-        <v>199</v>
-      </c>
-      <c r="G41" t="s">
-        <v>185</v>
-      </c>
-      <c r="H41" t="s">
-        <v>196</v>
-      </c>
-      <c r="I41" t="s">
-        <v>197</v>
-      </c>
-      <c r="J41" t="s">
-        <v>195</v>
-      </c>
-      <c r="K41">
-        <v>2.2799999999999998</v>
-      </c>
-      <c r="N41">
-        <v>2.13</v>
-      </c>
-      <c r="P41">
-        <v>2.21</v>
-      </c>
-      <c r="S41">
-        <v>2.27</v>
-      </c>
-      <c r="U41">
-        <v>2.2200000000000002</v>
-      </c>
-    </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>1</v>
-      </c>
-      <c r="B42" t="s">
-        <v>150</v>
-      </c>
-      <c r="C42" t="s">
-        <v>200</v>
-      </c>
-      <c r="D42">
-        <v>2016</v>
-      </c>
-      <c r="E42" t="s">
-        <v>201</v>
-      </c>
-      <c r="F42" t="s">
-        <v>199</v>
-      </c>
-      <c r="G42" t="s">
-        <v>185</v>
-      </c>
-      <c r="H42" t="s">
-        <v>210</v>
-      </c>
-      <c r="I42" t="s">
-        <v>202</v>
-      </c>
-      <c r="J42" t="s">
-        <v>203</v>
-      </c>
-      <c r="K42">
-        <v>0.8</v>
-      </c>
-      <c r="L42">
-        <v>0.8</v>
-      </c>
-      <c r="M42">
-        <v>0.8</v>
-      </c>
-      <c r="N42">
-        <v>0.8</v>
-      </c>
-      <c r="O42">
-        <v>0.8</v>
-      </c>
-      <c r="AF42" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>1</v>
-      </c>
-      <c r="B43" t="s">
-        <v>186</v>
-      </c>
-      <c r="C43" t="s">
-        <v>207</v>
-      </c>
-      <c r="D43">
-        <v>2011</v>
-      </c>
-      <c r="E43" t="s">
-        <v>189</v>
-      </c>
-      <c r="F43" t="s">
-        <v>206</v>
-      </c>
-      <c r="G43" t="s">
-        <v>185</v>
-      </c>
-      <c r="H43" t="s">
-        <v>149</v>
-      </c>
-      <c r="I43" t="s">
-        <v>204</v>
-      </c>
-      <c r="J43" t="s">
-        <v>205</v>
-      </c>
-      <c r="K43">
-        <v>1.17</v>
-      </c>
-      <c r="N43">
-        <v>3.86</v>
-      </c>
-    </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>1</v>
-      </c>
-      <c r="B44" t="s">
-        <v>186</v>
-      </c>
-      <c r="C44" t="s">
-        <v>209</v>
-      </c>
-      <c r="D44">
-        <v>2011</v>
-      </c>
-      <c r="E44" t="s">
-        <v>189</v>
-      </c>
-      <c r="F44" t="s">
-        <v>208</v>
-      </c>
-      <c r="G44" t="s">
-        <v>185</v>
-      </c>
-      <c r="H44" t="s">
-        <v>149</v>
-      </c>
-      <c r="I44" t="s">
-        <v>204</v>
-      </c>
-      <c r="J44" t="s">
-        <v>205</v>
-      </c>
-      <c r="K44">
-        <v>1.21</v>
-      </c>
-      <c r="N44">
-        <v>1.25</v>
-      </c>
-      <c r="Q44">
-        <v>1.32</v>
-      </c>
-    </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>1</v>
-      </c>
-      <c r="B45" t="s">
-        <v>186</v>
-      </c>
-      <c r="C45" t="s">
-        <v>213</v>
-      </c>
-      <c r="D45">
-        <v>2012</v>
-      </c>
-      <c r="E45" t="s">
-        <v>189</v>
-      </c>
-      <c r="F45" t="s">
-        <v>211</v>
-      </c>
-      <c r="G45" t="s">
-        <v>185</v>
-      </c>
-      <c r="H45" t="s">
-        <v>118</v>
-      </c>
-      <c r="I45" t="s">
-        <v>166</v>
-      </c>
-      <c r="J45" t="s">
-        <v>167</v>
-      </c>
-      <c r="K45">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="N45">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="Q45">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>1</v>
-      </c>
-      <c r="B46" t="s">
-        <v>186</v>
-      </c>
-      <c r="C46" t="s">
-        <v>213</v>
-      </c>
-      <c r="D46">
-        <v>2012</v>
-      </c>
-      <c r="E46" t="s">
-        <v>189</v>
-      </c>
-      <c r="F46" t="s">
-        <v>212</v>
-      </c>
-      <c r="G46" t="s">
-        <v>185</v>
-      </c>
-      <c r="H46" t="s">
-        <v>118</v>
-      </c>
-      <c r="I46" t="s">
-        <v>166</v>
-      </c>
-      <c r="J46" t="s">
-        <v>167</v>
-      </c>
-      <c r="K46">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="N46">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="Q46">
-        <v>1.17</v>
-      </c>
-    </row>
-    <row r="47" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>1</v>
-      </c>
-      <c r="B47" t="s">
-        <v>186</v>
-      </c>
-      <c r="C47" t="s">
-        <v>213</v>
-      </c>
-      <c r="D47">
-        <v>2012</v>
-      </c>
-      <c r="E47" t="s">
-        <v>189</v>
-      </c>
-      <c r="F47" t="s">
-        <v>211</v>
-      </c>
-      <c r="G47" t="s">
-        <v>185</v>
-      </c>
-      <c r="H47" t="s">
-        <v>127</v>
-      </c>
-      <c r="I47" t="s">
-        <v>135</v>
-      </c>
-      <c r="J47" t="s">
-        <v>136</v>
-      </c>
-      <c r="K47">
-        <v>1.46</v>
-      </c>
-      <c r="N47">
-        <v>1.7</v>
-      </c>
-      <c r="Q47">
-        <v>1.64</v>
-      </c>
-    </row>
-    <row r="48" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>1</v>
-      </c>
-      <c r="B48" t="s">
-        <v>186</v>
-      </c>
-      <c r="C48" t="s">
-        <v>213</v>
-      </c>
-      <c r="D48">
-        <v>2012</v>
-      </c>
-      <c r="E48" t="s">
-        <v>189</v>
-      </c>
-      <c r="F48" t="s">
-        <v>212</v>
-      </c>
-      <c r="G48" t="s">
-        <v>185</v>
-      </c>
-      <c r="H48" t="s">
-        <v>127</v>
-      </c>
-      <c r="I48" t="s">
-        <v>135</v>
-      </c>
-      <c r="J48" t="s">
-        <v>136</v>
-      </c>
-      <c r="K48">
-        <v>1.46</v>
-      </c>
-      <c r="N48">
-        <v>1.52</v>
-      </c>
-      <c r="Q48">
-        <v>1.43</v>
-      </c>
-    </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>1</v>
-      </c>
-      <c r="B49" t="s">
-        <v>186</v>
-      </c>
-      <c r="C49" t="s">
-        <v>213</v>
-      </c>
-      <c r="D49">
-        <v>2012</v>
-      </c>
-      <c r="E49" t="s">
-        <v>189</v>
-      </c>
-      <c r="F49" t="s">
-        <v>211</v>
-      </c>
-      <c r="G49" t="s">
-        <v>185</v>
-      </c>
-      <c r="H49" t="s">
-        <v>196</v>
-      </c>
-      <c r="I49" t="s">
-        <v>214</v>
-      </c>
-      <c r="J49" t="s">
-        <v>195</v>
-      </c>
-      <c r="K49">
-        <v>1.91</v>
-      </c>
-      <c r="N49">
-        <v>1.6</v>
-      </c>
-      <c r="Q49">
-        <v>1.57</v>
-      </c>
-    </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>1</v>
-      </c>
-      <c r="B50" t="s">
-        <v>186</v>
-      </c>
-      <c r="C50" t="s">
-        <v>213</v>
-      </c>
-      <c r="D50">
-        <v>2012</v>
-      </c>
-      <c r="E50" t="s">
-        <v>189</v>
-      </c>
-      <c r="F50" t="s">
-        <v>212</v>
-      </c>
-      <c r="G50" t="s">
-        <v>185</v>
-      </c>
-      <c r="H50" t="s">
-        <v>196</v>
-      </c>
-      <c r="I50" t="s">
-        <v>214</v>
-      </c>
-      <c r="J50" t="s">
-        <v>195</v>
-      </c>
-      <c r="K50">
-        <v>1.91</v>
-      </c>
-      <c r="N50">
-        <v>1.82</v>
-      </c>
-      <c r="Q50">
-        <v>1.81</v>
-      </c>
-    </row>
     <row r="51" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>1</v>
       </c>
       <c r="B51" t="s">
-        <v>186</v>
+        <v>10</v>
       </c>
       <c r="C51" t="s">
-        <v>215</v>
+        <v>82</v>
       </c>
       <c r="D51">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="E51" t="s">
-        <v>189</v>
+        <v>17</v>
       </c>
       <c r="F51" t="s">
-        <v>216</v>
+        <v>4</v>
       </c>
       <c r="G51" t="s">
-        <v>217</v>
+        <v>185</v>
       </c>
       <c r="H51" t="s">
-        <v>149</v>
+        <v>118</v>
       </c>
       <c r="I51" t="s">
-        <v>116</v>
+        <v>81</v>
       </c>
       <c r="J51" t="s">
-        <v>77</v>
+        <v>153</v>
       </c>
       <c r="K51">
-        <v>1.92</v>
-      </c>
-      <c r="N51">
-        <v>2.11</v>
-      </c>
-      <c r="P51">
-        <v>1.7</v>
-      </c>
-      <c r="Q51">
-        <v>1.86</v>
-      </c>
-      <c r="T51">
-        <v>1.91</v>
+        <v>1.2</v>
+      </c>
+      <c r="R51">
+        <v>1</v>
+      </c>
+      <c r="Z51">
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:31" x14ac:dyDescent="0.35">
@@ -4452,31 +4446,31 @@
         <v>1</v>
       </c>
       <c r="B52" t="s">
-        <v>186</v>
+        <v>10</v>
       </c>
       <c r="C52" t="s">
-        <v>218</v>
+        <v>151</v>
       </c>
       <c r="D52">
-        <v>2015</v>
+        <v>2011</v>
       </c>
       <c r="E52" t="s">
-        <v>189</v>
-      </c>
-      <c r="F52" t="s">
-        <v>216</v>
+        <v>152</v>
       </c>
       <c r="G52" t="s">
-        <v>217</v>
+        <v>185</v>
       </c>
       <c r="H52" t="s">
-        <v>149</v>
+        <v>118</v>
       </c>
       <c r="I52" t="s">
-        <v>116</v>
+        <v>81</v>
       </c>
       <c r="J52" t="s">
-        <v>77</v>
+        <v>153</v>
+      </c>
+      <c r="K52">
+        <v>0.98</v>
       </c>
     </row>
     <row r="53" spans="1:31" x14ac:dyDescent="0.35">
@@ -4484,43 +4478,40 @@
         <v>1</v>
       </c>
       <c r="B53" t="s">
-        <v>193</v>
+        <v>10</v>
       </c>
       <c r="C53" t="s">
-        <v>222</v>
+        <v>160</v>
       </c>
       <c r="D53">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="E53" t="s">
-        <v>189</v>
+        <v>158</v>
       </c>
       <c r="F53" t="s">
-        <v>221</v>
+        <v>159</v>
       </c>
       <c r="G53" t="s">
-        <v>217</v>
+        <v>185</v>
       </c>
       <c r="H53" t="s">
-        <v>172</v>
+        <v>118</v>
       </c>
       <c r="I53" t="s">
-        <v>219</v>
+        <v>81</v>
       </c>
       <c r="J53" t="s">
-        <v>220</v>
+        <v>153</v>
       </c>
       <c r="K53">
-        <v>2.25</v>
-      </c>
-      <c r="L53">
-        <v>1.98</v>
-      </c>
-      <c r="M53">
-        <v>2.23</v>
-      </c>
-      <c r="N53">
-        <v>2.27</v>
+        <v>1.2</v>
+      </c>
+      <c r="P53">
+        <v>1</v>
+      </c>
+      <c r="U53">
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:31" x14ac:dyDescent="0.35">
@@ -4528,49 +4519,40 @@
         <v>1</v>
       </c>
       <c r="B54" t="s">
-        <v>186</v>
+        <v>10</v>
       </c>
       <c r="C54" t="s">
-        <v>225</v>
+        <v>161</v>
       </c>
       <c r="D54">
-        <v>1983</v>
+        <v>2012</v>
       </c>
       <c r="E54" t="s">
-        <v>189</v>
+        <v>162</v>
       </c>
       <c r="F54" t="s">
-        <v>226</v>
+        <v>159</v>
       </c>
       <c r="G54" t="s">
-        <v>217</v>
+        <v>185</v>
       </c>
       <c r="H54" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="I54" t="s">
-        <v>124</v>
+        <v>81</v>
       </c>
       <c r="J54" t="s">
-        <v>123</v>
+        <v>153</v>
       </c>
       <c r="K54">
-        <v>1.26</v>
-      </c>
-      <c r="N54">
-        <v>1.21</v>
-      </c>
-      <c r="Q54">
-        <v>1.42</v>
-      </c>
-      <c r="T54">
-        <v>1.51</v>
-      </c>
-      <c r="W54">
-        <v>2.09</v>
-      </c>
-      <c r="AC54">
-        <v>2.33</v>
+        <v>1.2</v>
+      </c>
+      <c r="P54">
+        <v>1</v>
+      </c>
+      <c r="U54">
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="55" spans="1:31" x14ac:dyDescent="0.35">
@@ -4578,43 +4560,40 @@
         <v>1</v>
       </c>
       <c r="B55" t="s">
-        <v>186</v>
+        <v>10</v>
       </c>
       <c r="C55" t="s">
-        <v>227</v>
+        <v>163</v>
       </c>
       <c r="D55">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="E55" t="s">
-        <v>228</v>
+        <v>29</v>
       </c>
       <c r="F55" t="s">
-        <v>229</v>
+        <v>159</v>
       </c>
       <c r="G55" t="s">
-        <v>217</v>
+        <v>185</v>
       </c>
       <c r="H55" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="I55" t="s">
-        <v>124</v>
+        <v>81</v>
       </c>
       <c r="J55" t="s">
-        <v>123</v>
+        <v>153</v>
       </c>
       <c r="K55">
-        <v>2.68</v>
-      </c>
-      <c r="M55">
-        <v>2.56</v>
-      </c>
-      <c r="P55">
-        <v>2.56</v>
-      </c>
-      <c r="T55">
-        <v>2.0299999999999998</v>
+        <v>1.18</v>
+      </c>
+      <c r="R55">
+        <v>1.22</v>
+      </c>
+      <c r="W55">
+        <v>1.47</v>
       </c>
     </row>
     <row r="56" spans="1:31" x14ac:dyDescent="0.35">
@@ -4622,43 +4601,37 @@
         <v>1</v>
       </c>
       <c r="B56" t="s">
-        <v>186</v>
+        <v>10</v>
       </c>
       <c r="C56" t="s">
-        <v>227</v>
+        <v>164</v>
       </c>
       <c r="D56">
         <v>2008</v>
       </c>
       <c r="E56" t="s">
-        <v>228</v>
+        <v>173</v>
       </c>
       <c r="F56" t="s">
-        <v>216</v>
+        <v>174</v>
       </c>
       <c r="G56" t="s">
-        <v>217</v>
+        <v>185</v>
       </c>
       <c r="H56" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="I56" t="s">
-        <v>124</v>
+        <v>81</v>
       </c>
       <c r="J56" t="s">
-        <v>123</v>
+        <v>153</v>
       </c>
       <c r="K56">
-        <v>2.68</v>
-      </c>
-      <c r="M56">
-        <v>2.59</v>
+        <v>1.18</v>
       </c>
       <c r="P56">
-        <v>2.57</v>
-      </c>
-      <c r="T56">
-        <v>1.76</v>
+        <v>1.22</v>
       </c>
     </row>
     <row r="57" spans="1:31" x14ac:dyDescent="0.35">
@@ -4666,46 +4639,43 @@
         <v>1</v>
       </c>
       <c r="B57" t="s">
-        <v>193</v>
+        <v>10</v>
       </c>
       <c r="C57" t="s">
-        <v>235</v>
+        <v>165</v>
       </c>
       <c r="D57">
-        <v>2001</v>
+        <v>2016</v>
       </c>
       <c r="E57" t="s">
-        <v>189</v>
+        <v>29</v>
       </c>
       <c r="F57" t="s">
-        <v>236</v>
+        <v>159</v>
       </c>
       <c r="G57" t="s">
-        <v>217</v>
+        <v>185</v>
       </c>
       <c r="H57" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="I57" t="s">
-        <v>231</v>
+        <v>166</v>
       </c>
       <c r="J57" t="s">
-        <v>233</v>
+        <v>167</v>
       </c>
       <c r="K57">
-        <v>2.14</v>
+        <v>1.25</v>
       </c>
       <c r="P57">
-        <v>2.31</v>
+        <v>1.24</v>
       </c>
       <c r="U57">
-        <v>2.5</v>
-      </c>
-      <c r="Z57">
-        <v>2.2400000000000002</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="AE57">
-        <v>2.2799999999999998</v>
+        <v>1.1399999999999999</v>
       </c>
     </row>
     <row r="58" spans="1:31" x14ac:dyDescent="0.35">
@@ -4713,46 +4683,40 @@
         <v>1</v>
       </c>
       <c r="B58" t="s">
-        <v>193</v>
+        <v>10</v>
       </c>
       <c r="C58" t="s">
-        <v>237</v>
+        <v>168</v>
       </c>
       <c r="D58">
-        <v>2002</v>
+        <v>2017</v>
       </c>
       <c r="E58" t="s">
-        <v>189</v>
+        <v>29</v>
       </c>
       <c r="F58" t="s">
-        <v>236</v>
+        <v>159</v>
       </c>
       <c r="G58" t="s">
-        <v>217</v>
+        <v>185</v>
       </c>
       <c r="H58" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="I58" t="s">
-        <v>232</v>
+        <v>166</v>
       </c>
       <c r="J58" t="s">
-        <v>130</v>
+        <v>167</v>
       </c>
       <c r="K58">
-        <v>2.1</v>
+        <v>1.25</v>
       </c>
       <c r="P58">
-        <v>2.06</v>
-      </c>
-      <c r="U58">
-        <v>2.12</v>
-      </c>
-      <c r="Z58">
-        <v>2.56</v>
+        <v>0.98</v>
       </c>
       <c r="AE58">
-        <v>2.5099999999999998</v>
+        <v>1.45</v>
       </c>
     </row>
     <row r="59" spans="1:31" x14ac:dyDescent="0.35">
@@ -4760,22 +4724,22 @@
         <v>1</v>
       </c>
       <c r="B59" t="s">
-        <v>193</v>
+        <v>10</v>
       </c>
       <c r="C59" t="s">
-        <v>240</v>
+        <v>125</v>
       </c>
       <c r="D59">
-        <v>1998</v>
+        <v>2012</v>
       </c>
       <c r="E59" t="s">
-        <v>189</v>
+        <v>121</v>
       </c>
       <c r="F59" t="s">
-        <v>239</v>
+        <v>120</v>
       </c>
       <c r="G59" t="s">
-        <v>217</v>
+        <v>185</v>
       </c>
       <c r="H59" t="s">
         <v>122</v>
@@ -4784,25 +4748,22 @@
         <v>124</v>
       </c>
       <c r="J59" t="s">
-        <v>241</v>
+        <v>123</v>
       </c>
       <c r="K59">
-        <v>1.03</v>
-      </c>
-      <c r="O59">
-        <v>1.07</v>
-      </c>
-      <c r="S59">
-        <v>1.28</v>
-      </c>
-      <c r="W59">
-        <v>1.45</v>
-      </c>
-      <c r="AA59">
-        <v>1.91</v>
+        <v>1.47</v>
+      </c>
+      <c r="P59">
+        <v>1.25</v>
+      </c>
+      <c r="U59">
+        <v>1.36</v>
+      </c>
+      <c r="Z59">
+        <v>1.42</v>
       </c>
       <c r="AE59">
-        <v>1.96</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="60" spans="1:31" x14ac:dyDescent="0.35">
@@ -4810,34 +4771,52 @@
         <v>1</v>
       </c>
       <c r="B60" t="s">
-        <v>186</v>
+        <v>10</v>
       </c>
       <c r="C60" t="s">
-        <v>243</v>
+        <v>175</v>
       </c>
       <c r="D60">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="E60" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="F60" t="s">
-        <v>242</v>
+        <v>174</v>
       </c>
       <c r="G60" t="s">
-        <v>217</v>
+        <v>185</v>
       </c>
       <c r="H60" t="s">
-        <v>149</v>
+        <v>122</v>
       </c>
       <c r="I60" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="J60" t="s">
-        <v>77</v>
-      </c>
-      <c r="K60" t="s">
-        <v>244</v>
+        <v>123</v>
+      </c>
+      <c r="K60">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="Q60">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="T60">
+        <v>1.05</v>
+      </c>
+      <c r="W60">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Z60">
+        <v>1.06</v>
+      </c>
+      <c r="AB60">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="AE60">
+        <v>1.22</v>
       </c>
     </row>
     <row r="61" spans="1:31" x14ac:dyDescent="0.35">
@@ -4845,40 +4824,52 @@
         <v>1</v>
       </c>
       <c r="B61" t="s">
-        <v>186</v>
+        <v>10</v>
       </c>
       <c r="C61" t="s">
-        <v>246</v>
+        <v>176</v>
       </c>
       <c r="D61">
-        <v>2009</v>
+        <v>2007</v>
       </c>
       <c r="E61" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="F61" t="s">
-        <v>245</v>
+        <v>174</v>
       </c>
       <c r="G61" t="s">
-        <v>217</v>
+        <v>185</v>
       </c>
       <c r="H61" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="I61" t="s">
-        <v>81</v>
+        <v>124</v>
       </c>
       <c r="J61" t="s">
-        <v>153</v>
+        <v>123</v>
       </c>
       <c r="K61">
-        <v>0.83</v>
-      </c>
-      <c r="L61">
-        <v>0.82</v>
-      </c>
-      <c r="M61">
-        <v>0.83</v>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Q61">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="T61">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="W61">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Z61">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AB61">
+        <v>1.2</v>
+      </c>
+      <c r="AE61">
+        <v>1.2</v>
       </c>
     </row>
     <row r="62" spans="1:31" x14ac:dyDescent="0.35">
@@ -4886,40 +4877,46 @@
         <v>1</v>
       </c>
       <c r="B62" t="s">
-        <v>186</v>
+        <v>10</v>
       </c>
       <c r="C62" t="s">
-        <v>248</v>
+        <v>182</v>
       </c>
       <c r="D62">
-        <v>2002</v>
+        <v>2017</v>
       </c>
       <c r="E62" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="F62" t="s">
-        <v>247</v>
+        <v>174</v>
       </c>
       <c r="G62" t="s">
-        <v>249</v>
+        <v>185</v>
       </c>
       <c r="H62" t="s">
-        <v>149</v>
+        <v>122</v>
       </c>
       <c r="I62" t="s">
-        <v>78</v>
+        <v>124</v>
       </c>
       <c r="J62" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="K62">
-        <v>1.35</v>
-      </c>
-      <c r="M62">
-        <v>1.41</v>
-      </c>
-      <c r="O62">
-        <v>1.43</v>
+        <v>1.36</v>
+      </c>
+      <c r="Q62">
+        <v>1.45</v>
+      </c>
+      <c r="V62">
+        <v>1.45</v>
+      </c>
+      <c r="AA62">
+        <v>1.32</v>
+      </c>
+      <c r="AE62">
+        <v>1.86</v>
       </c>
     </row>
     <row r="63" spans="1:31" x14ac:dyDescent="0.35">
@@ -4927,61 +4924,62 @@
         <v>1</v>
       </c>
       <c r="B63" t="s">
-        <v>186</v>
+        <v>10</v>
       </c>
       <c r="C63" t="s">
-        <v>251</v>
+        <v>183</v>
       </c>
       <c r="D63">
-        <v>2002</v>
+        <v>2009</v>
       </c>
       <c r="E63" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="F63" t="s">
-        <v>250</v>
+        <v>174</v>
       </c>
       <c r="G63" t="s">
         <v>185</v>
       </c>
       <c r="H63" t="s">
-        <v>149</v>
+        <v>122</v>
       </c>
       <c r="I63" t="s">
-        <v>204</v>
+        <v>124</v>
       </c>
       <c r="J63" t="s">
-        <v>205</v>
+        <v>123</v>
       </c>
       <c r="K63">
-        <v>1.21</v>
-      </c>
-      <c r="N63">
-        <v>1.25</v>
-      </c>
-      <c r="Q63">
-        <v>1.32</v>
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="P63">
+        <v>1.29</v>
+      </c>
+      <c r="U63">
+        <v>1.45</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C72" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
+        <v>252</v>
+      </c>
+      <c r="C73" t="s">
         <v>253</v>
       </c>
-      <c r="C73" t="s">
-        <v>254</v>
-      </c>
     </row>
   </sheetData>
-  <sortState ref="A2:AF69">
-    <sortCondition ref="H2:H37"/>
+  <sortState ref="A2:AF73">
+    <sortCondition ref="B2:B73"/>
+    <sortCondition ref="H2:H73"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
25/06/18 Push - FIFO amounts added to excel
</commit_message>
<xml_diff>
--- a/alternativefeeddata.xlsx
+++ b/alternativefeeddata.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2545" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3374" uniqueCount="311">
   <si>
     <t xml:space="preserve">Taxon </t>
   </si>
@@ -785,9 +785,6 @@
     <t>Wuchang bream</t>
   </si>
   <si>
-    <t xml:space="preserve">Turbot </t>
-  </si>
-  <si>
     <t xml:space="preserve">Carnivorous </t>
   </si>
   <si>
@@ -821,36 +818,6 @@
     <t>Pangasius catfish</t>
   </si>
   <si>
-    <t xml:space="preserve">Grass carp </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crucian carp </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wuchang bream </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indian major carps </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nile tilapia </t>
-  </si>
-  <si>
-    <t>Pangsiid catfish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hybrid catfish </t>
-  </si>
-  <si>
-    <t xml:space="preserve">North African Catfish </t>
-  </si>
-  <si>
-    <t>Amur catfish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yellow catfish </t>
-  </si>
-  <si>
     <t>Snakehead</t>
   </si>
   <si>
@@ -863,54 +830,12 @@
     <t xml:space="preserve">Carachidae </t>
   </si>
   <si>
-    <t xml:space="preserve">River eel </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Atlantic Salmon </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Barramundi </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flounder </t>
-  </si>
-  <si>
     <t xml:space="preserve">Atlantic Cod </t>
   </si>
   <si>
-    <t xml:space="preserve">European seabass </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gilthead seabream </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grouper </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Red drum </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mullet </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Japanese amberjack </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chinese mitten crab </t>
-  </si>
-  <si>
     <t xml:space="preserve">Redclaw crayfish </t>
   </si>
   <si>
-    <t xml:space="preserve">Giant river prawn </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oriental river prawn </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Whiteleg shrimp </t>
-  </si>
-  <si>
     <t xml:space="preserve">Giant tiger prawn </t>
   </si>
   <si>
@@ -927,6 +852,114 @@
   </si>
   <si>
     <t>All</t>
+  </si>
+  <si>
+    <t>African catfish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amur catfish </t>
+  </si>
+  <si>
+    <t>Liu 2013</t>
+  </si>
+  <si>
+    <t>Yellow catfish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dong 2012 </t>
+  </si>
+  <si>
+    <t>Paripananont</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yuan et al 2011 </t>
+  </si>
+  <si>
+    <t>Fernandes 2004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lochmann 2009 </t>
+  </si>
+  <si>
+    <t>EelStg</t>
+  </si>
+  <si>
+    <t>River eel</t>
+  </si>
+  <si>
+    <t>Atlantic Salmon</t>
+  </si>
+  <si>
+    <t>Salmon</t>
+  </si>
+  <si>
+    <t>Rainbow trout</t>
+  </si>
+  <si>
+    <t>Barramundi</t>
+  </si>
+  <si>
+    <t>Milkfish</t>
+  </si>
+  <si>
+    <t>Hansen 2007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MDemersal </t>
+  </si>
+  <si>
+    <t>European Seabass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gitlhead seabream </t>
+  </si>
+  <si>
+    <t>Grouper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wang 2008 </t>
+  </si>
+  <si>
+    <t>Red drum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kureshy 2000 </t>
+  </si>
+  <si>
+    <t>Shapawi 2007</t>
+  </si>
+  <si>
+    <t>Shapawi 2008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">McCoogan 1997 </t>
+  </si>
+  <si>
+    <t>Mullet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Khoaian 2014 </t>
+  </si>
+  <si>
+    <t>Amberjack</t>
+  </si>
+  <si>
+    <t>Crustaceans</t>
+  </si>
+  <si>
+    <t>Chinese mitten crab</t>
+  </si>
+  <si>
+    <t>Saoud 2008</t>
+  </si>
+  <si>
+    <t>Giant river prawn</t>
+  </si>
+  <si>
+    <t>*Chinese FCR weighted by 61.5%</t>
+  </si>
+  <si>
+    <t>Oriental river prawn</t>
   </si>
 </sst>
 </file>
@@ -1253,23 +1286,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S40"/>
+  <dimension ref="A1:H177"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D172" sqref="D172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>232</v>
       </c>
@@ -1292,7 +1325,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>236</v>
       </c>
@@ -1315,7 +1348,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>236</v>
       </c>
@@ -1338,7 +1371,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>236</v>
       </c>
@@ -1361,7 +1394,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>236</v>
       </c>
@@ -1383,11 +1416,8 @@
       <c r="G5" t="s">
         <v>245</v>
       </c>
-      <c r="S5" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>236</v>
       </c>
@@ -1409,11 +1439,8 @@
       <c r="G6" t="s">
         <v>245</v>
       </c>
-      <c r="S6" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>236</v>
       </c>
@@ -1435,11 +1462,8 @@
       <c r="G7" t="s">
         <v>245</v>
       </c>
-      <c r="S7" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>246</v>
       </c>
@@ -1461,11 +1485,8 @@
       <c r="G8" t="s">
         <v>245</v>
       </c>
-      <c r="S8" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>246</v>
       </c>
@@ -1487,11 +1508,8 @@
       <c r="G9" t="s">
         <v>245</v>
       </c>
-      <c r="S9" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>251</v>
       </c>
@@ -1513,11 +1531,8 @@
       <c r="G10" t="s">
         <v>245</v>
       </c>
-      <c r="S10" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>251</v>
       </c>
@@ -1539,11 +1554,8 @@
       <c r="G11" t="s">
         <v>245</v>
       </c>
-      <c r="S11" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>249</v>
       </c>
@@ -1565,11 +1577,8 @@
       <c r="G12" t="s">
         <v>245</v>
       </c>
-      <c r="S12" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>249</v>
       </c>
@@ -1591,11 +1600,8 @@
       <c r="G13" t="s">
         <v>245</v>
       </c>
-      <c r="S13" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>250</v>
       </c>
@@ -1617,11 +1623,8 @@
       <c r="G14" t="s">
         <v>245</v>
       </c>
-      <c r="S14" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>250</v>
       </c>
@@ -1643,11 +1646,8 @@
       <c r="G15" t="s">
         <v>245</v>
       </c>
-      <c r="S15" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>150</v>
       </c>
@@ -1655,7 +1655,7 @@
         <v>151</v>
       </c>
       <c r="C16" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D16" t="s">
         <v>240</v>
@@ -1669,11 +1669,8 @@
       <c r="G16" t="s">
         <v>245</v>
       </c>
-      <c r="S16" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>150</v>
       </c>
@@ -1681,7 +1678,7 @@
         <v>151</v>
       </c>
       <c r="C17" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D17" t="s">
         <v>240</v>
@@ -1695,19 +1692,16 @@
       <c r="G17" t="s">
         <v>245</v>
       </c>
-      <c r="S17" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B18" t="s">
         <v>151</v>
       </c>
       <c r="C18" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D18" t="s">
         <v>240</v>
@@ -1721,19 +1715,16 @@
       <c r="G18" t="s">
         <v>245</v>
       </c>
-      <c r="S18" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B19" t="s">
         <v>151</v>
       </c>
       <c r="C19" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D19" t="s">
         <v>240</v>
@@ -1747,19 +1738,16 @@
       <c r="G19" t="s">
         <v>245</v>
       </c>
-      <c r="S19" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B20" t="s">
         <v>151</v>
       </c>
       <c r="C20" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D20" t="s">
         <v>240</v>
@@ -1773,11 +1761,8 @@
       <c r="G20" t="s">
         <v>245</v>
       </c>
-      <c r="S20" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>95</v>
       </c>
@@ -1785,7 +1770,7 @@
         <v>151</v>
       </c>
       <c r="C21" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D21" t="s">
         <v>240</v>
@@ -1797,13 +1782,10 @@
         <v>70.400000000000006</v>
       </c>
       <c r="G21" t="s">
-        <v>256</v>
-      </c>
-      <c r="S21" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>95</v>
       </c>
@@ -1811,7 +1793,7 @@
         <v>151</v>
       </c>
       <c r="C22" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D22" t="s">
         <v>240</v>
@@ -1823,21 +1805,18 @@
         <v>12.4</v>
       </c>
       <c r="G22" t="s">
-        <v>256</v>
-      </c>
-      <c r="S22" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>297</v>
+        <v>272</v>
       </c>
       <c r="B23" t="s">
         <v>106</v>
       </c>
       <c r="C23" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D23" t="s">
         <v>240</v>
@@ -1849,21 +1828,18 @@
         <v>5</v>
       </c>
       <c r="G23" t="s">
-        <v>259</v>
-      </c>
-      <c r="S23" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B24" t="s">
         <v>106</v>
       </c>
       <c r="C24" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D24" t="s">
         <v>240</v>
@@ -1875,21 +1851,18 @@
         <v>20</v>
       </c>
       <c r="G24" t="s">
-        <v>261</v>
-      </c>
-      <c r="S24" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B25" t="s">
         <v>106</v>
       </c>
       <c r="C25" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D25" t="s">
         <v>240</v>
@@ -1901,21 +1874,18 @@
         <v>1.5</v>
       </c>
       <c r="G25" t="s">
-        <v>261</v>
-      </c>
-      <c r="S25" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B26" t="s">
         <v>106</v>
       </c>
       <c r="C26" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D26" t="s">
         <v>240</v>
@@ -1927,21 +1897,18 @@
         <v>15</v>
       </c>
       <c r="G26" t="s">
-        <v>262</v>
-      </c>
-      <c r="S26" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B27" t="s">
         <v>106</v>
       </c>
       <c r="C27" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D27" t="s">
         <v>240</v>
@@ -1953,15 +1920,12 @@
         <v>3.4</v>
       </c>
       <c r="G27" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>262</v>
-      </c>
-      <c r="S27" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>263</v>
       </c>
       <c r="B28" t="s">
         <v>31</v>
@@ -1979,15 +1943,12 @@
         <v>26</v>
       </c>
       <c r="G28" t="s">
-        <v>296</v>
-      </c>
-      <c r="S28" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B29" t="s">
         <v>31</v>
@@ -2005,13 +1966,10 @@
         <v>2</v>
       </c>
       <c r="G29" t="s">
-        <v>296</v>
-      </c>
-      <c r="S29" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>135</v>
       </c>
@@ -2022,7 +1980,7 @@
         <v>237</v>
       </c>
       <c r="D30" t="s">
-        <v>299</v>
+        <v>274</v>
       </c>
       <c r="E30" t="s">
         <v>195</v>
@@ -2031,13 +1989,10 @@
         <v>0</v>
       </c>
       <c r="G30" t="s">
-        <v>298</v>
-      </c>
-      <c r="S30" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>135</v>
       </c>
@@ -2048,7 +2003,7 @@
         <v>237</v>
       </c>
       <c r="D31" t="s">
-        <v>299</v>
+        <v>274</v>
       </c>
       <c r="E31" t="s">
         <v>242</v>
@@ -2057,13 +2012,10 @@
         <v>0</v>
       </c>
       <c r="G31" t="s">
-        <v>298</v>
-      </c>
-      <c r="S31" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>135</v>
       </c>
@@ -2074,7 +2026,7 @@
         <v>237</v>
       </c>
       <c r="D32" t="s">
-        <v>299</v>
+        <v>274</v>
       </c>
       <c r="E32" t="s">
         <v>195</v>
@@ -2083,13 +2035,10 @@
         <v>10</v>
       </c>
       <c r="G32" t="s">
-        <v>256</v>
-      </c>
-      <c r="S32" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>135</v>
       </c>
@@ -2100,7 +2049,7 @@
         <v>237</v>
       </c>
       <c r="D33" t="s">
-        <v>299</v>
+        <v>274</v>
       </c>
       <c r="E33" t="s">
         <v>242</v>
@@ -2109,45 +2058,3322 @@
         <v>10</v>
       </c>
       <c r="G33" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>275</v>
+      </c>
+      <c r="B34" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" t="s">
+        <v>237</v>
+      </c>
+      <c r="D34" t="s">
+        <v>240</v>
+      </c>
+      <c r="E34" t="s">
+        <v>195</v>
+      </c>
+      <c r="F34">
+        <v>25</v>
+      </c>
+      <c r="G34" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>275</v>
+      </c>
+      <c r="B35" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" t="s">
+        <v>237</v>
+      </c>
+      <c r="D35" t="s">
+        <v>240</v>
+      </c>
+      <c r="E35" t="s">
+        <v>242</v>
+      </c>
+      <c r="F35">
+        <v>6</v>
+      </c>
+      <c r="G35" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>275</v>
+      </c>
+      <c r="B36" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36" t="s">
+        <v>237</v>
+      </c>
+      <c r="D36" t="s">
+        <v>238</v>
+      </c>
+      <c r="E36" t="s">
+        <v>195</v>
+      </c>
+      <c r="F36">
+        <v>43</v>
+      </c>
+      <c r="G36" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>275</v>
+      </c>
+      <c r="B37" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" t="s">
+        <v>237</v>
+      </c>
+      <c r="D37" t="s">
+        <v>238</v>
+      </c>
+      <c r="E37" t="s">
+        <v>242</v>
+      </c>
+      <c r="F37">
+        <v>3</v>
+      </c>
+      <c r="G37" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>275</v>
+      </c>
+      <c r="B38" t="s">
+        <v>31</v>
+      </c>
+      <c r="C38" t="s">
+        <v>237</v>
+      </c>
+      <c r="D38" t="s">
+        <v>238</v>
+      </c>
+      <c r="E38" t="s">
+        <v>195</v>
+      </c>
+      <c r="F38">
+        <v>50</v>
+      </c>
+      <c r="G38" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>275</v>
+      </c>
+      <c r="B39" t="s">
+        <v>31</v>
+      </c>
+      <c r="C39" t="s">
+        <v>237</v>
+      </c>
+      <c r="D39" t="s">
+        <v>238</v>
+      </c>
+      <c r="E39" t="s">
+        <v>242</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>275</v>
+      </c>
+      <c r="B40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40" t="s">
+        <v>237</v>
+      </c>
+      <c r="D40" t="s">
+        <v>238</v>
+      </c>
+      <c r="E40" t="s">
+        <v>195</v>
+      </c>
+      <c r="F40">
+        <v>50</v>
+      </c>
+      <c r="G40" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>275</v>
+      </c>
+      <c r="B41" t="s">
+        <v>31</v>
+      </c>
+      <c r="C41" t="s">
+        <v>237</v>
+      </c>
+      <c r="D41" t="s">
+        <v>238</v>
+      </c>
+      <c r="E41" t="s">
+        <v>242</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>275</v>
+      </c>
+      <c r="B42" t="s">
+        <v>31</v>
+      </c>
+      <c r="C42" t="s">
+        <v>237</v>
+      </c>
+      <c r="D42" t="s">
+        <v>239</v>
+      </c>
+      <c r="E42" t="s">
+        <v>195</v>
+      </c>
+      <c r="F42">
+        <v>30</v>
+      </c>
+      <c r="G42" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>275</v>
+      </c>
+      <c r="B43" t="s">
+        <v>31</v>
+      </c>
+      <c r="C43" t="s">
+        <v>237</v>
+      </c>
+      <c r="D43" t="s">
+        <v>239</v>
+      </c>
+      <c r="E43" t="s">
+        <v>242</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>275</v>
+      </c>
+      <c r="B44" t="s">
+        <v>31</v>
+      </c>
+      <c r="C44" t="s">
+        <v>237</v>
+      </c>
+      <c r="D44" t="s">
+        <v>240</v>
+      </c>
+      <c r="E44" t="s">
+        <v>195</v>
+      </c>
+      <c r="F44">
+        <v>20</v>
+      </c>
+      <c r="G44" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>275</v>
+      </c>
+      <c r="B45" t="s">
+        <v>31</v>
+      </c>
+      <c r="C45" t="s">
+        <v>237</v>
+      </c>
+      <c r="D45" t="s">
+        <v>240</v>
+      </c>
+      <c r="E45" t="s">
+        <v>242</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>275</v>
+      </c>
+      <c r="B46" t="s">
+        <v>31</v>
+      </c>
+      <c r="C46" t="s">
+        <v>237</v>
+      </c>
+      <c r="D46" t="s">
+        <v>240</v>
+      </c>
+      <c r="E46" t="s">
+        <v>195</v>
+      </c>
+      <c r="F46">
+        <v>55</v>
+      </c>
+      <c r="G46" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>275</v>
+      </c>
+      <c r="B47" t="s">
+        <v>31</v>
+      </c>
+      <c r="C47" t="s">
+        <v>237</v>
+      </c>
+      <c r="D47" t="s">
+        <v>240</v>
+      </c>
+      <c r="E47" t="s">
+        <v>242</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>275</v>
+      </c>
+      <c r="B48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C48" t="s">
+        <v>237</v>
+      </c>
+      <c r="D48" t="s">
+        <v>240</v>
+      </c>
+      <c r="E48" t="s">
+        <v>195</v>
+      </c>
+      <c r="F48">
+        <v>10</v>
+      </c>
+      <c r="G48" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>275</v>
+      </c>
+      <c r="B49" t="s">
+        <v>31</v>
+      </c>
+      <c r="C49" t="s">
+        <v>237</v>
+      </c>
+      <c r="D49" t="s">
+        <v>240</v>
+      </c>
+      <c r="E49" t="s">
+        <v>242</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>275</v>
+      </c>
+      <c r="B50" t="s">
+        <v>31</v>
+      </c>
+      <c r="C50" t="s">
+        <v>237</v>
+      </c>
+      <c r="D50" t="s">
+        <v>240</v>
+      </c>
+      <c r="E50" t="s">
+        <v>195</v>
+      </c>
+      <c r="F50">
+        <v>10</v>
+      </c>
+      <c r="G50" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>275</v>
+      </c>
+      <c r="B51" t="s">
+        <v>31</v>
+      </c>
+      <c r="C51" t="s">
+        <v>237</v>
+      </c>
+      <c r="D51" t="s">
+        <v>240</v>
+      </c>
+      <c r="E51" t="s">
+        <v>242</v>
+      </c>
+      <c r="F51">
+        <v>3.3</v>
+      </c>
+      <c r="G51" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>275</v>
+      </c>
+      <c r="B52" t="s">
+        <v>31</v>
+      </c>
+      <c r="C52" t="s">
+        <v>237</v>
+      </c>
+      <c r="D52" t="s">
+        <v>240</v>
+      </c>
+      <c r="E52" t="s">
+        <v>195</v>
+      </c>
+      <c r="F52">
+        <v>24.7</v>
+      </c>
+      <c r="G52" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>275</v>
+      </c>
+      <c r="B53" t="s">
+        <v>31</v>
+      </c>
+      <c r="C53" t="s">
+        <v>237</v>
+      </c>
+      <c r="D53" t="s">
+        <v>240</v>
+      </c>
+      <c r="E53" t="s">
+        <v>242</v>
+      </c>
+      <c r="F53">
+        <v>6.8</v>
+      </c>
+      <c r="G53" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>275</v>
+      </c>
+      <c r="B54" t="s">
+        <v>31</v>
+      </c>
+      <c r="C54" t="s">
+        <v>237</v>
+      </c>
+      <c r="D54" t="s">
+        <v>240</v>
+      </c>
+      <c r="E54" t="s">
+        <v>195</v>
+      </c>
+      <c r="F54">
+        <v>20</v>
+      </c>
+      <c r="G54" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>275</v>
+      </c>
+      <c r="B55" t="s">
+        <v>31</v>
+      </c>
+      <c r="C55" t="s">
+        <v>237</v>
+      </c>
+      <c r="D55" t="s">
+        <v>240</v>
+      </c>
+      <c r="E55" t="s">
+        <v>242</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>275</v>
+      </c>
+      <c r="B56" t="s">
+        <v>31</v>
+      </c>
+      <c r="C56" t="s">
+        <v>237</v>
+      </c>
+      <c r="D56" t="s">
+        <v>240</v>
+      </c>
+      <c r="E56" t="s">
+        <v>195</v>
+      </c>
+      <c r="F56">
+        <v>2</v>
+      </c>
+      <c r="G56" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>275</v>
+      </c>
+      <c r="B57" t="s">
+        <v>31</v>
+      </c>
+      <c r="C57" t="s">
+        <v>237</v>
+      </c>
+      <c r="D57" t="s">
+        <v>240</v>
+      </c>
+      <c r="E57" t="s">
+        <v>242</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>276</v>
+      </c>
+      <c r="B58" t="s">
+        <v>31</v>
+      </c>
+      <c r="C58" t="s">
+        <v>252</v>
+      </c>
+      <c r="D58" t="s">
+        <v>240</v>
+      </c>
+      <c r="E58" t="s">
+        <v>195</v>
+      </c>
+      <c r="F58">
+        <v>60</v>
+      </c>
+      <c r="G58" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>276</v>
+      </c>
+      <c r="B59" t="s">
+        <v>31</v>
+      </c>
+      <c r="C59" t="s">
+        <v>252</v>
+      </c>
+      <c r="D59" t="s">
+        <v>240</v>
+      </c>
+      <c r="E59" t="s">
+        <v>195</v>
+      </c>
+      <c r="F59">
+        <v>49.4</v>
+      </c>
+      <c r="G59" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>276</v>
+      </c>
+      <c r="B60" t="s">
+        <v>31</v>
+      </c>
+      <c r="C60" t="s">
+        <v>252</v>
+      </c>
+      <c r="D60" t="s">
+        <v>240</v>
+      </c>
+      <c r="E60" t="s">
+        <v>195</v>
+      </c>
+      <c r="F60">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="G60" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>276</v>
+      </c>
+      <c r="B61" t="s">
+        <v>31</v>
+      </c>
+      <c r="C61" t="s">
+        <v>252</v>
+      </c>
+      <c r="D61" t="s">
+        <v>240</v>
+      </c>
+      <c r="E61" t="s">
+        <v>195</v>
+      </c>
+      <c r="F61">
+        <v>28.2</v>
+      </c>
+      <c r="G61" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>276</v>
+      </c>
+      <c r="B62" t="s">
+        <v>31</v>
+      </c>
+      <c r="C62" t="s">
+        <v>252</v>
+      </c>
+      <c r="D62" t="s">
+        <v>240</v>
+      </c>
+      <c r="E62" t="s">
+        <v>195</v>
+      </c>
+      <c r="F62">
+        <v>55.2</v>
+      </c>
+      <c r="G62" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>276</v>
+      </c>
+      <c r="B63" t="s">
+        <v>31</v>
+      </c>
+      <c r="C63" t="s">
+        <v>252</v>
+      </c>
+      <c r="D63" t="s">
+        <v>240</v>
+      </c>
+      <c r="E63" t="s">
+        <v>195</v>
+      </c>
+      <c r="F63">
+        <v>44.6</v>
+      </c>
+      <c r="G63" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>276</v>
+      </c>
+      <c r="B64" t="s">
+        <v>31</v>
+      </c>
+      <c r="C64" t="s">
+        <v>252</v>
+      </c>
+      <c r="D64" t="s">
+        <v>240</v>
+      </c>
+      <c r="E64" t="s">
+        <v>195</v>
+      </c>
+      <c r="F64">
+        <v>34</v>
+      </c>
+      <c r="G64" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>276</v>
+      </c>
+      <c r="B65" t="s">
+        <v>31</v>
+      </c>
+      <c r="C65" t="s">
+        <v>252</v>
+      </c>
+      <c r="D65" t="s">
+        <v>240</v>
+      </c>
+      <c r="E65" t="s">
+        <v>195</v>
+      </c>
+      <c r="F65">
+        <v>23.4</v>
+      </c>
+      <c r="G65" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>276</v>
+      </c>
+      <c r="B66" t="s">
+        <v>31</v>
+      </c>
+      <c r="C66" t="s">
+        <v>252</v>
+      </c>
+      <c r="D66" t="s">
+        <v>240</v>
+      </c>
+      <c r="E66" t="s">
+        <v>195</v>
+      </c>
+      <c r="F66">
+        <v>50.4</v>
+      </c>
+      <c r="G66" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>276</v>
+      </c>
+      <c r="B67" t="s">
+        <v>31</v>
+      </c>
+      <c r="C67" t="s">
+        <v>252</v>
+      </c>
+      <c r="D67" t="s">
+        <v>240</v>
+      </c>
+      <c r="E67" t="s">
+        <v>195</v>
+      </c>
+      <c r="F67">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="G67" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>276</v>
+      </c>
+      <c r="B68" t="s">
+        <v>31</v>
+      </c>
+      <c r="C68" t="s">
+        <v>252</v>
+      </c>
+      <c r="D68" t="s">
+        <v>240</v>
+      </c>
+      <c r="E68" t="s">
+        <v>195</v>
+      </c>
+      <c r="F68">
+        <v>29.2</v>
+      </c>
+      <c r="G68" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>276</v>
+      </c>
+      <c r="B69" t="s">
+        <v>31</v>
+      </c>
+      <c r="C69" t="s">
+        <v>252</v>
+      </c>
+      <c r="D69" t="s">
+        <v>240</v>
+      </c>
+      <c r="E69" t="s">
+        <v>195</v>
+      </c>
+      <c r="F69">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="G69" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>278</v>
+      </c>
+      <c r="B70" t="s">
+        <v>31</v>
+      </c>
+      <c r="C70" t="s">
+        <v>252</v>
+      </c>
+      <c r="D70" t="s">
+        <v>240</v>
+      </c>
+      <c r="E70" t="s">
+        <v>195</v>
+      </c>
+      <c r="F70">
+        <v>48</v>
+      </c>
+      <c r="G70" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>278</v>
+      </c>
+      <c r="B71" t="s">
+        <v>31</v>
+      </c>
+      <c r="C71" t="s">
+        <v>252</v>
+      </c>
+      <c r="D71" t="s">
+        <v>240</v>
+      </c>
+      <c r="E71" t="s">
+        <v>242</v>
+      </c>
+      <c r="F71">
+        <v>5.6</v>
+      </c>
+      <c r="G71" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>263</v>
+      </c>
+      <c r="B72" t="s">
+        <v>31</v>
+      </c>
+      <c r="C72" t="s">
+        <v>252</v>
+      </c>
+      <c r="D72" t="s">
+        <v>240</v>
+      </c>
+      <c r="E72" t="s">
+        <v>195</v>
+      </c>
+      <c r="F72">
+        <v>17.5</v>
+      </c>
+      <c r="G72" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>264</v>
+      </c>
+      <c r="B73" t="s">
+        <v>248</v>
+      </c>
+      <c r="C73" t="s">
+        <v>252</v>
+      </c>
+      <c r="D73" t="s">
+        <v>239</v>
+      </c>
+      <c r="E73" t="s">
+        <v>195</v>
+      </c>
+      <c r="F73">
+        <v>49</v>
+      </c>
+      <c r="G73" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>264</v>
+      </c>
+      <c r="B74" t="s">
+        <v>248</v>
+      </c>
+      <c r="C74" t="s">
+        <v>252</v>
+      </c>
+      <c r="D74" t="s">
+        <v>239</v>
+      </c>
+      <c r="E74" t="s">
+        <v>242</v>
+      </c>
+      <c r="F74">
+        <v>5</v>
+      </c>
+      <c r="G74" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>264</v>
+      </c>
+      <c r="B75" t="s">
+        <v>248</v>
+      </c>
+      <c r="C75" t="s">
+        <v>252</v>
+      </c>
+      <c r="D75" t="s">
+        <v>240</v>
+      </c>
+      <c r="E75" t="s">
+        <v>195</v>
+      </c>
+      <c r="F75">
+        <v>40</v>
+      </c>
+      <c r="G75" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>264</v>
+      </c>
+      <c r="B76" t="s">
+        <v>248</v>
+      </c>
+      <c r="C76" t="s">
+        <v>252</v>
+      </c>
+      <c r="D76" t="s">
+        <v>240</v>
+      </c>
+      <c r="E76" t="s">
+        <v>242</v>
+      </c>
+      <c r="F76">
+        <v>2</v>
+      </c>
+      <c r="G76" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>265</v>
+      </c>
+      <c r="B77" t="s">
+        <v>284</v>
+      </c>
+      <c r="C77" t="s">
+        <v>252</v>
+      </c>
+      <c r="D77" t="s">
+        <v>240</v>
+      </c>
+      <c r="E77" t="s">
+        <v>195</v>
+      </c>
+      <c r="F77">
+        <v>50</v>
+      </c>
+      <c r="G77" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>266</v>
+      </c>
+      <c r="B78" t="s">
+        <v>248</v>
+      </c>
+      <c r="C78" t="s">
+        <v>237</v>
+      </c>
+      <c r="D78" t="s">
+        <v>240</v>
+      </c>
+      <c r="E78" t="s">
+        <v>195</v>
+      </c>
+      <c r="F78">
+        <v>10</v>
+      </c>
+      <c r="G78" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>266</v>
+      </c>
+      <c r="B79" t="s">
+        <v>248</v>
+      </c>
+      <c r="C79" t="s">
+        <v>237</v>
+      </c>
+      <c r="D79" t="s">
+        <v>240</v>
+      </c>
+      <c r="E79" t="s">
+        <v>195</v>
+      </c>
+      <c r="F79">
+        <v>10</v>
+      </c>
+      <c r="G79" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>285</v>
+      </c>
+      <c r="B80" t="s">
+        <v>284</v>
+      </c>
+      <c r="C80" t="s">
+        <v>252</v>
+      </c>
+      <c r="D80" t="s">
+        <v>238</v>
+      </c>
+      <c r="E80" t="s">
+        <v>195</v>
+      </c>
+      <c r="F80">
+        <v>70</v>
+      </c>
+      <c r="G80" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>285</v>
+      </c>
+      <c r="B81" t="s">
+        <v>284</v>
+      </c>
+      <c r="C81" t="s">
+        <v>252</v>
+      </c>
+      <c r="D81" t="s">
+        <v>238</v>
+      </c>
+      <c r="E81" t="s">
+        <v>195</v>
+      </c>
+      <c r="F81">
+        <v>70</v>
+      </c>
+      <c r="G81" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>285</v>
+      </c>
+      <c r="B82" t="s">
+        <v>284</v>
+      </c>
+      <c r="C82" t="s">
+        <v>252</v>
+      </c>
+      <c r="D82" t="s">
+        <v>239</v>
+      </c>
+      <c r="E82" t="s">
+        <v>195</v>
+      </c>
+      <c r="F82">
+        <v>68</v>
+      </c>
+      <c r="G82" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>285</v>
+      </c>
+      <c r="B83" t="s">
+        <v>284</v>
+      </c>
+      <c r="C83" t="s">
+        <v>252</v>
+      </c>
+      <c r="D83" t="s">
+        <v>239</v>
+      </c>
+      <c r="E83" t="s">
+        <v>195</v>
+      </c>
+      <c r="F83">
+        <v>65</v>
+      </c>
+      <c r="G83" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>285</v>
+      </c>
+      <c r="B84" t="s">
+        <v>284</v>
+      </c>
+      <c r="C84" t="s">
+        <v>252</v>
+      </c>
+      <c r="D84" t="s">
+        <v>240</v>
+      </c>
+      <c r="E84" t="s">
+        <v>195</v>
+      </c>
+      <c r="F84">
+        <v>62</v>
+      </c>
+      <c r="G84" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>286</v>
+      </c>
+      <c r="B85" t="s">
+        <v>287</v>
+      </c>
+      <c r="C85" t="s">
+        <v>252</v>
+      </c>
+      <c r="D85" t="s">
+        <v>238</v>
+      </c>
+      <c r="E85" t="s">
+        <v>195</v>
+      </c>
+      <c r="F85">
+        <v>60.5</v>
+      </c>
+      <c r="G85" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>286</v>
+      </c>
+      <c r="B86" t="s">
+        <v>287</v>
+      </c>
+      <c r="C86" t="s">
+        <v>252</v>
+      </c>
+      <c r="D86" t="s">
+        <v>239</v>
+      </c>
+      <c r="E86" t="s">
+        <v>195</v>
+      </c>
+      <c r="F86">
+        <v>40.1</v>
+      </c>
+      <c r="G86" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>286</v>
+      </c>
+      <c r="B87" t="s">
+        <v>287</v>
+      </c>
+      <c r="C87" t="s">
+        <v>252</v>
+      </c>
+      <c r="D87" t="s">
+        <v>240</v>
+      </c>
+      <c r="E87" t="s">
+        <v>195</v>
+      </c>
+      <c r="F87">
+        <v>32.4</v>
+      </c>
+      <c r="G87" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>286</v>
+      </c>
+      <c r="B88" t="s">
+        <v>287</v>
+      </c>
+      <c r="C88" t="s">
+        <v>252</v>
+      </c>
+      <c r="D88" t="s">
+        <v>240</v>
+      </c>
+      <c r="E88" t="s">
+        <v>195</v>
+      </c>
+      <c r="F88">
+        <v>28.8</v>
+      </c>
+      <c r="G88" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>286</v>
+      </c>
+      <c r="B89" t="s">
+        <v>287</v>
+      </c>
+      <c r="C89" t="s">
+        <v>252</v>
+      </c>
+      <c r="D89" t="s">
+        <v>240</v>
+      </c>
+      <c r="E89" t="s">
+        <v>195</v>
+      </c>
+      <c r="F89">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="G89" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>286</v>
+      </c>
+      <c r="B90" t="s">
+        <v>287</v>
+      </c>
+      <c r="C90" t="s">
+        <v>252</v>
+      </c>
+      <c r="D90" t="s">
+        <v>238</v>
+      </c>
+      <c r="E90" t="s">
+        <v>242</v>
+      </c>
+      <c r="F90">
+        <v>10.4</v>
+      </c>
+      <c r="G90" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>286</v>
+      </c>
+      <c r="B91" t="s">
+        <v>287</v>
+      </c>
+      <c r="C91" t="s">
+        <v>252</v>
+      </c>
+      <c r="D91" t="s">
+        <v>239</v>
+      </c>
+      <c r="E91" t="s">
+        <v>242</v>
+      </c>
+      <c r="F91">
+        <v>14.8</v>
+      </c>
+      <c r="G91" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>286</v>
+      </c>
+      <c r="B92" t="s">
+        <v>287</v>
+      </c>
+      <c r="C92" t="s">
+        <v>252</v>
+      </c>
+      <c r="D92" t="s">
+        <v>240</v>
+      </c>
+      <c r="E92" t="s">
+        <v>242</v>
+      </c>
+      <c r="F92">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="G92" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>286</v>
+      </c>
+      <c r="B93" t="s">
+        <v>287</v>
+      </c>
+      <c r="C93" t="s">
+        <v>252</v>
+      </c>
+      <c r="D93" t="s">
+        <v>240</v>
+      </c>
+      <c r="E93" t="s">
+        <v>242</v>
+      </c>
+      <c r="F93">
+        <v>25.8</v>
+      </c>
+      <c r="G93" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>286</v>
+      </c>
+      <c r="B94" t="s">
+        <v>287</v>
+      </c>
+      <c r="C94" t="s">
+        <v>252</v>
+      </c>
+      <c r="D94" t="s">
+        <v>240</v>
+      </c>
+      <c r="E94" t="s">
+        <v>242</v>
+      </c>
+      <c r="F94">
+        <v>19.2</v>
+      </c>
+      <c r="G94" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>288</v>
+      </c>
+      <c r="B95" t="s">
+        <v>287</v>
+      </c>
+      <c r="C95" t="s">
+        <v>252</v>
+      </c>
+      <c r="D95" t="s">
+        <v>238</v>
+      </c>
+      <c r="E95" t="s">
+        <v>195</v>
+      </c>
+      <c r="F95">
+        <v>68</v>
+      </c>
+      <c r="G95" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>288</v>
+      </c>
+      <c r="B96" t="s">
+        <v>287</v>
+      </c>
+      <c r="C96" t="s">
+        <v>252</v>
+      </c>
+      <c r="D96" t="s">
+        <v>238</v>
+      </c>
+      <c r="E96" t="s">
+        <v>195</v>
+      </c>
+      <c r="F96">
+        <v>68</v>
+      </c>
+      <c r="G96" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>288</v>
+      </c>
+      <c r="B97" t="s">
+        <v>287</v>
+      </c>
+      <c r="C97" t="s">
+        <v>252</v>
+      </c>
+      <c r="D97" t="s">
+        <v>239</v>
+      </c>
+      <c r="E97" t="s">
+        <v>195</v>
+      </c>
+      <c r="F97">
+        <v>46</v>
+      </c>
+      <c r="G97" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>288</v>
+      </c>
+      <c r="B98" t="s">
+        <v>287</v>
+      </c>
+      <c r="C98" t="s">
+        <v>252</v>
+      </c>
+      <c r="D98" t="s">
+        <v>240</v>
+      </c>
+      <c r="E98" t="s">
+        <v>195</v>
+      </c>
+      <c r="F98">
+        <v>30</v>
+      </c>
+      <c r="G98" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>288</v>
+      </c>
+      <c r="B99" t="s">
+        <v>287</v>
+      </c>
+      <c r="C99" t="s">
+        <v>252</v>
+      </c>
+      <c r="D99" t="s">
+        <v>240</v>
+      </c>
+      <c r="E99" t="s">
+        <v>195</v>
+      </c>
+      <c r="F99">
+        <v>34</v>
+      </c>
+      <c r="G99" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>288</v>
+      </c>
+      <c r="B100" t="s">
+        <v>287</v>
+      </c>
+      <c r="C100" t="s">
+        <v>252</v>
+      </c>
+      <c r="D100" t="s">
+        <v>238</v>
+      </c>
+      <c r="E100" t="s">
+        <v>242</v>
+      </c>
+      <c r="F100">
+        <v>10</v>
+      </c>
+      <c r="G100" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>288</v>
+      </c>
+      <c r="B101" t="s">
+        <v>287</v>
+      </c>
+      <c r="C101" t="s">
+        <v>252</v>
+      </c>
+      <c r="D101" t="s">
+        <v>238</v>
+      </c>
+      <c r="E101" t="s">
+        <v>242</v>
+      </c>
+      <c r="F101">
+        <v>10</v>
+      </c>
+      <c r="G101" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>288</v>
+      </c>
+      <c r="B102" t="s">
+        <v>287</v>
+      </c>
+      <c r="C102" t="s">
+        <v>252</v>
+      </c>
+      <c r="D102" t="s">
+        <v>239</v>
+      </c>
+      <c r="E102" t="s">
+        <v>242</v>
+      </c>
+      <c r="F102">
+        <v>12</v>
+      </c>
+      <c r="G102" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>288</v>
+      </c>
+      <c r="B103" t="s">
+        <v>287</v>
+      </c>
+      <c r="C103" t="s">
+        <v>252</v>
+      </c>
+      <c r="D103" t="s">
+        <v>240</v>
+      </c>
+      <c r="E103" t="s">
+        <v>242</v>
+      </c>
+      <c r="F103">
+        <v>9</v>
+      </c>
+      <c r="G103" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>288</v>
+      </c>
+      <c r="B104" t="s">
+        <v>287</v>
+      </c>
+      <c r="C104" t="s">
+        <v>252</v>
+      </c>
+      <c r="D104" t="s">
+        <v>240</v>
+      </c>
+      <c r="E104" t="s">
+        <v>242</v>
+      </c>
+      <c r="F104">
+        <v>10</v>
+      </c>
+      <c r="G104" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>289</v>
+      </c>
+      <c r="B105" t="s">
+        <v>248</v>
+      </c>
+      <c r="C105" t="s">
+        <v>252</v>
+      </c>
+      <c r="D105" t="s">
+        <v>238</v>
+      </c>
+      <c r="E105" t="s">
+        <v>195</v>
+      </c>
+      <c r="F105">
+        <v>15</v>
+      </c>
+      <c r="G105" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>289</v>
+      </c>
+      <c r="B106" t="s">
+        <v>248</v>
+      </c>
+      <c r="C106" t="s">
+        <v>252</v>
+      </c>
+      <c r="D106" t="s">
+        <v>239</v>
+      </c>
+      <c r="E106" t="s">
+        <v>195</v>
+      </c>
+      <c r="F106">
+        <v>5</v>
+      </c>
+      <c r="G106" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>289</v>
+      </c>
+      <c r="B107" t="s">
+        <v>248</v>
+      </c>
+      <c r="C107" t="s">
+        <v>252</v>
+      </c>
+      <c r="D107" t="s">
+        <v>240</v>
+      </c>
+      <c r="E107" t="s">
+        <v>195</v>
+      </c>
+      <c r="F107">
+        <v>10</v>
+      </c>
+      <c r="G107" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>289</v>
+      </c>
+      <c r="B108" t="s">
+        <v>248</v>
+      </c>
+      <c r="C108" t="s">
+        <v>252</v>
+      </c>
+      <c r="D108" t="s">
+        <v>238</v>
+      </c>
+      <c r="E108" t="s">
+        <v>242</v>
+      </c>
+      <c r="F108">
+        <v>0</v>
+      </c>
+      <c r="G108" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>289</v>
+      </c>
+      <c r="B109" t="s">
+        <v>248</v>
+      </c>
+      <c r="C109" t="s">
+        <v>252</v>
+      </c>
+      <c r="D109" t="s">
+        <v>239</v>
+      </c>
+      <c r="E109" t="s">
+        <v>242</v>
+      </c>
+      <c r="F109">
+        <v>0</v>
+      </c>
+      <c r="G109" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>289</v>
+      </c>
+      <c r="B110" t="s">
+        <v>248</v>
+      </c>
+      <c r="C110" t="s">
+        <v>252</v>
+      </c>
+      <c r="D110" t="s">
+        <v>240</v>
+      </c>
+      <c r="E110" t="s">
+        <v>242</v>
+      </c>
+      <c r="F110">
+        <v>3.5</v>
+      </c>
+      <c r="G110" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>290</v>
+      </c>
+      <c r="B111" t="s">
+        <v>248</v>
+      </c>
+      <c r="C111" t="s">
+        <v>237</v>
+      </c>
+      <c r="D111" t="s">
+        <v>239</v>
+      </c>
+      <c r="E111" t="s">
+        <v>195</v>
+      </c>
+      <c r="F111">
+        <v>25</v>
+      </c>
+      <c r="G111" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>290</v>
+      </c>
+      <c r="B112" t="s">
+        <v>248</v>
+      </c>
+      <c r="C112" t="s">
+        <v>237</v>
+      </c>
+      <c r="D112" t="s">
+        <v>240</v>
+      </c>
+      <c r="E112" t="s">
+        <v>195</v>
+      </c>
+      <c r="F112">
+        <v>4</v>
+      </c>
+      <c r="G112" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>267</v>
+      </c>
+      <c r="B113" t="s">
+        <v>292</v>
+      </c>
+      <c r="C113" t="s">
+        <v>252</v>
+      </c>
+      <c r="D113" t="s">
+        <v>240</v>
+      </c>
+      <c r="E113" t="s">
+        <v>163</v>
+      </c>
+      <c r="F113">
+        <v>69.400000000000006</v>
+      </c>
+      <c r="G113" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>267</v>
+      </c>
+      <c r="B114" t="s">
+        <v>292</v>
+      </c>
+      <c r="C114" t="s">
+        <v>252</v>
+      </c>
+      <c r="D114" t="s">
+        <v>240</v>
+      </c>
+      <c r="E114" t="s">
+        <v>242</v>
+      </c>
+      <c r="F114">
+        <v>11.2</v>
+      </c>
+      <c r="G114" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>293</v>
+      </c>
+      <c r="B115" t="s">
+        <v>292</v>
+      </c>
+      <c r="C115" t="s">
+        <v>252</v>
+      </c>
+      <c r="D115" t="s">
+        <v>240</v>
+      </c>
+      <c r="E115" t="s">
+        <v>195</v>
+      </c>
+      <c r="F115">
+        <v>52</v>
+      </c>
+      <c r="G115" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>293</v>
+      </c>
+      <c r="B116" t="s">
+        <v>292</v>
+      </c>
+      <c r="C116" t="s">
+        <v>252</v>
+      </c>
+      <c r="D116" t="s">
+        <v>238</v>
+      </c>
+      <c r="E116" t="s">
+        <v>195</v>
+      </c>
+      <c r="F116">
+        <v>55</v>
+      </c>
+      <c r="G116" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>293</v>
+      </c>
+      <c r="B117" t="s">
+        <v>292</v>
+      </c>
+      <c r="C117" t="s">
+        <v>252</v>
+      </c>
+      <c r="D117" t="s">
+        <v>238</v>
+      </c>
+      <c r="E117" t="s">
+        <v>195</v>
+      </c>
+      <c r="F117">
+        <v>51</v>
+      </c>
+      <c r="G117" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>293</v>
+      </c>
+      <c r="B118" t="s">
+        <v>292</v>
+      </c>
+      <c r="C118" t="s">
+        <v>252</v>
+      </c>
+      <c r="D118" t="s">
+        <v>238</v>
+      </c>
+      <c r="E118" t="s">
+        <v>195</v>
+      </c>
+      <c r="F118">
+        <v>56</v>
+      </c>
+      <c r="G118" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>293</v>
+      </c>
+      <c r="B119" t="s">
+        <v>292</v>
+      </c>
+      <c r="C119" t="s">
+        <v>252</v>
+      </c>
+      <c r="D119" t="s">
+        <v>238</v>
+      </c>
+      <c r="E119" t="s">
+        <v>195</v>
+      </c>
+      <c r="F119">
+        <v>40</v>
+      </c>
+      <c r="G119" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>293</v>
+      </c>
+      <c r="B120" t="s">
+        <v>292</v>
+      </c>
+      <c r="C120" t="s">
+        <v>252</v>
+      </c>
+      <c r="D120" t="s">
+        <v>240</v>
+      </c>
+      <c r="E120" t="s">
+        <v>242</v>
+      </c>
+      <c r="F120">
+        <v>16</v>
+      </c>
+      <c r="G120" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>293</v>
+      </c>
+      <c r="B121" t="s">
+        <v>292</v>
+      </c>
+      <c r="C121" t="s">
+        <v>252</v>
+      </c>
+      <c r="D121" t="s">
+        <v>238</v>
+      </c>
+      <c r="E121" t="s">
+        <v>242</v>
+      </c>
+      <c r="F121">
+        <v>9</v>
+      </c>
+      <c r="G121" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>293</v>
+      </c>
+      <c r="B122" t="s">
+        <v>292</v>
+      </c>
+      <c r="C122" t="s">
+        <v>252</v>
+      </c>
+      <c r="D122" t="s">
+        <v>238</v>
+      </c>
+      <c r="E122" t="s">
+        <v>242</v>
+      </c>
+      <c r="F122">
+        <v>0</v>
+      </c>
+      <c r="G122" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>293</v>
+      </c>
+      <c r="B123" t="s">
+        <v>292</v>
+      </c>
+      <c r="C123" t="s">
+        <v>252</v>
+      </c>
+      <c r="D123" t="s">
+        <v>238</v>
+      </c>
+      <c r="E123" t="s">
+        <v>242</v>
+      </c>
+      <c r="F123">
+        <v>5</v>
+      </c>
+      <c r="G123" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>293</v>
+      </c>
+      <c r="B124" t="s">
+        <v>292</v>
+      </c>
+      <c r="C124" t="s">
+        <v>252</v>
+      </c>
+      <c r="D124" t="s">
+        <v>238</v>
+      </c>
+      <c r="E124" t="s">
+        <v>242</v>
+      </c>
+      <c r="F124">
+        <v>0</v>
+      </c>
+      <c r="G124" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>294</v>
+      </c>
+      <c r="B125" t="s">
+        <v>292</v>
+      </c>
+      <c r="C125" t="s">
+        <v>252</v>
+      </c>
+      <c r="D125" t="s">
+        <v>240</v>
+      </c>
+      <c r="E125" t="s">
+        <v>163</v>
+      </c>
+      <c r="F125">
+        <v>70.400000000000006</v>
+      </c>
+      <c r="G125" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>294</v>
+      </c>
+      <c r="B126" t="s">
+        <v>292</v>
+      </c>
+      <c r="C126" t="s">
+        <v>252</v>
+      </c>
+      <c r="D126" t="s">
+        <v>240</v>
+      </c>
+      <c r="E126" t="s">
+        <v>242</v>
+      </c>
+      <c r="F126">
+        <v>12.4</v>
+      </c>
+      <c r="G126" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>295</v>
+      </c>
+      <c r="B127" t="s">
+        <v>151</v>
+      </c>
+      <c r="C127" t="s">
+        <v>252</v>
+      </c>
+      <c r="D127" t="s">
+        <v>240</v>
+      </c>
+      <c r="E127" t="s">
+        <v>163</v>
+      </c>
+      <c r="F127">
+        <v>50</v>
+      </c>
+      <c r="G127" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>295</v>
+      </c>
+      <c r="B128" t="s">
+        <v>151</v>
+      </c>
+      <c r="C128" t="s">
+        <v>252</v>
+      </c>
+      <c r="D128" t="s">
+        <v>240</v>
+      </c>
+      <c r="E128" t="s">
+        <v>242</v>
+      </c>
+      <c r="F128">
+        <v>3.4</v>
+      </c>
+      <c r="G128" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>295</v>
+      </c>
+      <c r="B129" t="s">
+        <v>151</v>
+      </c>
+      <c r="C129" t="s">
+        <v>252</v>
+      </c>
+      <c r="D129" t="s">
+        <v>240</v>
+      </c>
+      <c r="E129" t="s">
+        <v>163</v>
+      </c>
+      <c r="F129">
+        <v>69.400000000000006</v>
+      </c>
+      <c r="G129" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>295</v>
+      </c>
+      <c r="B130" t="s">
+        <v>151</v>
+      </c>
+      <c r="C130" t="s">
+        <v>252</v>
+      </c>
+      <c r="D130" t="s">
+        <v>240</v>
+      </c>
+      <c r="E130" t="s">
+        <v>242</v>
+      </c>
+      <c r="F130">
+        <v>0</v>
+      </c>
+      <c r="G130" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>297</v>
+      </c>
+      <c r="B131" t="s">
+        <v>151</v>
+      </c>
+      <c r="C131" t="s">
+        <v>252</v>
+      </c>
+      <c r="D131" t="s">
+        <v>240</v>
+      </c>
+      <c r="E131" t="s">
+        <v>163</v>
+      </c>
+      <c r="F131">
+        <v>53.44</v>
+      </c>
+      <c r="G131" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>297</v>
+      </c>
+      <c r="B132" t="s">
+        <v>151</v>
+      </c>
+      <c r="C132" t="s">
+        <v>252</v>
+      </c>
+      <c r="D132" t="s">
+        <v>240</v>
+      </c>
+      <c r="E132" t="s">
+        <v>242</v>
+      </c>
+      <c r="F132">
+        <v>2.34</v>
+      </c>
+      <c r="G132" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>297</v>
+      </c>
+      <c r="B133" t="s">
+        <v>151</v>
+      </c>
+      <c r="C133" t="s">
+        <v>252</v>
+      </c>
+      <c r="D133" t="s">
+        <v>240</v>
+      </c>
+      <c r="E133" t="s">
+        <v>163</v>
+      </c>
+      <c r="F133">
+        <v>54.68</v>
+      </c>
+      <c r="G133" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>297</v>
+      </c>
+      <c r="B134" t="s">
+        <v>151</v>
+      </c>
+      <c r="C134" t="s">
+        <v>252</v>
+      </c>
+      <c r="D134" t="s">
+        <v>240</v>
+      </c>
+      <c r="E134" t="s">
+        <v>242</v>
+      </c>
+      <c r="F134">
+        <v>0.74</v>
+      </c>
+      <c r="G134" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>297</v>
+      </c>
+      <c r="B135" t="s">
+        <v>151</v>
+      </c>
+      <c r="C135" t="s">
+        <v>252</v>
+      </c>
+      <c r="D135" t="s">
+        <v>240</v>
+      </c>
+      <c r="E135" t="s">
+        <v>242</v>
+      </c>
+      <c r="F135">
+        <v>30</v>
+      </c>
+      <c r="G135" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>302</v>
+      </c>
+      <c r="B136" t="s">
+        <v>302</v>
+      </c>
+      <c r="C136" t="s">
+        <v>252</v>
+      </c>
+      <c r="D136" t="s">
+        <v>238</v>
+      </c>
+      <c r="E136" t="s">
+        <v>163</v>
+      </c>
+      <c r="F136">
+        <v>2.5</v>
+      </c>
+      <c r="G136" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>302</v>
+      </c>
+      <c r="B137" t="s">
+        <v>302</v>
+      </c>
+      <c r="C137" t="s">
+        <v>237</v>
+      </c>
+      <c r="D137" t="s">
+        <v>239</v>
+      </c>
+      <c r="E137" t="s">
+        <v>163</v>
+      </c>
+      <c r="F137">
+        <v>29</v>
+      </c>
+      <c r="G137" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>304</v>
+      </c>
+      <c r="B138" t="s">
+        <v>188</v>
+      </c>
+      <c r="C138" t="s">
+        <v>252</v>
+      </c>
+      <c r="D138" t="s">
+        <v>239</v>
+      </c>
+      <c r="E138" t="s">
+        <v>195</v>
+      </c>
+      <c r="F138">
+        <v>60</v>
+      </c>
+      <c r="G138" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>304</v>
+      </c>
+      <c r="B139" t="s">
+        <v>188</v>
+      </c>
+      <c r="C139" t="s">
+        <v>252</v>
+      </c>
+      <c r="D139" t="s">
+        <v>239</v>
+      </c>
+      <c r="E139" t="s">
+        <v>242</v>
+      </c>
+      <c r="F139">
+        <v>16</v>
+      </c>
+      <c r="G139" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>306</v>
+      </c>
+      <c r="B140" t="s">
+        <v>305</v>
+      </c>
+      <c r="C140" t="s">
+        <v>237</v>
+      </c>
+      <c r="D140" t="s">
+        <v>239</v>
+      </c>
+      <c r="E140" t="s">
+        <v>163</v>
+      </c>
+      <c r="F140">
+        <v>32</v>
+      </c>
+      <c r="G140" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>306</v>
+      </c>
+      <c r="B141" t="s">
+        <v>305</v>
+      </c>
+      <c r="C141" t="s">
+        <v>237</v>
+      </c>
+      <c r="D141" t="s">
+        <v>240</v>
+      </c>
+      <c r="E141" t="s">
+        <v>163</v>
+      </c>
+      <c r="F141">
+        <v>24.5</v>
+      </c>
+      <c r="G141" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>268</v>
+      </c>
+      <c r="B142" t="s">
+        <v>305</v>
+      </c>
+      <c r="C142" t="s">
+        <v>237</v>
+      </c>
+      <c r="D142" t="s">
+        <v>231</v>
+      </c>
+      <c r="E142" t="s">
+        <v>163</v>
+      </c>
+      <c r="F142">
+        <v>150</v>
+      </c>
+      <c r="G142" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>268</v>
+      </c>
+      <c r="B143" t="s">
+        <v>305</v>
+      </c>
+      <c r="C143" t="s">
+        <v>237</v>
+      </c>
+      <c r="D143" t="s">
+        <v>231</v>
+      </c>
+      <c r="E143" t="s">
+        <v>242</v>
+      </c>
+      <c r="F143">
+        <v>3.9</v>
+      </c>
+      <c r="G143" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>308</v>
+      </c>
+      <c r="B144" t="s">
+        <v>174</v>
+      </c>
+      <c r="C144" t="s">
+        <v>237</v>
+      </c>
+      <c r="D144" t="s">
+        <v>240</v>
+      </c>
+      <c r="E144" t="s">
+        <v>163</v>
+      </c>
+      <c r="F144">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="G144" t="s">
+        <v>245</v>
+      </c>
+      <c r="H144" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>308</v>
+      </c>
+      <c r="B145" t="s">
+        <v>174</v>
+      </c>
+      <c r="C145" t="s">
+        <v>237</v>
+      </c>
+      <c r="D145" t="s">
+        <v>240</v>
+      </c>
+      <c r="E145" t="s">
+        <v>163</v>
+      </c>
+      <c r="F145">
+        <v>27.8</v>
+      </c>
+      <c r="G145" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>308</v>
+      </c>
+      <c r="B146" t="s">
+        <v>174</v>
+      </c>
+      <c r="C146" t="s">
+        <v>237</v>
+      </c>
+      <c r="D146" t="s">
+        <v>240</v>
+      </c>
+      <c r="E146" t="s">
+        <v>163</v>
+      </c>
+      <c r="F146">
+        <v>23.5</v>
+      </c>
+      <c r="G146" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>308</v>
+      </c>
+      <c r="B147" t="s">
+        <v>174</v>
+      </c>
+      <c r="C147" t="s">
+        <v>237</v>
+      </c>
+      <c r="D147" t="s">
+        <v>240</v>
+      </c>
+      <c r="E147" t="s">
+        <v>163</v>
+      </c>
+      <c r="F147">
+        <v>23</v>
+      </c>
+      <c r="G147" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>308</v>
+      </c>
+      <c r="B148" t="s">
+        <v>174</v>
+      </c>
+      <c r="C148" t="s">
+        <v>237</v>
+      </c>
+      <c r="D148" t="s">
+        <v>240</v>
+      </c>
+      <c r="E148" t="s">
+        <v>242</v>
+      </c>
+      <c r="F148">
+        <v>3.7</v>
+      </c>
+      <c r="G148" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>310</v>
+      </c>
+      <c r="B149" t="s">
+        <v>174</v>
+      </c>
+      <c r="C149" t="s">
+        <v>237</v>
+      </c>
+      <c r="D149" t="s">
+        <v>231</v>
+      </c>
+      <c r="E149" t="s">
+        <v>163</v>
+      </c>
+      <c r="F149">
+        <v>23.3</v>
+      </c>
+      <c r="G149" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>310</v>
+      </c>
+      <c r="B150" t="s">
+        <v>174</v>
+      </c>
+      <c r="C150" t="s">
+        <v>237</v>
+      </c>
+      <c r="D150" t="s">
+        <v>240</v>
+      </c>
+      <c r="E150" t="s">
+        <v>163</v>
+      </c>
+      <c r="F150">
+        <v>19</v>
+      </c>
+      <c r="G150" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>310</v>
+      </c>
+      <c r="B151" t="s">
+        <v>174</v>
+      </c>
+      <c r="C151" t="s">
+        <v>237</v>
+      </c>
+      <c r="D151" t="s">
+        <v>240</v>
+      </c>
+      <c r="E151" t="s">
+        <v>163</v>
+      </c>
+      <c r="F151">
+        <v>11.3</v>
+      </c>
+      <c r="G151" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>192</v>
+      </c>
+      <c r="B152" t="s">
+        <v>174</v>
+      </c>
+      <c r="C152" t="s">
+        <v>237</v>
+      </c>
+      <c r="D152" t="s">
+        <v>231</v>
+      </c>
+      <c r="E152" t="s">
+        <v>163</v>
+      </c>
+      <c r="F152">
+        <v>30</v>
+      </c>
+      <c r="G152" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>192</v>
+      </c>
+      <c r="B153" t="s">
+        <v>174</v>
+      </c>
+      <c r="C153" t="s">
+        <v>237</v>
+      </c>
+      <c r="D153" t="s">
+        <v>240</v>
+      </c>
+      <c r="E153" t="s">
+        <v>163</v>
+      </c>
+      <c r="F153">
+        <v>25</v>
+      </c>
+      <c r="G153" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>192</v>
+      </c>
+      <c r="B154" t="s">
+        <v>174</v>
+      </c>
+      <c r="C154" t="s">
+        <v>237</v>
+      </c>
+      <c r="D154" t="s">
+        <v>240</v>
+      </c>
+      <c r="E154" t="s">
+        <v>163</v>
+      </c>
+      <c r="F154">
+        <v>23</v>
+      </c>
+      <c r="G154" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>192</v>
+      </c>
+      <c r="B155" t="s">
+        <v>174</v>
+      </c>
+      <c r="C155" t="s">
+        <v>237</v>
+      </c>
+      <c r="D155" t="s">
+        <v>240</v>
+      </c>
+      <c r="E155" t="s">
+        <v>242</v>
+      </c>
+      <c r="F155">
+        <v>1</v>
+      </c>
+      <c r="G155" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>192</v>
+      </c>
+      <c r="B156" t="s">
+        <v>174</v>
+      </c>
+      <c r="C156" t="s">
+        <v>237</v>
+      </c>
+      <c r="D156" t="s">
+        <v>240</v>
+      </c>
+      <c r="E156" t="s">
+        <v>242</v>
+      </c>
+      <c r="F156">
+        <v>1</v>
+      </c>
+      <c r="G156" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>192</v>
+      </c>
+      <c r="B157" t="s">
+        <v>174</v>
+      </c>
+      <c r="C157" t="s">
+        <v>237</v>
+      </c>
+      <c r="D157" t="s">
+        <v>240</v>
+      </c>
+      <c r="E157" t="s">
+        <v>242</v>
+      </c>
+      <c r="F157">
+        <v>1</v>
+      </c>
+      <c r="G157" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>269</v>
+      </c>
+      <c r="B158" t="s">
+        <v>174</v>
+      </c>
+      <c r="C158" t="s">
         <v>256</v>
       </c>
-      <c r="S33" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S34" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S35" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S36" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S37" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S38" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S39" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S40" t="s">
-        <v>295</v>
+      <c r="D158" t="s">
+        <v>231</v>
+      </c>
+      <c r="E158" t="s">
+        <v>163</v>
+      </c>
+      <c r="F158">
+        <v>5</v>
+      </c>
+      <c r="G158" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>269</v>
+      </c>
+      <c r="B159" t="s">
+        <v>174</v>
+      </c>
+      <c r="C159" t="s">
+        <v>256</v>
+      </c>
+      <c r="D159" t="s">
+        <v>231</v>
+      </c>
+      <c r="E159" t="s">
+        <v>163</v>
+      </c>
+      <c r="F159">
+        <v>6</v>
+      </c>
+      <c r="G159" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>269</v>
+      </c>
+      <c r="B160" t="s">
+        <v>174</v>
+      </c>
+      <c r="C160" t="s">
+        <v>256</v>
+      </c>
+      <c r="D160" t="s">
+        <v>231</v>
+      </c>
+      <c r="E160" t="s">
+        <v>242</v>
+      </c>
+      <c r="F160">
+        <v>0.7</v>
+      </c>
+      <c r="G160" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>269</v>
+      </c>
+      <c r="B161" t="s">
+        <v>174</v>
+      </c>
+      <c r="C161" t="s">
+        <v>256</v>
+      </c>
+      <c r="D161" t="s">
+        <v>231</v>
+      </c>
+      <c r="E161" t="s">
+        <v>242</v>
+      </c>
+      <c r="F161">
+        <v>0</v>
+      </c>
+      <c r="G161" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>269</v>
+      </c>
+      <c r="B162" t="s">
+        <v>174</v>
+      </c>
+      <c r="C162" t="s">
+        <v>252</v>
+      </c>
+      <c r="D162" t="s">
+        <v>240</v>
+      </c>
+      <c r="E162" t="s">
+        <v>163</v>
+      </c>
+      <c r="F162">
+        <v>28</v>
+      </c>
+      <c r="G162" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>269</v>
+      </c>
+      <c r="B163" t="s">
+        <v>174</v>
+      </c>
+      <c r="C163" t="s">
+        <v>252</v>
+      </c>
+      <c r="D163" t="s">
+        <v>240</v>
+      </c>
+      <c r="E163" t="s">
+        <v>163</v>
+      </c>
+      <c r="F163">
+        <v>33</v>
+      </c>
+      <c r="G163" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>269</v>
+      </c>
+      <c r="B164" t="s">
+        <v>174</v>
+      </c>
+      <c r="C164" t="s">
+        <v>252</v>
+      </c>
+      <c r="D164" t="s">
+        <v>240</v>
+      </c>
+      <c r="E164" t="s">
+        <v>163</v>
+      </c>
+      <c r="F164">
+        <v>18</v>
+      </c>
+      <c r="G164" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>269</v>
+      </c>
+      <c r="B165" t="s">
+        <v>174</v>
+      </c>
+      <c r="C165" t="s">
+        <v>252</v>
+      </c>
+      <c r="D165" t="s">
+        <v>240</v>
+      </c>
+      <c r="E165" t="s">
+        <v>163</v>
+      </c>
+      <c r="F165">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="G165" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>269</v>
+      </c>
+      <c r="B166" t="s">
+        <v>174</v>
+      </c>
+      <c r="C166" t="s">
+        <v>252</v>
+      </c>
+      <c r="D166" t="s">
+        <v>240</v>
+      </c>
+      <c r="E166" t="s">
+        <v>163</v>
+      </c>
+      <c r="F166">
+        <v>25.2</v>
+      </c>
+      <c r="G166" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>269</v>
+      </c>
+      <c r="B167" t="s">
+        <v>174</v>
+      </c>
+      <c r="C167" t="s">
+        <v>252</v>
+      </c>
+      <c r="D167" t="s">
+        <v>240</v>
+      </c>
+      <c r="E167" t="s">
+        <v>242</v>
+      </c>
+      <c r="F167">
+        <v>3</v>
+      </c>
+      <c r="G167" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>269</v>
+      </c>
+      <c r="B168" t="s">
+        <v>174</v>
+      </c>
+      <c r="C168" t="s">
+        <v>252</v>
+      </c>
+      <c r="D168" t="s">
+        <v>240</v>
+      </c>
+      <c r="E168" t="s">
+        <v>242</v>
+      </c>
+      <c r="F168">
+        <v>3.5</v>
+      </c>
+      <c r="G168" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>269</v>
+      </c>
+      <c r="B169" t="s">
+        <v>174</v>
+      </c>
+      <c r="C169" t="s">
+        <v>252</v>
+      </c>
+      <c r="D169" t="s">
+        <v>240</v>
+      </c>
+      <c r="E169" t="s">
+        <v>242</v>
+      </c>
+      <c r="F169">
+        <v>0.7</v>
+      </c>
+      <c r="G169" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>269</v>
+      </c>
+      <c r="B170" t="s">
+        <v>174</v>
+      </c>
+      <c r="C170" t="s">
+        <v>252</v>
+      </c>
+      <c r="D170" t="s">
+        <v>240</v>
+      </c>
+      <c r="E170" t="s">
+        <v>242</v>
+      </c>
+      <c r="F170">
+        <v>5</v>
+      </c>
+      <c r="G170" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>269</v>
+      </c>
+      <c r="B171" t="s">
+        <v>174</v>
+      </c>
+      <c r="C171" t="s">
+        <v>252</v>
+      </c>
+      <c r="D171" t="s">
+        <v>240</v>
+      </c>
+      <c r="E171" t="s">
+        <v>242</v>
+      </c>
+      <c r="F171">
+        <v>0</v>
+      </c>
+      <c r="G171" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>270</v>
+      </c>
+      <c r="B172" t="s">
+        <v>174</v>
+      </c>
+      <c r="C172" t="s">
+        <v>237</v>
+      </c>
+      <c r="D172" t="s">
+        <v>231</v>
+      </c>
+      <c r="E172" t="s">
+        <v>163</v>
+      </c>
+      <c r="F172">
+        <v>27</v>
+      </c>
+      <c r="G172" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>270</v>
+      </c>
+      <c r="B173" t="s">
+        <v>174</v>
+      </c>
+      <c r="C173" t="s">
+        <v>237</v>
+      </c>
+      <c r="D173" t="s">
+        <v>240</v>
+      </c>
+      <c r="E173" t="s">
+        <v>163</v>
+      </c>
+      <c r="F173">
+        <v>25</v>
+      </c>
+      <c r="G173" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>270</v>
+      </c>
+      <c r="B174" t="s">
+        <v>174</v>
+      </c>
+      <c r="C174" t="s">
+        <v>237</v>
+      </c>
+      <c r="D174" t="s">
+        <v>240</v>
+      </c>
+      <c r="E174" t="s">
+        <v>163</v>
+      </c>
+      <c r="F174">
+        <v>25</v>
+      </c>
+      <c r="G174" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>270</v>
+      </c>
+      <c r="B175" t="s">
+        <v>174</v>
+      </c>
+      <c r="C175" t="s">
+        <v>237</v>
+      </c>
+      <c r="D175" t="s">
+        <v>231</v>
+      </c>
+      <c r="E175" t="s">
+        <v>242</v>
+      </c>
+      <c r="F175">
+        <v>2</v>
+      </c>
+      <c r="G175" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>270</v>
+      </c>
+      <c r="B176" t="s">
+        <v>174</v>
+      </c>
+      <c r="C176" t="s">
+        <v>237</v>
+      </c>
+      <c r="D176" t="s">
+        <v>240</v>
+      </c>
+      <c r="E176" t="s">
+        <v>242</v>
+      </c>
+      <c r="F176">
+        <v>2</v>
+      </c>
+      <c r="G176" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>270</v>
+      </c>
+      <c r="B177" t="s">
+        <v>174</v>
+      </c>
+      <c r="C177" t="s">
+        <v>237</v>
+      </c>
+      <c r="D177" t="s">
+        <v>240</v>
+      </c>
+      <c r="E177" t="s">
+        <v>242</v>
+      </c>
+      <c r="F177">
+        <v>2</v>
+      </c>
+      <c r="G177" t="s">
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -2161,8 +5387,8 @@
   <dimension ref="A1:O222"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A177" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J218" sqref="J218"/>
+      <pane ySplit="1" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A223" sqref="A223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10807,7 +14033,7 @@
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="C41" sqref="C41"/>

</xml_diff>

<commit_message>
Updated figure 1 - stuck on how to assign random parameters to each country and species for figuire 2
</commit_message>
<xml_diff>
--- a/alternativefeeddata.xlsx
+++ b/alternativefeeddata.xlsx
@@ -1286,10 +1286,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H177"/>
+  <dimension ref="A1:K177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D172" sqref="D172"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1302,7 +1302,7 @@
     <col min="7" max="7" width="27.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>232</v>
       </c>
@@ -1325,7 +1325,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>236</v>
       </c>
@@ -1347,8 +1347,12 @@
       <c r="G2" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <f>AVERAGE(F2:F4)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>236</v>
       </c>
@@ -1371,7 +1375,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>236</v>
       </c>
@@ -1394,7 +1398,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>236</v>
       </c>
@@ -1417,7 +1421,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>236</v>
       </c>
@@ -1440,7 +1444,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>236</v>
       </c>
@@ -1463,7 +1467,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>246</v>
       </c>
@@ -1485,8 +1489,16 @@
       <c r="G8" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <f>AVERAGE(F8:F9)</f>
+        <v>2</v>
+      </c>
+      <c r="J8">
+        <f>AVERAGE(H8,H10,H12,H14,H23,H24)</f>
+        <v>5.916666666666667</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>246</v>
       </c>
@@ -1509,12 +1521,12 @@
         <v>245</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>251</v>
       </c>
       <c r="B10" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C10" t="s">
         <v>243</v>
@@ -1531,13 +1543,17 @@
       <c r="G10" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <f>AVERAGE(F10:F11)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>251</v>
       </c>
       <c r="B11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C11" t="s">
         <v>243</v>
@@ -1555,7 +1571,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>249</v>
       </c>
@@ -1577,8 +1593,12 @@
       <c r="G12" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <f>AVERAGE(F12:F13)</f>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>249</v>
       </c>
@@ -1601,7 +1621,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>250</v>
       </c>
@@ -1623,8 +1643,12 @@
       <c r="G14" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14">
+        <f>AVERAGE(F14:F15)</f>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>250</v>
       </c>
@@ -1647,7 +1671,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>150</v>
       </c>
@@ -1670,7 +1694,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>150</v>
       </c>
@@ -1693,7 +1717,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>253</v>
       </c>
@@ -1716,7 +1740,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>254</v>
       </c>
@@ -1739,7 +1763,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>254</v>
       </c>
@@ -1762,7 +1786,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>95</v>
       </c>
@@ -1785,7 +1809,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>95</v>
       </c>
@@ -1808,7 +1832,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>272</v>
       </c>
@@ -1830,8 +1854,11 @@
       <c r="G23" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>257</v>
       </c>
@@ -1853,8 +1880,12 @@
       <c r="G24" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24">
+        <f>AVERAGE(F24,F26)</f>
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>257</v>
       </c>
@@ -1876,8 +1907,12 @@
       <c r="G25" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25">
+        <f>AVERAGE(F25,F27)</f>
+        <v>2.4500000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>257</v>
       </c>
@@ -1900,7 +1935,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>257</v>
       </c>
@@ -1923,7 +1958,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>262</v>
       </c>
@@ -1946,7 +1981,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>262</v>
       </c>
@@ -1969,7 +2004,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>135</v>
       </c>
@@ -1991,8 +2026,12 @@
       <c r="G30" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30">
+        <f>AVERAGE(F30,F32)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>135</v>
       </c>
@@ -2015,7 +2054,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>135</v>
       </c>
@@ -2038,7 +2077,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>135</v>
       </c>
@@ -2061,7 +2100,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>275</v>
       </c>
@@ -2083,8 +2122,12 @@
       <c r="G34" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34">
+        <f>AVERAGE(F34,F36,F38,F40,F42,F44,F46,F48,F50,F52,F54,F56)</f>
+        <v>28.308333333333334</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>275</v>
       </c>
@@ -2107,7 +2150,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>275</v>
       </c>
@@ -2130,7 +2173,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>275</v>
       </c>
@@ -2153,7 +2196,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>275</v>
       </c>
@@ -2176,7 +2219,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>275</v>
       </c>
@@ -2199,7 +2242,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>275</v>
       </c>
@@ -2222,7 +2265,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>275</v>
       </c>
@@ -2244,8 +2287,12 @@
       <c r="G41" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J41">
+        <f>AVERAGE(H34,H58)</f>
+        <v>34.745075757575755</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>275</v>
       </c>
@@ -2268,7 +2315,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>275</v>
       </c>
@@ -2291,7 +2338,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>275</v>
       </c>
@@ -2314,7 +2361,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>275</v>
       </c>
@@ -2337,7 +2384,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>275</v>
       </c>
@@ -2360,7 +2407,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>275</v>
       </c>
@@ -2383,7 +2430,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>275</v>
       </c>
@@ -2406,7 +2453,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>275</v>
       </c>
@@ -2429,7 +2476,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>275</v>
       </c>
@@ -2452,7 +2499,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>275</v>
       </c>
@@ -2475,7 +2522,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>275</v>
       </c>
@@ -2498,7 +2545,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>275</v>
       </c>
@@ -2521,7 +2568,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>275</v>
       </c>
@@ -2544,7 +2591,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>275</v>
       </c>
@@ -2567,7 +2614,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>275</v>
       </c>
@@ -2590,7 +2637,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>275</v>
       </c>
@@ -2613,7 +2660,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>276</v>
       </c>
@@ -2635,8 +2682,12 @@
       <c r="G58" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H58">
+        <f>AVERAGE(F58:F68)</f>
+        <v>41.18181818181818</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>276</v>
       </c>
@@ -2659,7 +2710,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>276</v>
       </c>
@@ -2682,7 +2733,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>276</v>
       </c>
@@ -2705,7 +2756,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>276</v>
       </c>
@@ -2728,7 +2779,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>276</v>
       </c>
@@ -2751,7 +2802,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>276</v>
       </c>
@@ -2774,7 +2825,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>276</v>
       </c>
@@ -2797,7 +2848,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>276</v>
       </c>
@@ -2820,7 +2871,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>276</v>
       </c>
@@ -2843,7 +2894,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>276</v>
       </c>
@@ -2866,7 +2917,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>276</v>
       </c>
@@ -2889,7 +2940,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>278</v>
       </c>
@@ -2912,7 +2963,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>278</v>
       </c>
@@ -2934,8 +2985,12 @@
       <c r="G71" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H71">
+        <f>F71</f>
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>263</v>
       </c>
@@ -2958,7 +3013,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>264</v>
       </c>
@@ -2981,7 +3036,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>264</v>
       </c>
@@ -3004,7 +3059,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>264</v>
       </c>
@@ -3027,7 +3082,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>264</v>
       </c>
@@ -3050,7 +3105,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>265</v>
       </c>
@@ -3073,7 +3128,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>266</v>
       </c>
@@ -3096,7 +3151,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>266</v>
       </c>
@@ -3119,7 +3174,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>285</v>
       </c>
@@ -3141,8 +3196,12 @@
       <c r="G80" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H80">
+        <f>AVERAGE(F80:F84)</f>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>285</v>
       </c>
@@ -3165,7 +3224,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>285</v>
       </c>
@@ -3188,7 +3247,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>285</v>
       </c>
@@ -3211,7 +3270,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>285</v>
       </c>
@@ -3234,7 +3293,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>286</v>
       </c>
@@ -3256,8 +3315,12 @@
       <c r="G85" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H85">
+        <f>AVERAGE(F85:F89)</f>
+        <v>39.5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>286</v>
       </c>
@@ -3280,7 +3343,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>286</v>
       </c>
@@ -3303,7 +3366,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>286</v>
       </c>
@@ -3326,7 +3389,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>286</v>
       </c>
@@ -3348,8 +3411,12 @@
       <c r="G89" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J89">
+        <f>AVERAGE(H85,H95)</f>
+        <v>44.35</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>286</v>
       </c>
@@ -3371,8 +3438,12 @@
       <c r="G90" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H90">
+        <f>AVERAGE(F90:F94)</f>
+        <v>17.920000000000002</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>286</v>
       </c>
@@ -3395,7 +3466,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>286</v>
       </c>
@@ -3418,7 +3489,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>286</v>
       </c>
@@ -3441,7 +3512,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>286</v>
       </c>
@@ -3464,7 +3535,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>288</v>
       </c>
@@ -3486,8 +3557,12 @@
       <c r="G95" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H95">
+        <f>AVERAGE(F95:F99)</f>
+        <v>49.2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>288</v>
       </c>
@@ -3510,7 +3585,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>288</v>
       </c>
@@ -3533,7 +3608,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>288</v>
       </c>
@@ -3556,7 +3631,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>288</v>
       </c>
@@ -3579,7 +3654,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>288</v>
       </c>
@@ -3601,8 +3676,12 @@
       <c r="G100" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H100">
+        <f>AVERAGE(F100:F104)</f>
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>288</v>
       </c>
@@ -3625,7 +3704,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>288</v>
       </c>
@@ -3648,7 +3727,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>288</v>
       </c>
@@ -3671,7 +3750,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>288</v>
       </c>
@@ -3694,7 +3773,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>289</v>
       </c>
@@ -3717,7 +3796,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>289</v>
       </c>
@@ -3740,7 +3819,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>289</v>
       </c>
@@ -3763,7 +3842,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>289</v>
       </c>
@@ -3786,7 +3865,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>289</v>
       </c>
@@ -3809,7 +3888,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>289</v>
       </c>
@@ -3832,7 +3911,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>290</v>
       </c>
@@ -3855,7 +3934,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>290</v>
       </c>
@@ -3878,7 +3957,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>267</v>
       </c>
@@ -3901,7 +3980,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>267</v>
       </c>
@@ -3924,7 +4003,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>293</v>
       </c>
@@ -3947,7 +4026,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>293</v>
       </c>
@@ -3969,8 +4048,12 @@
       <c r="G116" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H116">
+        <f>AVERAGE(F115:F119)</f>
+        <v>50.8</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>293</v>
       </c>
@@ -3992,8 +4075,12 @@
       <c r="G117" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H117">
+        <f>AVERAGE(F120:F124)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>293</v>
       </c>
@@ -4016,7 +4103,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>293</v>
       </c>
@@ -4039,7 +4126,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>293</v>
       </c>
@@ -4062,7 +4149,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>293</v>
       </c>
@@ -4085,7 +4172,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>293</v>
       </c>
@@ -4108,7 +4195,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>293</v>
       </c>
@@ -4131,7 +4218,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>293</v>
       </c>
@@ -4154,7 +4241,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>294</v>
       </c>
@@ -4176,8 +4263,11 @@
       <c r="G125" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H125">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>294</v>
       </c>
@@ -4199,8 +4289,11 @@
       <c r="G126" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H126">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>295</v>
       </c>
@@ -4222,8 +4315,12 @@
       <c r="G127" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H127">
+        <f>AVERAGE(F127,F129)</f>
+        <v>59.7</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>295</v>
       </c>
@@ -4245,8 +4342,12 @@
       <c r="G128" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H128">
+        <f>AVERAGE(F128,F130)</f>
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>295</v>
       </c>
@@ -4268,8 +4369,12 @@
       <c r="G129" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K129">
+        <f>AVERAGE(H125,H127,H131,H136,H116)</f>
+        <v>50.061999999999998</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>295</v>
       </c>
@@ -4292,7 +4397,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>297</v>
       </c>
@@ -4314,8 +4419,12 @@
       <c r="G131" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H131">
+        <f>AVERAGE(F131,F133)</f>
+        <v>54.06</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>297</v>
       </c>
@@ -4337,8 +4446,12 @@
       <c r="G132" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H132">
+        <f>AVERAGE(F132,F134,F135)</f>
+        <v>11.026666666666666</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>297</v>
       </c>
@@ -4361,7 +4474,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>297</v>
       </c>
@@ -4384,7 +4497,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>297</v>
       </c>
@@ -4407,7 +4520,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>302</v>
       </c>
@@ -4429,8 +4542,12 @@
       <c r="G136" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H136">
+        <f>AVERAGE(F136:F137)</f>
+        <v>15.75</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>302</v>
       </c>
@@ -4453,7 +4570,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>304</v>
       </c>
@@ -4476,7 +4593,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>304</v>
       </c>
@@ -4499,7 +4616,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>306</v>
       </c>
@@ -4521,8 +4638,12 @@
       <c r="G140" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H140">
+        <f>AVERAGE(F140:F142)</f>
+        <v>23.833333333333332</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>306</v>
       </c>
@@ -4545,7 +4666,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>268</v>
       </c>
@@ -4562,13 +4683,13 @@
         <v>163</v>
       </c>
       <c r="F142">
-        <v>150</v>
+        <v>15</v>
       </c>
       <c r="G142" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>268</v>
       </c>
@@ -4591,7 +4712,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>308</v>
       </c>
@@ -4617,7 +4738,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>308</v>
       </c>
@@ -4639,8 +4760,12 @@
       <c r="G145" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H145">
+        <f>AVERAGE(F144:F146)</f>
+        <v>28.366666666666664</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>308</v>
       </c>
@@ -4662,8 +4787,12 @@
       <c r="G146" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H146">
+        <f>AVERAGE(F148)</f>
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>308</v>
       </c>
@@ -4685,8 +4814,12 @@
       <c r="G147" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H147">
+        <f>AVERAGE(F148)</f>
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>308</v>
       </c>
@@ -4709,7 +4842,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>310</v>
       </c>
@@ -4731,8 +4864,16 @@
       <c r="G149" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H149">
+        <f>AVERAGE(F149:F151)</f>
+        <v>17.866666666666664</v>
+      </c>
+      <c r="K149">
+        <f>AVERAGE(H145,H149,H152,H158,H172)</f>
+        <v>23.834285714285713</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>310</v>
       </c>
@@ -4755,7 +4896,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>310</v>
       </c>
@@ -4777,8 +4918,12 @@
       <c r="G151" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K151">
+        <f>AVERAGE(H155,H160,H175)</f>
+        <v>1.5374999999999999</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>192</v>
       </c>
@@ -4800,8 +4945,12 @@
       <c r="G152" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H152">
+        <f>AVERAGE(F152:F154)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>192</v>
       </c>
@@ -4824,7 +4973,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>192</v>
       </c>
@@ -4847,7 +4996,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>192</v>
       </c>
@@ -4869,8 +5018,11 @@
       <c r="G155" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>192</v>
       </c>
@@ -4893,7 +5045,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>192</v>
       </c>
@@ -4916,7 +5068,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>269</v>
       </c>
@@ -4938,8 +5090,12 @@
       <c r="G158" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H158">
+        <f>AVERAGE(F158:F159,F162:F166)</f>
+        <v>21.271428571428572</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>269</v>
       </c>
@@ -4962,7 +5118,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>269</v>
       </c>
@@ -4984,8 +5140,12 @@
       <c r="G160" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H160">
+        <f>AVERAGE(F160:F161,F167:F171,)</f>
+        <v>1.6125</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>269</v>
       </c>
@@ -5008,7 +5168,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>269</v>
       </c>
@@ -5031,7 +5191,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>269</v>
       </c>
@@ -5054,7 +5214,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>269</v>
       </c>
@@ -5077,7 +5237,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>269</v>
       </c>
@@ -5100,7 +5260,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>269</v>
       </c>
@@ -5123,7 +5283,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>269</v>
       </c>
@@ -5146,7 +5306,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>269</v>
       </c>
@@ -5169,7 +5329,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>269</v>
       </c>
@@ -5192,7 +5352,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>269</v>
       </c>
@@ -5215,7 +5375,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>269</v>
       </c>
@@ -5238,7 +5398,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>270</v>
       </c>
@@ -5260,8 +5420,12 @@
       <c r="G172" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H172">
+        <f>AVERAGE(F172:F174)</f>
+        <v>25.666666666666668</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>270</v>
       </c>
@@ -5284,7 +5448,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>270</v>
       </c>
@@ -5307,7 +5471,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>270</v>
       </c>
@@ -5329,8 +5493,11 @@
       <c r="G175" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H175">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>270</v>
       </c>

</xml_diff>